<commit_message>
date::dpy conforms with chrono move date enumes to xll_date.cpp
</commit_message>
<xml_diff>
--- a/bondxll/bondlib.xlsx
+++ b/bondxll/bondlib.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keith\source\repos\tmcrossx\bondlib\bondxll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74F409B-C767-4CF7-8A0F-3F0A93F1CDB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C8A31C-1C9C-4ECD-AC94-FBFF0D329747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{06412BBD-41CB-406E-9C18-9630F19E364B}"/>
   </bookViews>
@@ -135,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -144,12 +144,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -466,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92863B8-4C87-4474-B5B0-52EEB5BB3C33}">
-  <dimension ref="B2:H16"/>
+  <dimension ref="B2:Y17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -479,28 +478,21 @@
     <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="B2" s="4" t="s">
+    <row r="2" spans="2:25" ht="21" x14ac:dyDescent="0.35">
+      <c r="B2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B4" s="6" t="s">
+    <row r="4" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="B4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>45080</v>
       </c>
-      <c r="G4" s="5" cm="1">
-        <f t="array" ref="G4">_xll.TMX.DATE.ADD.YEARS(dated,1)</f>
-        <v>45445</v>
-      </c>
-      <c r="H4" cm="1">
-        <f t="array" ref="H4">_xll.TMX.DATE.DCF.YEARS(dated,G4)</f>
-        <v>0.99931553730321698</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="G4" s="4"/>
+    </row>
+    <row r="6" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -514,7 +506,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>1</v>
       </c>
@@ -522,19 +514,15 @@
         <v>0.05</v>
       </c>
       <c r="D7" s="2" cm="1">
-        <f t="array" ref="D7">_xll.\TMX.BOND.SIMPLE(maturity, coupon)</f>
-        <v>1930819800032</v>
-      </c>
-      <c r="E7" s="7" cm="1">
-        <f t="array" ref="E7">_xll.\TMX.BOND.INSTRUMENT(bond, dated)</f>
-        <v>-6.2774385622041925E+66</v>
-      </c>
-      <c r="F7" t="e" cm="1">
-        <f t="array" ref="F7">_xll.TMX.INSTRUMENT(E7)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+        <f t="array" ref="D7">_xll.\TMX.BOND.SIMPLE(B7, C7)</f>
+        <v>1973456868832</v>
+      </c>
+      <c r="E7" s="2" cm="1">
+        <f t="array" ref="E7">_xll.\TMX.BOND.INSTRUMENT(D7, dated)</f>
+        <v>1973458239920</v>
+      </c>
+    </row>
+    <row r="8" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>2</v>
       </c>
@@ -542,15 +530,15 @@
         <v>0.05</v>
       </c>
       <c r="D8" s="2" cm="1">
-        <f t="array" ref="D8">_xll.\TMX.BOND.SIMPLE(maturity, coupon)</f>
-        <v>1931115280208</v>
-      </c>
-      <c r="E8" s="7" cm="1">
-        <f t="array" ref="E8">_xll.\TMX.BOND.INSTRUMENT(bond)</f>
-        <v>-6.2774385622041925E+66</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+        <f t="array" ref="D8">_xll.\TMX.BOND.SIMPLE(B8, C8)</f>
+        <v>1973456868256</v>
+      </c>
+      <c r="E8" s="2" cm="1">
+        <f t="array" ref="E8">_xll.\TMX.BOND.INSTRUMENT(D8, dated)</f>
+        <v>1971666615376</v>
+      </c>
+    </row>
+    <row r="9" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>3</v>
       </c>
@@ -558,15 +546,15 @@
         <v>0.05</v>
       </c>
       <c r="D9" s="2" cm="1">
-        <f t="array" ref="D9">_xll.\TMX.BOND.SIMPLE(maturity, coupon)</f>
-        <v>1931115280976</v>
-      </c>
-      <c r="E9" s="7" cm="1">
-        <f t="array" ref="E9">_xll.\TMX.BOND.INSTRUMENT(bond)</f>
-        <v>-6.2774385622041925E+66</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+        <f t="array" ref="D9">_xll.\TMX.BOND.SIMPLE(B9, C9)</f>
+        <v>1973456870656</v>
+      </c>
+      <c r="E9" s="2" cm="1">
+        <f t="array" ref="E9">_xll.\TMX.BOND.INSTRUMENT(D9, dated)</f>
+        <v>1971666611056</v>
+      </c>
+    </row>
+    <row r="10" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>4</v>
       </c>
@@ -574,15 +562,15 @@
         <v>0.05</v>
       </c>
       <c r="D10" s="2" cm="1">
-        <f t="array" ref="D10">_xll.\TMX.BOND.SIMPLE(maturity, coupon)</f>
-        <v>1931115278480</v>
-      </c>
-      <c r="E10" s="7" cm="1">
-        <f t="array" ref="E10">_xll.\TMX.BOND.INSTRUMENT(bond)</f>
-        <v>-6.2774385622041925E+66</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+        <f t="array" ref="D10">_xll.\TMX.BOND.SIMPLE(B10, C10)</f>
+        <v>1973456870848</v>
+      </c>
+      <c r="E10" s="2" cm="1">
+        <f t="array" ref="E10">_xll.\TMX.BOND.INSTRUMENT(D10, dated)</f>
+        <v>1971666613072</v>
+      </c>
+    </row>
+    <row r="11" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>5</v>
       </c>
@@ -590,15 +578,15 @@
         <v>0.05</v>
       </c>
       <c r="D11" s="2" cm="1">
-        <f t="array" ref="D11">_xll.\TMX.BOND.SIMPLE(maturity, coupon)</f>
-        <v>1931115278096</v>
-      </c>
-      <c r="E11" s="7" cm="1">
-        <f t="array" ref="E11">_xll.\TMX.BOND.INSTRUMENT(bond)</f>
-        <v>-6.2774385622041925E+66</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
+        <f t="array" ref="D11">_xll.\TMX.BOND.SIMPLE(B11, C11)</f>
+        <v>1973456872000</v>
+      </c>
+      <c r="E11" s="2" cm="1">
+        <f t="array" ref="E11">_xll.\TMX.BOND.INSTRUMENT(D11, dated)</f>
+        <v>1971666616960</v>
+      </c>
+    </row>
+    <row r="12" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>6</v>
       </c>
@@ -606,15 +594,15 @@
         <v>0.05</v>
       </c>
       <c r="D12" s="2" cm="1">
-        <f t="array" ref="D12">_xll.\TMX.BOND.SIMPLE(maturity, coupon)</f>
-        <v>1931115277712</v>
-      </c>
-      <c r="E12" s="7" cm="1">
-        <f t="array" ref="E12">_xll.\TMX.BOND.INSTRUMENT(bond)</f>
-        <v>-6.2774385622041925E+66</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
+        <f t="array" ref="D12">_xll.\TMX.BOND.SIMPLE(B12, C12)</f>
+        <v>1973456868640</v>
+      </c>
+      <c r="E12" s="2" cm="1">
+        <f t="array" ref="E12">_xll.\TMX.BOND.INSTRUMENT(D12, dated)</f>
+        <v>1971666611920</v>
+      </c>
+    </row>
+    <row r="13" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>7</v>
       </c>
@@ -622,15 +610,15 @@
         <v>0.05</v>
       </c>
       <c r="D13" s="2" cm="1">
-        <f t="array" ref="D13">_xll.\TMX.BOND.SIMPLE(maturity, coupon)</f>
-        <v>1931115280016</v>
-      </c>
-      <c r="E13" s="7" cm="1">
-        <f t="array" ref="E13">_xll.\TMX.BOND.INSTRUMENT(bond)</f>
-        <v>-6.2774385622041925E+66</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
+        <f t="array" ref="D13">_xll.\TMX.BOND.SIMPLE(B13, C13)</f>
+        <v>1973456868928</v>
+      </c>
+      <c r="E13" s="2" cm="1">
+        <f t="array" ref="E13">_xll.\TMX.BOND.INSTRUMENT(D13, dated)</f>
+        <v>1971666614368</v>
+      </c>
+    </row>
+    <row r="14" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>8</v>
       </c>
@@ -638,15 +626,15 @@
         <v>0.05</v>
       </c>
       <c r="D14" s="2" cm="1">
-        <f t="array" ref="D14">_xll.\TMX.BOND.SIMPLE(maturity, coupon)</f>
-        <v>1931115277808</v>
-      </c>
-      <c r="E14" s="7" cm="1">
-        <f t="array" ref="E14">_xll.\TMX.BOND.INSTRUMENT(bond)</f>
-        <v>-6.2774385622041925E+66</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
+        <f t="array" ref="D14">_xll.\TMX.BOND.SIMPLE(B14, C14)</f>
+        <v>1973456871328</v>
+      </c>
+      <c r="E14" s="2" cm="1">
+        <f t="array" ref="E14">_xll.\TMX.BOND.INSTRUMENT(D14, dated)</f>
+        <v>1971666619408</v>
+      </c>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>9</v>
       </c>
@@ -654,15 +642,15 @@
         <v>0.05</v>
       </c>
       <c r="D15" s="2" cm="1">
-        <f t="array" ref="D15">_xll.\TMX.BOND.SIMPLE(maturity, coupon)</f>
-        <v>1931115281744</v>
-      </c>
-      <c r="E15" s="7" cm="1">
-        <f t="array" ref="E15">_xll.\TMX.BOND.INSTRUMENT(bond)</f>
-        <v>-6.2774385622041925E+66</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
+        <f t="array" ref="D15">_xll.\TMX.BOND.SIMPLE(B15, C15)</f>
+        <v>1973456874784</v>
+      </c>
+      <c r="E15" s="2" cm="1">
+        <f t="array" ref="E15">_xll.\TMX.BOND.INSTRUMENT(D15, dated)</f>
+        <v>1971666612928</v>
+      </c>
+    </row>
+    <row r="16" spans="2:25" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>10</v>
       </c>
@@ -670,12 +658,135 @@
         <v>0.05</v>
       </c>
       <c r="D16" s="2" cm="1">
-        <f t="array" ref="D16">_xll.\TMX.BOND.SIMPLE(maturity, coupon)</f>
-        <v>1931115278000</v>
-      </c>
-      <c r="E16" s="7" cm="1">
-        <f t="array" ref="E16">_xll.\TMX.BOND.INSTRUMENT(bond)</f>
-        <v>-6.2774385622041925E+66</v>
+        <f t="array" ref="D16">_xll.\TMX.BOND.SIMPLE(B16, C16)</f>
+        <v>1973456871904</v>
+      </c>
+      <c r="E16" s="2" cm="1">
+        <f t="array" ref="E16">_xll.\TMX.BOND.INSTRUMENT(D16, dated)</f>
+        <v>1971666610480</v>
+      </c>
+      <c r="F16" cm="1">
+        <f t="array" ref="F16:Y17">_xll.TMX.INSTRUMENT(E16)</f>
+        <v>0.49829907527190836</v>
+      </c>
+      <c r="G16">
+        <v>0.99659815054381673</v>
+      </c>
+      <c r="H16">
+        <v>1.4948972258157252</v>
+      </c>
+      <c r="I16">
+        <v>1.9931963010876335</v>
+      </c>
+      <c r="J16">
+        <v>2.4914953763595418</v>
+      </c>
+      <c r="K16">
+        <v>2.9897944516314503</v>
+      </c>
+      <c r="L16">
+        <v>3.4880935269033588</v>
+      </c>
+      <c r="M16">
+        <v>3.9863926021752669</v>
+      </c>
+      <c r="N16">
+        <v>4.4846916774471755</v>
+      </c>
+      <c r="O16">
+        <v>4.9829907527190835</v>
+      </c>
+      <c r="P16">
+        <v>5.4812898279909925</v>
+      </c>
+      <c r="Q16">
+        <v>5.9795889032629006</v>
+      </c>
+      <c r="R16">
+        <v>6.4778879785348087</v>
+      </c>
+      <c r="S16">
+        <v>6.9761870538067177</v>
+      </c>
+      <c r="T16">
+        <v>7.4744861290786258</v>
+      </c>
+      <c r="U16">
+        <v>7.9727852043505338</v>
+      </c>
+      <c r="V16">
+        <v>8.4710842796224419</v>
+      </c>
+      <c r="W16">
+        <v>8.9693833548943509</v>
+      </c>
+      <c r="X16">
+        <v>9.4676824301662599</v>
+      </c>
+      <c r="Y16">
+        <v>9.9659815054381671</v>
+      </c>
+    </row>
+    <row r="17" spans="6:25" x14ac:dyDescent="0.35">
+      <c r="F17">
+        <v>2.4861111111111112E-2</v>
+      </c>
+      <c r="G17">
+        <v>2.4861111111111112E-2</v>
+      </c>
+      <c r="H17">
+        <v>2.4861111111111112E-2</v>
+      </c>
+      <c r="I17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="J17">
+        <v>2.4861111111111112E-2</v>
+      </c>
+      <c r="K17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="L17">
+        <v>2.4861111111111112E-2</v>
+      </c>
+      <c r="M17">
+        <v>2.5138888888888891E-2</v>
+      </c>
+      <c r="N17">
+        <v>2.4722222222222225E-2</v>
+      </c>
+      <c r="O17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="P17">
+        <v>2.4722222222222225E-2</v>
+      </c>
+      <c r="Q17">
+        <v>2.5138888888888891E-2</v>
+      </c>
+      <c r="R17">
+        <v>2.4722222222222225E-2</v>
+      </c>
+      <c r="S17">
+        <v>2.5138888888888891E-2</v>
+      </c>
+      <c r="T17">
+        <v>2.4722222222222225E-2</v>
+      </c>
+      <c r="U17">
+        <v>2.5138888888888891E-2</v>
+      </c>
+      <c r="V17">
+        <v>2.4722222222222225E-2</v>
+      </c>
+      <c r="W17">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="X17">
+        <v>2.4722222222222225E-2</v>
+      </c>
+      <c r="Y17">
+        <v>2.5138888888888891E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ho-Lee pwflate::curve_base NVI class
</commit_message>
<xml_diff>
--- a/bondxll/bondlib.xlsx
+++ b/bondxll/bondlib.xlsx
@@ -8,44 +8,56 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keith\source\repos\tmcrossx\bondlib\bondxll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02EECB9-6A5C-4E6C-8850-81054CE66AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C952BEC-7358-4CA0-BF4E-E0C04C614EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{06412BBD-41CB-406E-9C18-9630F19E364B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{06412BBD-41CB-406E-9C18-9630F19E364B}"/>
   </bookViews>
   <sheets>
     <sheet name="Enum" sheetId="4" r:id="rId1"/>
-    <sheet name="Date" sheetId="2" r:id="rId2"/>
-    <sheet name="Curve" sheetId="3" r:id="rId3"/>
-    <sheet name="Bond" sheetId="5" r:id="rId4"/>
-    <sheet name="Bootstrap" sheetId="1" r:id="rId5"/>
+    <sheet name="Black" sheetId="6" r:id="rId2"/>
+    <sheet name="Date" sheetId="2" r:id="rId3"/>
+    <sheet name="Curve" sheetId="3" r:id="rId4"/>
+    <sheet name="Bond" sheetId="5" r:id="rId5"/>
+    <sheet name="Bootstrap" sheetId="1" r:id="rId6"/>
+    <sheet name="Ho-Lee" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="bond">Bootstrap!$E$7:$E$16</definedName>
     <definedName name="bond.simple">Bond!$C$6</definedName>
-    <definedName name="coupon" localSheetId="3">Bond!$C$3</definedName>
+    <definedName name="coupon" localSheetId="4">Bond!$C$3</definedName>
     <definedName name="coupon">Bootstrap!$C$7:$C$16</definedName>
-    <definedName name="curve" localSheetId="2">Curve!$I$2</definedName>
+    <definedName name="curve" localSheetId="3">Curve!$I$2</definedName>
     <definedName name="curve">Bootstrap!$G$6</definedName>
     <definedName name="curve_">Curve!$I$6</definedName>
     <definedName name="date">Date!$C$2</definedName>
-    <definedName name="dated" localSheetId="3">Bond!$C$7</definedName>
+    <definedName name="dated" localSheetId="4">Bond!$C$7</definedName>
     <definedName name="dated">Bootstrap!$C$4</definedName>
-    <definedName name="day_count" localSheetId="3">Bond!$C$5</definedName>
+    <definedName name="day_count" localSheetId="4">Bond!$C$5</definedName>
     <definedName name="days">Date!$C$10</definedName>
+    <definedName name="Dt">'Ho-Lee'!$C$6</definedName>
+    <definedName name="Du">'Ho-Lee'!$C$7</definedName>
     <definedName name="extrapolate">Curve!$C$6</definedName>
-    <definedName name="frequency" localSheetId="3">Bond!$C$4</definedName>
-    <definedName name="instrument" localSheetId="3">Bond!$C$8</definedName>
+    <definedName name="f">Black!$C$2</definedName>
+    <definedName name="frequency" localSheetId="4">Bond!$C$4</definedName>
+    <definedName name="instrument" localSheetId="4">Bond!$C$8</definedName>
     <definedName name="instrument">Bootstrap!$F$7:$F$16</definedName>
-    <definedName name="maturity" localSheetId="3">Bond!$C$2</definedName>
+    <definedName name="k">Black!$C$4</definedName>
+    <definedName name="logD">'Ho-Lee'!$C$9</definedName>
+    <definedName name="maturity" localSheetId="4">Bond!$C$2</definedName>
     <definedName name="maturity">Bootstrap!$B$7:$B$16</definedName>
     <definedName name="months">Date!$C$9</definedName>
     <definedName name="price">Bootstrap!$D$7:$D$16</definedName>
+    <definedName name="r_">'Ho-Lee'!$C$2</definedName>
     <definedName name="rate">Curve!$C$3:$C$5</definedName>
+    <definedName name="s">Black!$C$3</definedName>
     <definedName name="shift">Curve!$I$3</definedName>
+    <definedName name="t">'Ho-Lee'!$C$4</definedName>
     <definedName name="time">Curve!$B$3:$B$5</definedName>
     <definedName name="translate">Curve!$I$5</definedName>
+    <definedName name="u">'Ho-Lee'!$C$5</definedName>
     <definedName name="years">Date!$C$3</definedName>
     <definedName name="years_">Date!$C$8</definedName>
+    <definedName name="σ">'Ho-Lee'!$C$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -90,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
   <si>
     <t>maturity</t>
   </si>
@@ -225,6 +237,60 @@
   </si>
   <si>
     <t>convexity</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>moneyness</t>
+  </si>
+  <si>
+    <t>delta</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>vega</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>σ</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>D_t(u)</t>
+  </si>
+  <si>
+    <t>Dt</t>
+  </si>
+  <si>
+    <t>Du</t>
+  </si>
+  <si>
+    <t>ED</t>
+  </si>
+  <si>
+    <t>ELogD</t>
+  </si>
+  <si>
+    <t>VarLogD</t>
+  </si>
+  <si>
+    <t>logD</t>
   </si>
 </sst>
 </file>
@@ -596,37 +662,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.2</c:v>
@@ -893,127 +959,127 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1</c:v>
+                  <c:v>0.37731695875497728</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.10909090909090909</c:v>
+                  <c:v>0.36119723523179753</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.11666666666666668</c:v>
+                  <c:v>0.34776413229581438</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1230769230769231</c:v>
+                  <c:v>0.33639766058075177</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.12857142857142859</c:v>
+                  <c:v>0.32665497053926945</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.13333333333333336</c:v>
+                  <c:v>0.31821130583665147</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.13750000000000004</c:v>
+                  <c:v>0.3108230992218608</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.14117647058823532</c:v>
+                  <c:v>0.30430409338528075</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.14444444444444446</c:v>
+                  <c:v>0.29850942153054294</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.14736842105263159</c:v>
+                  <c:v>0.29332471513419855</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.15000000000000005</c:v>
+                  <c:v>0.28865847937748867</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.1571428571428572</c:v>
+                  <c:v>0.28919855178808446</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.16363636363636369</c:v>
+                  <c:v>0.28968952670680786</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.1695652173913044</c:v>
+                  <c:v>0.29013780815433798</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.17500000000000004</c:v>
+                  <c:v>0.29054873281457388</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.18000000000000005</c:v>
+                  <c:v>0.29092678350199092</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.18461538461538468</c:v>
+                  <c:v>0.291275753367299</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.18888888888888894</c:v>
+                  <c:v>0.29159887361295456</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.19285714285714292</c:v>
+                  <c:v>0.29189891384106331</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.19655172413793109</c:v>
+                  <c:v>0.29217826163964739</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.20000000000000012</c:v>
+                  <c:v>0.29243898625165921</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.20645161290322592</c:v>
+                  <c:v>0.29590869637257339</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.21250000000000013</c:v>
+                  <c:v>0.2991615496109305</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.21818181818181831</c:v>
+                  <c:v>0.30221726022878109</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.223529411764706</c:v>
+                  <c:v>0.30509322316322873</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.2285714285714287</c:v>
+                  <c:v>0.30780484535856506</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.23333333333333345</c:v>
+                  <c:v>0.31036582187638267</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.23783783783783796</c:v>
+                  <c:v>0.31278836723107506</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.24210526315789485</c:v>
+                  <c:v>0.31508341019867836</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.24615384615384628</c:v>
+                  <c:v>0.31726075865512249</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.25000000000000011</c:v>
+                  <c:v>0.31932923968874438</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1193,124 +1259,124 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99004983374916811</c:v>
+                  <c:v>0.96297127539850957</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.98019867330675525</c:v>
+                  <c:v>0.92731367724263203</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.97044553354850815</c:v>
+                  <c:v>0.89297643446881925</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.96078943915232318</c:v>
+                  <c:v>0.85991065600125238</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.95122942450071402</c:v>
+                  <c:v>0.82806926113829504</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.94176453358424872</c:v>
+                  <c:v>0.79740691251664542</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.93239381990594827</c:v>
+                  <c:v>0.7678799515577418</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.92311634638663576</c:v>
+                  <c:v>0.73944633630450429</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.91393118527122819</c:v>
+                  <c:v>0.71206558155990374</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.90483741803595963</c:v>
+                  <c:v>0.68569870124212184</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.88692043671715748</c:v>
+                  <c:v>0.67212095724569298</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.86935823539880586</c:v>
+                  <c:v>0.65881207059389468</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.85214378896621135</c:v>
+                  <c:v>0.64576671755461201</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.835270211411272</c:v>
+                  <c:v>0.63297967981268888</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.81873075307798182</c:v>
+                  <c:v>0.62044584238253231</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.80251879796247838</c:v>
+                  <c:v>0.60816019156205037</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.78662786106655336</c:v>
+                  <c:v>0.59611781292710386</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.77105158580356614</c:v>
+                  <c:v>0.58431388936567175</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.75578374145572536</c:v>
+                  <c:v>0.5727436991509417</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.74081822068171777</c:v>
+                  <c:v>0.56140261405255643</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.71892373343192606</c:v>
+                  <c:v>0.54481065932976036</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.69767632607103092</c:v>
+                  <c:v>0.5287090709761838</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.67705687449816454</c:v>
+                  <c:v>0.51308335647541869</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.65704681981505664</c:v>
+                  <c:v>0.49791945162964713</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.63762815162177311</c:v>
+                  <c:v>0.48320370790091349</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.61878339180614061</c:v>
+                  <c:v>0.4689228801265195</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.60049557881226578</c:v>
+                  <c:v>0.4550641145974833</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.58274825237398942</c:v>
+                  <c:v>0.44161493748933417</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.56552543869953686</c:v>
+                  <c:v>0.42856324363482795</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.54881163609402606</c:v>
+                  <c:v>0.41589728562847983</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.52729242404304821</c:v>
+                  <c:v>0.39958971980396069</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.50661699236558921</c:v>
+                  <c:v>0.38392158278148136</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.48675225595997129</c:v>
+                  <c:v>0.36886780219909165</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.46766642700990885</c:v>
+                  <c:v>0.35440428879621533</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.44932896411722123</c:v>
+                  <c:v>0.34050789786569369</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.43171052342907934</c:v>
+                  <c:v>0.32715639221731641</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.41478291168158099</c:v>
+                  <c:v>0.31432840659357286</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.3985190410845138</c:v>
+                  <c:v>0.30200341348068227</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.38289288597511167</c:v>
+                  <c:v>0.2901616902601919</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.367879441171442</c:v>
+                  <c:v>0.27878428764857993</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1935,307 +2001,307 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>4.9688644922257018E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9688644922257018E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9688644922257018E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9688644922257018E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9688644922257018E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9688644922257018E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9688644922257018E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9688644922257018E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.9688644922257018E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.9688644922257018E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.9688644922257018E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.1859212468108845E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.1859212468108845E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.1859212468108845E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.1859212468108845E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.1859212468108845E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.1859212468108845E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.1859212468108845E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.1859212468108845E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.1859212468108845E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.1859212468108845E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.7683063278025691E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.7683063278025691E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.7683063278025691E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.7683063278025691E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.7683063278025691E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.7683063278025691E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.7683063278025691E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.7683063278025691E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.7683063278025691E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.7683063278025691E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.9823073127630173E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.9823073127630173E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.9823073127630173E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.9823073127630173E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.9823073127630173E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.9823073127630173E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.9823073127630173E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.9823073127630173E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.9823073127630173E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.9823073127630173E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.9688644922258357E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.9688644922258357E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.9688644922258357E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4.9688644922258357E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.9688644922258357E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.9688644922258357E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.9688644922258357E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4.9688644922258357E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.9688644922258357E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4.9688644922258357E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>4.9823073127630096E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>4.9688644922257615E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>4.9688644922257615E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>4.9688644922257615E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>4.9688644922257615E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>4.9688644922257615E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>4.9688644922257615E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>4.9688644922257615E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>4.9688644922257615E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>4.9688644922257615E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>4.9688644922257615E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>4.9823073127629867E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>4.9823073127629867E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>4.9823073127629867E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>4.9823073127629867E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>4.9823073127629867E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>4.9823073127629867E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>4.9823073127629867E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>4.9823073127629867E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>4.9823073127629867E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>4.9823073127629867E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2243,7 +2309,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-1EE4-4982-B496-53DEE2E034B9}"/>
+              <c16:uniqueId val="{00000000-B005-4570-9F3F-EEFA829C54BE}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2255,11 +2321,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="385689792"/>
-        <c:axId val="385679232"/>
+        <c:axId val="289138832"/>
+        <c:axId val="289154672"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="385689792"/>
+        <c:axId val="289138832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2316,16 +2382,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385679232"/>
+        <c:crossAx val="289154672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="385679232"/>
+        <c:axId val="289154672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="0.1"/>
-          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2380,7 +2444,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="385689792"/>
+        <c:crossAx val="289138832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3594,22 +3658,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>397192</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>82867</xdr:rowOff>
+      <xdr:colOff>225136</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>230333</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>159067</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>82867</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>554182</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>64078</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3E9958D-3DD3-E102-F25C-5D5F958EFF69}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9CF8C2A-8671-2722-4FB4-852E4DB6992D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3964,7 +4028,7 @@
       </c>
       <c r="E3" s="5" cm="1">
         <f t="array" ref="E3">_xll.TMX_DAY_COUNT_30_360()</f>
-        <v>140716345864955</v>
+        <v>140716431061820</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
@@ -3980,7 +4044,7 @@
       </c>
       <c r="E4" s="5" cm="1">
         <f t="array" ref="E4">_xll.TMX_DAY_COUNT_ACTUAL_360()</f>
-        <v>140716345857945</v>
+        <v>140716431054760</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
@@ -3996,7 +4060,7 @@
       </c>
       <c r="E5" s="5" cm="1">
         <f t="array" ref="E5">_xll.TMX_DAY_COUNT_ACTUAL_365()</f>
-        <v>140716345863355</v>
+        <v>140716431060195</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -4012,7 +4076,7 @@
       </c>
       <c r="E6" s="5" cm="1">
         <f t="array" ref="E6">_xll.TMX_DAY_COUNT_ACTUAL_ACTUAL()</f>
-        <v>140716345868405</v>
+        <v>140716431065320</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
@@ -4021,7 +4085,7 @@
       </c>
       <c r="E7" s="5" cm="1">
         <f t="array" ref="E7">_xll.TMX_DAY_COUNT_YEARS()</f>
-        <v>140716345898895</v>
+        <v>140716431096015</v>
       </c>
     </row>
   </sheetData>
@@ -4030,6 +4094,121 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D05E6F0E-62B3-47B5-8C49-DACF71BB425D}">
+  <dimension ref="B2:E9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" cm="1">
+        <f t="array" ref="C5">_xll.TMX.BLACK.MONEYNESS(f, s, k)</f>
+        <v>0.05</v>
+      </c>
+      <c r="D5">
+        <v>1E-3</v>
+      </c>
+      <c r="E5">
+        <f>-D5</f>
+        <v>-1E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" cm="1">
+        <f t="array" ref="C6">_xll.TMX.BLACK.PUT.VALUE(f, s, k)</f>
+        <v>3.987761167674492</v>
+      </c>
+      <c r="D6" cm="1">
+        <f t="array" ref="D6">_xll.TMX.BLACK.PUT.VALUE(f + D5, s, k)</f>
+        <v>3.9872811264024222</v>
+      </c>
+      <c r="E6" cm="1">
+        <f t="array" ref="E6">_xll.TMX.BLACK.PUT.VALUE(f + E5, s, k)</f>
+        <v>3.9882412487909491</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" cm="1">
+        <f t="array" ref="C7">_xll.TMX.BLACK.PUT.DELTA(f, s, k)</f>
+        <v>-0.48006119416162751</v>
+      </c>
+      <c r="D7">
+        <f>(D6-E6)/(D5-E5)</f>
+        <v>-0.48006119426347027</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" cm="1">
+        <f t="array" ref="C8">_xll.TMX.BLACK.PUT.GAMMA(f, s, k)</f>
+        <v>3.9844391409476404E-2</v>
+      </c>
+      <c r="D8">
+        <f>(D6-2*C6+E6)/(D5^2)</f>
+        <v>3.984438734505602E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" cm="1">
+        <f t="array" ref="C9">_xll.TMX.BLACK.PUT.VEGA(f, s, k)</f>
+        <v>39.844391409476401</v>
+      </c>
+      <c r="D9" cm="1">
+        <f t="array" ref="D9">(_xll.TMX.BLACK.PUT.VALUE(f, s + D5, k) - _xll.TMX.BLACK.PUT.VALUE(f, s + E5, k))/(D5 - E5)</f>
+        <v>39.844389753440623</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6DAD46C-D019-4BB0-8142-A427C42D3B36}">
   <dimension ref="B2:D11"/>
   <sheetViews>
@@ -4050,7 +4229,7 @@
       </c>
       <c r="C2" s="8">
         <f ca="1">TODAY()</f>
-        <v>45091</v>
+        <v>45093</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
@@ -4059,7 +4238,7 @@
       </c>
       <c r="C3" s="9">
         <f ca="1">10*RAND()</f>
-        <v>6.0795388229777094</v>
+        <v>3.9318059039872058</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4068,18 +4247,18 @@
       </c>
       <c r="C4" s="2" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">_xll.TMX.DATE.ADD_YEARS(date,years)</f>
-        <v>47311.505949074075</v>
+        <v>46529.062615740739</v>
       </c>
       <c r="D4">
         <f ca="1">C4</f>
-        <v>47311.505949074075</v>
+        <v>46529.062615740739</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="2" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">_xll.TMX.DATE.ADD_YEARS(C4,-years)</f>
-        <v>45091</v>
+        <v>45093</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">C5-date</f>
@@ -4092,18 +4271,18 @@
       </c>
       <c r="C6" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">_xll.TMX.DATE.SUB_YEARS(C4,date)</f>
-        <v>6.0781535555144872</v>
+        <v>3.9316344620354968</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="2" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">_xll.TMX.DATE.ADD_YEARS(date,C6)</f>
-        <v>47311</v>
+        <v>46529</v>
       </c>
       <c r="D7">
         <f ca="1">C7</f>
-        <v>47311</v>
+        <v>46529</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4148,7 +4327,7 @@
       </c>
       <c r="C11" s="2" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">_xll.TMX.DATE.ADD_YMD(date, years_,months, days)</f>
-        <v>45521</v>
+        <v>45523</v>
       </c>
     </row>
   </sheetData>
@@ -4160,7 +4339,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B429FC-4136-41AD-B308-B590D229D902}">
   <dimension ref="B2:N43"/>
   <sheetViews>
@@ -4189,8 +4368,8 @@
         <v>7</v>
       </c>
       <c r="I2" s="5" cm="1">
-        <f t="array" ref="I2">_xll.\TMX.PWFLAT.CURVE(time, rate, extrapolate)</f>
-        <v>2392573155104</v>
+        <f t="array" aca="1" ref="I2" ca="1">_xll.\TMX.PWFLAT.CURVE(time, rate, extrapolate)</f>
+        <v>2534312649600</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>16</v>
@@ -4210,14 +4389,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="15">
-        <v>0.1</v>
+        <f ca="1">RAND()</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="E3" cm="1">
-        <f t="array" ref="E3:F6">TRANSPOSE(_xll.TMX.PWFLAT.CURVE(curve_))</f>
+        <f t="array" aca="1" ref="E3:F6" ca="1">TRANSPOSE(_xll.TMX.PWFLAT.CURVE(curve_))</f>
         <v>1</v>
       </c>
       <c r="F3" s="16">
-        <v>0.1</v>
+        <f ca="1"/>
+        <v>0.37731695875497728</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="3" t="s">
@@ -4231,15 +4412,15 @@
         <v>0</v>
       </c>
       <c r="L3" cm="1">
-        <f t="array" ref="L3">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K3)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="L3" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K3)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="M3" cm="1">
-        <f t="array" ref="M3">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K3)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="M3" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K3)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="N3" cm="1">
-        <f t="array" ref="N3">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K3)</f>
+        <f t="array" aca="1" ref="N3" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K3)</f>
         <v>1</v>
       </c>
     </row>
@@ -4251,29 +4432,31 @@
         <v>0.2</v>
       </c>
       <c r="E4">
+        <f ca="1"/>
         <v>2</v>
       </c>
       <c r="F4">
+        <f ca="1"/>
         <v>0.2</v>
       </c>
       <c r="I4" s="5" cm="1">
-        <f t="array" ref="I4">_xll.\TMX.PWFLAT.CURVE.SHIFT(curve, shift)</f>
-        <v>2392573154576</v>
+        <f t="array" aca="1" ref="I4" ca="1">_xll.\TMX.PWFLAT.CURVE.SHIFT(curve, shift)</f>
+        <v>2534312650128</v>
       </c>
       <c r="K4">
         <v>0.1</v>
       </c>
       <c r="L4" cm="1">
-        <f t="array" ref="L4">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K4)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="L4" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K4)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="M4" cm="1">
-        <f t="array" ref="M4">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K4)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="M4" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K4)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="N4" cm="1">
-        <f t="array" ref="N4">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K4)</f>
-        <v>0.99004983374916811</v>
+        <f t="array" aca="1" ref="N4" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K4)</f>
+        <v>0.96297127539850957</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
@@ -4284,9 +4467,11 @@
         <v>0.3</v>
       </c>
       <c r="E5">
+        <f ca="1"/>
         <v>3</v>
       </c>
       <c r="F5">
+        <f ca="1"/>
         <v>0.3</v>
       </c>
       <c r="H5" s="3" t="s">
@@ -4299,16 +4484,16 @@
         <v>0.2</v>
       </c>
       <c r="L5" cm="1">
-        <f t="array" ref="L5">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K5)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="L5" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K5)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="M5" cm="1">
-        <f t="array" ref="M5">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K5)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="M5" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K5)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="N5" cm="1">
-        <f t="array" ref="N5">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K5)</f>
-        <v>0.98019867330675525</v>
+        <f t="array" aca="1" ref="N5" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K5)</f>
+        <v>0.92731367724263203</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
@@ -4319,32 +4504,34 @@
         <v>0.4</v>
       </c>
       <c r="E6">
+        <f ca="1"/>
         <v>3</v>
       </c>
       <c r="F6">
+        <f ca="1"/>
         <v>0.4</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>24</v>
       </c>
       <c r="I6" s="5" cm="1">
-        <f t="array" ref="I6">_xll.\TMX.PWFLAT.CURVE.TRANSLATE(I4, translate)</f>
-        <v>2392573153168</v>
+        <f t="array" aca="1" ref="I6" ca="1">_xll.\TMX.PWFLAT.CURVE.TRANSLATE(I4, translate)</f>
+        <v>2534312638336</v>
       </c>
       <c r="K6">
         <v>0.30000000000000004</v>
       </c>
       <c r="L6" cm="1">
-        <f t="array" ref="L6">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K6)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="L6" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K6)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="M6" cm="1">
-        <f t="array" ref="M6">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K6)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="M6" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K6)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="N6" cm="1">
-        <f t="array" ref="N6">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K6)</f>
-        <v>0.97044553354850815</v>
+        <f t="array" aca="1" ref="N6" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K6)</f>
+        <v>0.89297643446881925</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -4352,16 +4539,16 @@
         <v>0.4</v>
       </c>
       <c r="L7" cm="1">
-        <f t="array" ref="L7">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K7)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="L7" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K7)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="M7" cm="1">
-        <f t="array" ref="M7">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K7)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="M7" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K7)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="N7" cm="1">
-        <f t="array" ref="N7">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K7)</f>
-        <v>0.96078943915232318</v>
+        <f t="array" aca="1" ref="N7" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K7)</f>
+        <v>0.85991065600125238</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
@@ -4369,16 +4556,16 @@
         <v>0.5</v>
       </c>
       <c r="L8" cm="1">
-        <f t="array" ref="L8">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K8)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="L8" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K8)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="M8" cm="1">
-        <f t="array" ref="M8">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K8)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="M8" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K8)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="N8" cm="1">
-        <f t="array" ref="N8">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K8)</f>
-        <v>0.95122942450071402</v>
+        <f t="array" aca="1" ref="N8" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K8)</f>
+        <v>0.82806926113829504</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
@@ -4386,16 +4573,16 @@
         <v>0.6</v>
       </c>
       <c r="L9" cm="1">
-        <f t="array" ref="L9">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K9)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="L9" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K9)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="M9" cm="1">
-        <f t="array" ref="M9">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K9)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="M9" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K9)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="N9" cm="1">
-        <f t="array" ref="N9">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K9)</f>
-        <v>0.94176453358424872</v>
+        <f t="array" aca="1" ref="N9" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K9)</f>
+        <v>0.79740691251664542</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
@@ -4403,16 +4590,16 @@
         <v>0.7</v>
       </c>
       <c r="L10" cm="1">
-        <f t="array" ref="L10">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K10)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="L10" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K10)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="M10" cm="1">
-        <f t="array" ref="M10">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K10)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="M10" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K10)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="N10" cm="1">
-        <f t="array" ref="N10">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K10)</f>
-        <v>0.93239381990594827</v>
+        <f t="array" aca="1" ref="N10" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K10)</f>
+        <v>0.7678799515577418</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -4420,16 +4607,16 @@
         <v>0.79999999999999993</v>
       </c>
       <c r="L11" cm="1">
-        <f t="array" ref="L11">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K11)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="L11" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K11)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="M11" cm="1">
-        <f t="array" ref="M11">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K11)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="M11" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K11)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="N11" cm="1">
-        <f t="array" ref="N11">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K11)</f>
-        <v>0.92311634638663576</v>
+        <f t="array" aca="1" ref="N11" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K11)</f>
+        <v>0.73944633630450429</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -4437,16 +4624,16 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="L12" cm="1">
-        <f t="array" ref="L12">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K12)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="L12" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K12)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="M12" cm="1">
-        <f t="array" ref="M12">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K12)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="M12" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K12)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="N12" cm="1">
-        <f t="array" ref="N12">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K12)</f>
-        <v>0.91393118527122819</v>
+        <f t="array" aca="1" ref="N12" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K12)</f>
+        <v>0.71206558155990374</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -4454,16 +4641,16 @@
         <v>0.99999999999999989</v>
       </c>
       <c r="L13" cm="1">
-        <f t="array" ref="L13">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K13)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="L13" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K13)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="M13" cm="1">
-        <f t="array" ref="M13">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K13)</f>
-        <v>0.1</v>
+        <f t="array" aca="1" ref="M13" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K13)</f>
+        <v>0.37731695875497728</v>
       </c>
       <c r="N13" cm="1">
-        <f t="array" ref="N13">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K13)</f>
-        <v>0.90483741803595963</v>
+        <f t="array" aca="1" ref="N13" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K13)</f>
+        <v>0.68569870124212184</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
@@ -4471,16 +4658,16 @@
         <v>1.0999999999999999</v>
       </c>
       <c r="L14" cm="1">
-        <f t="array" ref="L14">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K14)</f>
+        <f t="array" aca="1" ref="L14" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K14)</f>
         <v>0.2</v>
       </c>
       <c r="M14" cm="1">
-        <f t="array" ref="M14">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K14)</f>
-        <v>0.10909090909090909</v>
+        <f t="array" aca="1" ref="M14" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K14)</f>
+        <v>0.36119723523179753</v>
       </c>
       <c r="N14" cm="1">
-        <f t="array" ref="N14">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K14)</f>
-        <v>0.88692043671715748</v>
+        <f t="array" aca="1" ref="N14" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K14)</f>
+        <v>0.67212095724569298</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -4488,16 +4675,16 @@
         <v>1.2</v>
       </c>
       <c r="L15" cm="1">
-        <f t="array" ref="L15">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K15)</f>
+        <f t="array" aca="1" ref="L15" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K15)</f>
         <v>0.2</v>
       </c>
       <c r="M15" cm="1">
-        <f t="array" ref="M15">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K15)</f>
-        <v>0.11666666666666668</v>
+        <f t="array" aca="1" ref="M15" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K15)</f>
+        <v>0.34776413229581438</v>
       </c>
       <c r="N15" cm="1">
-        <f t="array" ref="N15">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K15)</f>
-        <v>0.86935823539880586</v>
+        <f t="array" aca="1" ref="N15" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K15)</f>
+        <v>0.65881207059389468</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
@@ -4505,16 +4692,16 @@
         <v>1.3</v>
       </c>
       <c r="L16" cm="1">
-        <f t="array" ref="L16">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K16)</f>
+        <f t="array" aca="1" ref="L16" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K16)</f>
         <v>0.2</v>
       </c>
       <c r="M16" cm="1">
-        <f t="array" ref="M16">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K16)</f>
-        <v>0.1230769230769231</v>
+        <f t="array" aca="1" ref="M16" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K16)</f>
+        <v>0.33639766058075177</v>
       </c>
       <c r="N16" cm="1">
-        <f t="array" ref="N16">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K16)</f>
-        <v>0.85214378896621135</v>
+        <f t="array" aca="1" ref="N16" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K16)</f>
+        <v>0.64576671755461201</v>
       </c>
     </row>
     <row r="17" spans="11:14" x14ac:dyDescent="0.3">
@@ -4522,16 +4709,16 @@
         <v>1.4000000000000001</v>
       </c>
       <c r="L17" cm="1">
-        <f t="array" ref="L17">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K17)</f>
+        <f t="array" aca="1" ref="L17" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K17)</f>
         <v>0.2</v>
       </c>
       <c r="M17" cm="1">
-        <f t="array" ref="M17">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K17)</f>
-        <v>0.12857142857142859</v>
+        <f t="array" aca="1" ref="M17" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K17)</f>
+        <v>0.32665497053926945</v>
       </c>
       <c r="N17" cm="1">
-        <f t="array" ref="N17">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K17)</f>
-        <v>0.835270211411272</v>
+        <f t="array" aca="1" ref="N17" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K17)</f>
+        <v>0.63297967981268888</v>
       </c>
     </row>
     <row r="18" spans="11:14" x14ac:dyDescent="0.3">
@@ -4539,16 +4726,16 @@
         <v>1.5000000000000002</v>
       </c>
       <c r="L18" cm="1">
-        <f t="array" ref="L18">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K18)</f>
+        <f t="array" aca="1" ref="L18" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K18)</f>
         <v>0.2</v>
       </c>
       <c r="M18" cm="1">
-        <f t="array" ref="M18">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K18)</f>
-        <v>0.13333333333333336</v>
+        <f t="array" aca="1" ref="M18" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K18)</f>
+        <v>0.31821130583665147</v>
       </c>
       <c r="N18" cm="1">
-        <f t="array" ref="N18">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K18)</f>
-        <v>0.81873075307798182</v>
+        <f t="array" aca="1" ref="N18" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K18)</f>
+        <v>0.62044584238253231</v>
       </c>
     </row>
     <row r="19" spans="11:14" x14ac:dyDescent="0.3">
@@ -4556,16 +4743,16 @@
         <v>1.6000000000000003</v>
       </c>
       <c r="L19" cm="1">
-        <f t="array" ref="L19">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K19)</f>
+        <f t="array" aca="1" ref="L19" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K19)</f>
         <v>0.2</v>
       </c>
       <c r="M19" cm="1">
-        <f t="array" ref="M19">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K19)</f>
-        <v>0.13750000000000004</v>
+        <f t="array" aca="1" ref="M19" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K19)</f>
+        <v>0.3108230992218608</v>
       </c>
       <c r="N19" cm="1">
-        <f t="array" ref="N19">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K19)</f>
-        <v>0.80251879796247838</v>
+        <f t="array" aca="1" ref="N19" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K19)</f>
+        <v>0.60816019156205037</v>
       </c>
     </row>
     <row r="20" spans="11:14" x14ac:dyDescent="0.3">
@@ -4573,16 +4760,16 @@
         <v>1.7000000000000004</v>
       </c>
       <c r="L20" cm="1">
-        <f t="array" ref="L20">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K20)</f>
+        <f t="array" aca="1" ref="L20" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K20)</f>
         <v>0.2</v>
       </c>
       <c r="M20" cm="1">
-        <f t="array" ref="M20">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K20)</f>
-        <v>0.14117647058823532</v>
+        <f t="array" aca="1" ref="M20" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K20)</f>
+        <v>0.30430409338528075</v>
       </c>
       <c r="N20" cm="1">
-        <f t="array" ref="N20">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K20)</f>
-        <v>0.78662786106655336</v>
+        <f t="array" aca="1" ref="N20" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K20)</f>
+        <v>0.59611781292710386</v>
       </c>
     </row>
     <row r="21" spans="11:14" x14ac:dyDescent="0.3">
@@ -4590,16 +4777,16 @@
         <v>1.8000000000000005</v>
       </c>
       <c r="L21" cm="1">
-        <f t="array" ref="L21">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K21)</f>
+        <f t="array" aca="1" ref="L21" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K21)</f>
         <v>0.2</v>
       </c>
       <c r="M21" cm="1">
-        <f t="array" ref="M21">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K21)</f>
-        <v>0.14444444444444446</v>
+        <f t="array" aca="1" ref="M21" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K21)</f>
+        <v>0.29850942153054294</v>
       </c>
       <c r="N21" cm="1">
-        <f t="array" ref="N21">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K21)</f>
-        <v>0.77105158580356614</v>
+        <f t="array" aca="1" ref="N21" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K21)</f>
+        <v>0.58431388936567175</v>
       </c>
     </row>
     <row r="22" spans="11:14" x14ac:dyDescent="0.3">
@@ -4607,16 +4794,16 @@
         <v>1.9000000000000006</v>
       </c>
       <c r="L22" cm="1">
-        <f t="array" ref="L22">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K22)</f>
+        <f t="array" aca="1" ref="L22" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K22)</f>
         <v>0.2</v>
       </c>
       <c r="M22" cm="1">
-        <f t="array" ref="M22">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K22)</f>
-        <v>0.14736842105263159</v>
+        <f t="array" aca="1" ref="M22" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K22)</f>
+        <v>0.29332471513419855</v>
       </c>
       <c r="N22" cm="1">
-        <f t="array" ref="N22">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K22)</f>
-        <v>0.75578374145572536</v>
+        <f t="array" aca="1" ref="N22" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K22)</f>
+        <v>0.5727436991509417</v>
       </c>
     </row>
     <row r="23" spans="11:14" x14ac:dyDescent="0.3">
@@ -4624,16 +4811,16 @@
         <v>2.0000000000000004</v>
       </c>
       <c r="L23" cm="1">
-        <f t="array" ref="L23">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K23)</f>
+        <f t="array" aca="1" ref="L23" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K23)</f>
         <v>0.3</v>
       </c>
       <c r="M23" cm="1">
-        <f t="array" ref="M23">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K23)</f>
-        <v>0.15000000000000005</v>
+        <f t="array" aca="1" ref="M23" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K23)</f>
+        <v>0.28865847937748867</v>
       </c>
       <c r="N23" cm="1">
-        <f t="array" ref="N23">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K23)</f>
-        <v>0.74081822068171777</v>
+        <f t="array" aca="1" ref="N23" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K23)</f>
+        <v>0.56140261405255643</v>
       </c>
     </row>
     <row r="24" spans="11:14" x14ac:dyDescent="0.3">
@@ -4641,16 +4828,16 @@
         <v>2.1000000000000005</v>
       </c>
       <c r="L24" cm="1">
-        <f t="array" ref="L24">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K24)</f>
+        <f t="array" aca="1" ref="L24" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K24)</f>
         <v>0.3</v>
       </c>
       <c r="M24" cm="1">
-        <f t="array" ref="M24">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K24)</f>
-        <v>0.1571428571428572</v>
+        <f t="array" aca="1" ref="M24" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K24)</f>
+        <v>0.28919855178808446</v>
       </c>
       <c r="N24" cm="1">
-        <f t="array" ref="N24">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K24)</f>
-        <v>0.71892373343192606</v>
+        <f t="array" aca="1" ref="N24" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K24)</f>
+        <v>0.54481065932976036</v>
       </c>
     </row>
     <row r="25" spans="11:14" x14ac:dyDescent="0.3">
@@ -4658,16 +4845,16 @@
         <v>2.2000000000000006</v>
       </c>
       <c r="L25" cm="1">
-        <f t="array" ref="L25">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K25)</f>
+        <f t="array" aca="1" ref="L25" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K25)</f>
         <v>0.3</v>
       </c>
       <c r="M25" cm="1">
-        <f t="array" ref="M25">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K25)</f>
-        <v>0.16363636363636369</v>
+        <f t="array" aca="1" ref="M25" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K25)</f>
+        <v>0.28968952670680786</v>
       </c>
       <c r="N25" cm="1">
-        <f t="array" ref="N25">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K25)</f>
-        <v>0.69767632607103092</v>
+        <f t="array" aca="1" ref="N25" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K25)</f>
+        <v>0.5287090709761838</v>
       </c>
     </row>
     <row r="26" spans="11:14" x14ac:dyDescent="0.3">
@@ -4675,16 +4862,16 @@
         <v>2.3000000000000007</v>
       </c>
       <c r="L26" cm="1">
-        <f t="array" ref="L26">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K26)</f>
+        <f t="array" aca="1" ref="L26" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K26)</f>
         <v>0.3</v>
       </c>
       <c r="M26" cm="1">
-        <f t="array" ref="M26">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K26)</f>
-        <v>0.1695652173913044</v>
+        <f t="array" aca="1" ref="M26" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K26)</f>
+        <v>0.29013780815433798</v>
       </c>
       <c r="N26" cm="1">
-        <f t="array" ref="N26">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K26)</f>
-        <v>0.67705687449816454</v>
+        <f t="array" aca="1" ref="N26" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K26)</f>
+        <v>0.51308335647541869</v>
       </c>
     </row>
     <row r="27" spans="11:14" x14ac:dyDescent="0.3">
@@ -4692,16 +4879,16 @@
         <v>2.4000000000000008</v>
       </c>
       <c r="L27" cm="1">
-        <f t="array" ref="L27">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K27)</f>
+        <f t="array" aca="1" ref="L27" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K27)</f>
         <v>0.3</v>
       </c>
       <c r="M27" cm="1">
-        <f t="array" ref="M27">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K27)</f>
-        <v>0.17500000000000004</v>
+        <f t="array" aca="1" ref="M27" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K27)</f>
+        <v>0.29054873281457388</v>
       </c>
       <c r="N27" cm="1">
-        <f t="array" ref="N27">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K27)</f>
-        <v>0.65704681981505664</v>
+        <f t="array" aca="1" ref="N27" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K27)</f>
+        <v>0.49791945162964713</v>
       </c>
     </row>
     <row r="28" spans="11:14" x14ac:dyDescent="0.3">
@@ -4709,16 +4896,16 @@
         <v>2.5000000000000009</v>
       </c>
       <c r="L28" cm="1">
-        <f t="array" ref="L28">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K28)</f>
+        <f t="array" aca="1" ref="L28" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K28)</f>
         <v>0.3</v>
       </c>
       <c r="M28" cm="1">
-        <f t="array" ref="M28">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K28)</f>
-        <v>0.18000000000000005</v>
+        <f t="array" aca="1" ref="M28" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K28)</f>
+        <v>0.29092678350199092</v>
       </c>
       <c r="N28" cm="1">
-        <f t="array" ref="N28">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K28)</f>
-        <v>0.63762815162177311</v>
+        <f t="array" aca="1" ref="N28" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K28)</f>
+        <v>0.48320370790091349</v>
       </c>
     </row>
     <row r="29" spans="11:14" x14ac:dyDescent="0.3">
@@ -4726,16 +4913,16 @@
         <v>2.600000000000001</v>
       </c>
       <c r="L29" cm="1">
-        <f t="array" ref="L29">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K29)</f>
+        <f t="array" aca="1" ref="L29" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K29)</f>
         <v>0.3</v>
       </c>
       <c r="M29" cm="1">
-        <f t="array" ref="M29">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K29)</f>
-        <v>0.18461538461538468</v>
+        <f t="array" aca="1" ref="M29" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K29)</f>
+        <v>0.291275753367299</v>
       </c>
       <c r="N29" cm="1">
-        <f t="array" ref="N29">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K29)</f>
-        <v>0.61878339180614061</v>
+        <f t="array" aca="1" ref="N29" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K29)</f>
+        <v>0.4689228801265195</v>
       </c>
     </row>
     <row r="30" spans="11:14" x14ac:dyDescent="0.3">
@@ -4743,16 +4930,16 @@
         <v>2.7000000000000011</v>
       </c>
       <c r="L30" cm="1">
-        <f t="array" ref="L30">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K30)</f>
+        <f t="array" aca="1" ref="L30" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K30)</f>
         <v>0.3</v>
       </c>
       <c r="M30" cm="1">
-        <f t="array" ref="M30">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K30)</f>
-        <v>0.18888888888888894</v>
+        <f t="array" aca="1" ref="M30" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K30)</f>
+        <v>0.29159887361295456</v>
       </c>
       <c r="N30" cm="1">
-        <f t="array" ref="N30">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K30)</f>
-        <v>0.60049557881226578</v>
+        <f t="array" aca="1" ref="N30" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K30)</f>
+        <v>0.4550641145974833</v>
       </c>
     </row>
     <row r="31" spans="11:14" x14ac:dyDescent="0.3">
@@ -4760,16 +4947,16 @@
         <v>2.8000000000000012</v>
       </c>
       <c r="L31" cm="1">
-        <f t="array" ref="L31">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K31)</f>
+        <f t="array" aca="1" ref="L31" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K31)</f>
         <v>0.3</v>
       </c>
       <c r="M31" cm="1">
-        <f t="array" ref="M31">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K31)</f>
-        <v>0.19285714285714292</v>
+        <f t="array" aca="1" ref="M31" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K31)</f>
+        <v>0.29189891384106331</v>
       </c>
       <c r="N31" cm="1">
-        <f t="array" ref="N31">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K31)</f>
-        <v>0.58274825237398942</v>
+        <f t="array" aca="1" ref="N31" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K31)</f>
+        <v>0.44161493748933417</v>
       </c>
     </row>
     <row r="32" spans="11:14" x14ac:dyDescent="0.3">
@@ -4777,16 +4964,16 @@
         <v>2.9000000000000012</v>
       </c>
       <c r="L32" cm="1">
-        <f t="array" ref="L32">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K32)</f>
+        <f t="array" aca="1" ref="L32" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K32)</f>
         <v>0.3</v>
       </c>
       <c r="M32" cm="1">
-        <f t="array" ref="M32">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K32)</f>
-        <v>0.19655172413793109</v>
+        <f t="array" aca="1" ref="M32" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K32)</f>
+        <v>0.29217826163964739</v>
       </c>
       <c r="N32" cm="1">
-        <f t="array" ref="N32">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K32)</f>
-        <v>0.56552543869953686</v>
+        <f t="array" aca="1" ref="N32" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K32)</f>
+        <v>0.42856324363482795</v>
       </c>
     </row>
     <row r="33" spans="11:14" x14ac:dyDescent="0.3">
@@ -4794,16 +4981,16 @@
         <v>3.0000000000000013</v>
       </c>
       <c r="L33" cm="1">
-        <f t="array" ref="L33">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K33)</f>
+        <f t="array" aca="1" ref="L33" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K33)</f>
         <v>0.4</v>
       </c>
       <c r="M33" cm="1">
-        <f t="array" ref="M33">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K33)</f>
-        <v>0.20000000000000012</v>
+        <f t="array" aca="1" ref="M33" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K33)</f>
+        <v>0.29243898625165921</v>
       </c>
       <c r="N33" cm="1">
-        <f t="array" ref="N33">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K33)</f>
-        <v>0.54881163609402606</v>
+        <f t="array" aca="1" ref="N33" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K33)</f>
+        <v>0.41589728562847983</v>
       </c>
     </row>
     <row r="34" spans="11:14" x14ac:dyDescent="0.3">
@@ -4811,16 +4998,16 @@
         <v>3.1000000000000014</v>
       </c>
       <c r="L34" cm="1">
-        <f t="array" ref="L34">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K34)</f>
+        <f t="array" aca="1" ref="L34" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K34)</f>
         <v>0.4</v>
       </c>
       <c r="M34" cm="1">
-        <f t="array" ref="M34">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K34)</f>
-        <v>0.20645161290322592</v>
+        <f t="array" aca="1" ref="M34" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K34)</f>
+        <v>0.29590869637257339</v>
       </c>
       <c r="N34" cm="1">
-        <f t="array" ref="N34">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K34)</f>
-        <v>0.52729242404304821</v>
+        <f t="array" aca="1" ref="N34" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K34)</f>
+        <v>0.39958971980396069</v>
       </c>
     </row>
     <row r="35" spans="11:14" x14ac:dyDescent="0.3">
@@ -4828,16 +5015,16 @@
         <v>3.2000000000000015</v>
       </c>
       <c r="L35" cm="1">
-        <f t="array" ref="L35">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K35)</f>
+        <f t="array" aca="1" ref="L35" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K35)</f>
         <v>0.4</v>
       </c>
       <c r="M35" cm="1">
-        <f t="array" ref="M35">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K35)</f>
-        <v>0.21250000000000013</v>
+        <f t="array" aca="1" ref="M35" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K35)</f>
+        <v>0.2991615496109305</v>
       </c>
       <c r="N35" cm="1">
-        <f t="array" ref="N35">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K35)</f>
-        <v>0.50661699236558921</v>
+        <f t="array" aca="1" ref="N35" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K35)</f>
+        <v>0.38392158278148136</v>
       </c>
     </row>
     <row r="36" spans="11:14" x14ac:dyDescent="0.3">
@@ -4845,16 +5032,16 @@
         <v>3.3000000000000016</v>
       </c>
       <c r="L36" cm="1">
-        <f t="array" ref="L36">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K36)</f>
+        <f t="array" aca="1" ref="L36" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K36)</f>
         <v>0.4</v>
       </c>
       <c r="M36" cm="1">
-        <f t="array" ref="M36">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K36)</f>
-        <v>0.21818181818181831</v>
+        <f t="array" aca="1" ref="M36" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K36)</f>
+        <v>0.30221726022878109</v>
       </c>
       <c r="N36" cm="1">
-        <f t="array" ref="N36">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K36)</f>
-        <v>0.48675225595997129</v>
+        <f t="array" aca="1" ref="N36" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K36)</f>
+        <v>0.36886780219909165</v>
       </c>
     </row>
     <row r="37" spans="11:14" x14ac:dyDescent="0.3">
@@ -4862,16 +5049,16 @@
         <v>3.4000000000000017</v>
       </c>
       <c r="L37" cm="1">
-        <f t="array" ref="L37">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K37)</f>
+        <f t="array" aca="1" ref="L37" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K37)</f>
         <v>0.4</v>
       </c>
       <c r="M37" cm="1">
-        <f t="array" ref="M37">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K37)</f>
-        <v>0.223529411764706</v>
+        <f t="array" aca="1" ref="M37" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K37)</f>
+        <v>0.30509322316322873</v>
       </c>
       <c r="N37" cm="1">
-        <f t="array" ref="N37">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K37)</f>
-        <v>0.46766642700990885</v>
+        <f t="array" aca="1" ref="N37" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K37)</f>
+        <v>0.35440428879621533</v>
       </c>
     </row>
     <row r="38" spans="11:14" x14ac:dyDescent="0.3">
@@ -4879,16 +5066,16 @@
         <v>3.5000000000000018</v>
       </c>
       <c r="L38" cm="1">
-        <f t="array" ref="L38">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K38)</f>
+        <f t="array" aca="1" ref="L38" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K38)</f>
         <v>0.4</v>
       </c>
       <c r="M38" cm="1">
-        <f t="array" ref="M38">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K38)</f>
-        <v>0.2285714285714287</v>
+        <f t="array" aca="1" ref="M38" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K38)</f>
+        <v>0.30780484535856506</v>
       </c>
       <c r="N38" cm="1">
-        <f t="array" ref="N38">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K38)</f>
-        <v>0.44932896411722123</v>
+        <f t="array" aca="1" ref="N38" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K38)</f>
+        <v>0.34050789786569369</v>
       </c>
     </row>
     <row r="39" spans="11:14" x14ac:dyDescent="0.3">
@@ -4896,16 +5083,16 @@
         <v>3.6000000000000019</v>
       </c>
       <c r="L39" cm="1">
-        <f t="array" ref="L39">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K39)</f>
+        <f t="array" aca="1" ref="L39" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K39)</f>
         <v>0.4</v>
       </c>
       <c r="M39" cm="1">
-        <f t="array" ref="M39">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K39)</f>
-        <v>0.23333333333333345</v>
+        <f t="array" aca="1" ref="M39" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K39)</f>
+        <v>0.31036582187638267</v>
       </c>
       <c r="N39" cm="1">
-        <f t="array" ref="N39">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K39)</f>
-        <v>0.43171052342907934</v>
+        <f t="array" aca="1" ref="N39" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K39)</f>
+        <v>0.32715639221731641</v>
       </c>
     </row>
     <row r="40" spans="11:14" x14ac:dyDescent="0.3">
@@ -4913,16 +5100,16 @@
         <v>3.700000000000002</v>
       </c>
       <c r="L40" cm="1">
-        <f t="array" ref="L40">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K40)</f>
+        <f t="array" aca="1" ref="L40" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K40)</f>
         <v>0.4</v>
       </c>
       <c r="M40" cm="1">
-        <f t="array" ref="M40">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K40)</f>
-        <v>0.23783783783783796</v>
+        <f t="array" aca="1" ref="M40" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K40)</f>
+        <v>0.31278836723107506</v>
       </c>
       <c r="N40" cm="1">
-        <f t="array" ref="N40">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K40)</f>
-        <v>0.41478291168158099</v>
+        <f t="array" aca="1" ref="N40" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K40)</f>
+        <v>0.31432840659357286</v>
       </c>
     </row>
     <row r="41" spans="11:14" x14ac:dyDescent="0.3">
@@ -4930,16 +5117,16 @@
         <v>3.800000000000002</v>
       </c>
       <c r="L41" cm="1">
-        <f t="array" ref="L41">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K41)</f>
+        <f t="array" aca="1" ref="L41" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K41)</f>
         <v>0.4</v>
       </c>
       <c r="M41" cm="1">
-        <f t="array" ref="M41">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K41)</f>
-        <v>0.24210526315789485</v>
+        <f t="array" aca="1" ref="M41" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K41)</f>
+        <v>0.31508341019867836</v>
       </c>
       <c r="N41" cm="1">
-        <f t="array" ref="N41">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K41)</f>
-        <v>0.3985190410845138</v>
+        <f t="array" aca="1" ref="N41" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K41)</f>
+        <v>0.30200341348068227</v>
       </c>
     </row>
     <row r="42" spans="11:14" x14ac:dyDescent="0.3">
@@ -4947,16 +5134,16 @@
         <v>3.9000000000000021</v>
       </c>
       <c r="L42" cm="1">
-        <f t="array" ref="L42">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K42)</f>
+        <f t="array" aca="1" ref="L42" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K42)</f>
         <v>0.4</v>
       </c>
       <c r="M42" cm="1">
-        <f t="array" ref="M42">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K42)</f>
-        <v>0.24615384615384628</v>
+        <f t="array" aca="1" ref="M42" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K42)</f>
+        <v>0.31726075865512249</v>
       </c>
       <c r="N42" cm="1">
-        <f t="array" ref="N42">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K42)</f>
-        <v>0.38289288597511167</v>
+        <f t="array" aca="1" ref="N42" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K42)</f>
+        <v>0.2901616902601919</v>
       </c>
     </row>
     <row r="43" spans="11:14" x14ac:dyDescent="0.3">
@@ -4964,16 +5151,16 @@
         <v>4.0000000000000018</v>
       </c>
       <c r="L43" cm="1">
-        <f t="array" ref="L43">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K43)</f>
+        <f t="array" aca="1" ref="L43" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K43)</f>
         <v>0.4</v>
       </c>
       <c r="M43" cm="1">
-        <f t="array" ref="M43">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K43)</f>
-        <v>0.25000000000000011</v>
+        <f t="array" aca="1" ref="M43" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K43)</f>
+        <v>0.31932923968874438</v>
       </c>
       <c r="N43" cm="1">
-        <f t="array" ref="N43">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K43)</f>
-        <v>0.367879441171442</v>
+        <f t="array" aca="1" ref="N43" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K43)</f>
+        <v>0.27878428764857993</v>
       </c>
     </row>
   </sheetData>
@@ -4982,7 +5169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8A3DD8-75E7-4A72-9366-AF366CC35FAC}">
   <dimension ref="B1:G552"/>
   <sheetViews>
@@ -5012,7 +5199,7 @@
       </c>
       <c r="E2" s="5" cm="1">
         <f t="array" ref="E2">_xll.\TMX.BOND.SIMPLE(D2,D3,D4,D5)</f>
-        <v>2394369033232</v>
+        <v>2319073701568</v>
       </c>
       <c r="F2" cm="1">
         <f t="array" ref="F2:F5">_xll.TMX.BOND.SIMPLE(E2)</f>
@@ -5067,10 +5254,10 @@
         <v>31</v>
       </c>
       <c r="D5" s="5">
-        <v>140716345864955</v>
+        <v>140716431061820</v>
       </c>
       <c r="F5" s="5">
-        <v>140716345864955</v>
+        <v>140716431061820</v>
       </c>
       <c r="G5" s="17" t="b">
         <f t="shared" si="0"/>
@@ -5083,7 +5270,7 @@
       </c>
       <c r="C6" s="5" cm="1">
         <f t="array" ref="C6">_xll.\TMX.BOND.SIMPLE(maturity, coupon, _xll.ENUM(frequency), _xll.ENUM(day_count))</f>
-        <v>2394369038320</v>
+        <v>2319073704352</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -5092,25 +5279,25 @@
       </c>
       <c r="C7" s="2">
         <f ca="1">TODAY()</f>
-        <v>45091</v>
+        <v>45093</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="5" cm="1">
+      <c r="C8" s="5" t="e" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_xll.\TMX.BOND.INSTRUMENT(bond.simple, dated)</f>
-        <v>2392569839008</v>
+        <v>#NUM!</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C9" s="20" cm="1">
+      <c r="C9" s="20" t="e" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">_xll.TMX.VALUE.YIELD(instrument, 1)</f>
-        <v>4.8786680314628891E-2</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
@@ -5129,9 +5316,9 @@
       <c r="B12" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="20" cm="1">
+      <c r="C12" s="20" t="e" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">_xll.TMX.VALUE.COMPOUND_YIELD(C9,12/_xll.ENUM(frequency))</f>
-        <v>4.9996341958828738E-2</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
@@ -5147,122 +5334,85 @@
       <c r="G13" s="2"/>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C14" cm="1">
-        <f t="array" aca="1" ref="C14:D17" ca="1">TRANSPOSE(_xll.TMX.INSTRUMENT(instrument))</f>
-        <v>1.0020739645577939</v>
-      </c>
-      <c r="D14">
-        <f ca="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="E14" s="2" cm="1">
-        <f t="array" aca="1" ref="E14:E17" ca="1">_xlfn.MAP(INDEX(_xlfn.ANCHORARRAY(C14),,1),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.DATE.ADD_YEARS(dated,_xlpm.t)))</f>
-        <v>45457</v>
+      <c r="C14" t="e" cm="1">
+        <f t="array" aca="1" ref="C14" ca="1">TRANSPOSE(_xll.TMX.INSTRUMENT(instrument))</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E14" s="2" t="e" cm="1">
+        <f t="array" aca="1" ref="E14" ca="1">_xlfn.MAP(INDEX(_xlfn.ANCHORARRAY(C14),,1),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.DATE.ADD_YEARS(dated,_xlpm.t)))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="G14" s="2"/>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C15">
-        <f ca="1"/>
-        <v>2.0014100221085989</v>
-      </c>
-      <c r="D15">
-        <f ca="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="E15" s="2">
-        <f ca="1"/>
-        <v>45821.999988425923</v>
-      </c>
+      <c r="E15" s="2"/>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C16">
-        <f ca="1"/>
-        <v>3.0007460796594043</v>
-      </c>
-      <c r="D16">
-        <f ca="1"/>
-        <v>0.05</v>
-      </c>
-      <c r="E16" s="2">
-        <f ca="1"/>
-        <v>46187</v>
-      </c>
+      <c r="E16" s="2"/>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C17">
-        <f ca="1"/>
-        <v>4.0000821372102093</v>
-      </c>
-      <c r="D17">
-        <f ca="1"/>
-        <v>1.05</v>
-      </c>
-      <c r="E17" s="2">
-        <f ca="1"/>
-        <v>46552</v>
-      </c>
+    <row r="17" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E17" s="2"/>
       <c r="G17" s="2"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E19" s="2"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E20" s="2"/>
       <c r="G20" s="2"/>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E21" s="2"/>
       <c r="G21" s="2"/>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E22" s="2"/>
       <c r="G22" s="2"/>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E23" s="2"/>
       <c r="G23" s="2"/>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E32" s="2"/>
       <c r="G32" s="2"/>
     </row>
@@ -7174,11 +7324,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92863B8-4C87-4474-B5B0-52EEB5BB3C33}">
   <dimension ref="B2:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7231,9 +7381,9 @@
       <c r="F6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="5" cm="1">
-        <f t="array" ref="G6">_xll.\TMX.BOOTSTRAP(instrument, price)</f>
-        <v>2392573154048</v>
+      <c r="G6" s="5" t="e" cm="1">
+        <f t="array" aca="1" ref="G6" ca="1">_xll.\TMX.BOOTSTRAP(instrument, price)</f>
+        <v>#NUM!</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>16</v>
@@ -7254,19 +7404,19 @@
       </c>
       <c r="E7" s="5" cm="1">
         <f t="array" ref="E7">_xll.\TMX.BOND.SIMPLE(B7, C7)</f>
-        <v>2394369038032</v>
+        <v>2319073702816</v>
       </c>
       <c r="F7" s="5" cm="1">
         <f t="array" ref="F7">_xll.\TMX.BOND.INSTRUMENT(E7, dated)</f>
-        <v>2392574244672</v>
+        <v>2319074063488</v>
       </c>
       <c r="H7" cm="1">
         <f t="array" ref="H7:H107">_xlfn.SEQUENCE(1+10/H5,1,0,H5)</f>
         <v>0</v>
       </c>
-      <c r="I7" s="21" cm="1">
-        <f t="array" ref="I7:I107">_xlfn.MAP(_xlfn.ANCHORARRAY(H7),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.PWFLAT.CURVE.VALUE(curve,_xlpm.t)))</f>
-        <v>4.9688644922257018E-2</v>
+      <c r="I7" s="21" t="e" cm="1">
+        <f t="array" aca="1" ref="I7:I107" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(H7),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.PWFLAT.CURVE.VALUE(curve,_xlpm.t)))</f>
+        <v>#VALUE!</v>
       </c>
       <c r="J7" s="2"/>
     </row>
@@ -7275,24 +7425,26 @@
         <v>2</v>
       </c>
       <c r="C8" s="18">
-        <v>5.0999999999999997E-2</v>
+        <f ca="1">0.05 + 0.01*RAND()</f>
+        <v>5.3918100718761297E-2</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
       </c>
       <c r="E8" s="5" cm="1">
-        <f t="array" ref="E8">_xll.\TMX.BOND.SIMPLE(B8, C8)</f>
-        <v>2394369041488</v>
+        <f t="array" aca="1" ref="E8" ca="1">_xll.\TMX.BOND.SIMPLE(B8, C8)</f>
+        <v>2534307269392</v>
       </c>
       <c r="F8" s="5" cm="1">
-        <f t="array" ref="F8">_xll.\TMX.BOND.INSTRUMENT(E8, dated)</f>
-        <v>2392574249856</v>
+        <f t="array" aca="1" ref="F8" ca="1">_xll.\TMX.BOND.INSTRUMENT(E8, dated)</f>
+        <v>2536171316944</v>
       </c>
       <c r="H8">
         <v>0.1</v>
       </c>
-      <c r="I8">
-        <v>4.9688644922257018E-2</v>
+      <c r="I8" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.3">
@@ -7307,17 +7459,18 @@
       </c>
       <c r="E9" s="5" cm="1">
         <f t="array" ref="E9">_xll.\TMX.BOND.SIMPLE(B9, C9)</f>
-        <v>2394369041392</v>
+        <v>2319073701280</v>
       </c>
       <c r="F9" s="5" cm="1">
         <f t="array" ref="F9">_xll.\TMX.BOND.INSTRUMENT(E9, dated)</f>
-        <v>2392574243808</v>
+        <v>2319074061040</v>
       </c>
       <c r="H9">
         <v>0.2</v>
       </c>
-      <c r="I9">
-        <v>4.9688644922257018E-2</v>
+      <c r="I9" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
@@ -7332,17 +7485,18 @@
       </c>
       <c r="E10" s="5" cm="1">
         <f t="array" ref="E10">_xll.\TMX.BOND.SIMPLE(B10, C10)</f>
-        <v>2394369042064</v>
+        <v>2319073705696</v>
       </c>
       <c r="F10" s="5" cm="1">
         <f t="array" ref="F10">_xll.\TMX.BOND.INSTRUMENT(E10, dated)</f>
-        <v>2392574245824</v>
+        <v>2319074060032</v>
       </c>
       <c r="H10">
         <v>0.30000000000000004</v>
       </c>
-      <c r="I10">
-        <v>4.9688644922257018E-2</v>
+      <c r="I10" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.3">
@@ -7357,17 +7511,18 @@
       </c>
       <c r="E11" s="5" cm="1">
         <f t="array" ref="E11">_xll.\TMX.BOND.SIMPLE(B11, C11)</f>
-        <v>2394369041584</v>
+        <v>2319073700512</v>
       </c>
       <c r="F11" s="5" cm="1">
         <f t="array" ref="F11">_xll.\TMX.BOND.INSTRUMENT(E11, dated)</f>
-        <v>2392574249280</v>
+        <v>2319074063776</v>
       </c>
       <c r="H11">
         <v>0.4</v>
       </c>
-      <c r="I11">
-        <v>4.9688644922257018E-2</v>
+      <c r="I11" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
@@ -7382,17 +7537,18 @@
       </c>
       <c r="E12" s="5" cm="1">
         <f t="array" ref="E12">_xll.\TMX.BOND.SIMPLE(B12, C12)</f>
-        <v>2394369037072</v>
+        <v>2319073705600</v>
       </c>
       <c r="F12" s="5" cm="1">
         <f t="array" ref="F12">_xll.\TMX.BOND.INSTRUMENT(E12, dated)</f>
-        <v>2392574242512</v>
+        <v>2319074065360</v>
       </c>
       <c r="H12">
         <v>0.5</v>
       </c>
-      <c r="I12">
-        <v>4.9688644922257018E-2</v>
+      <c r="I12" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
@@ -7407,17 +7563,18 @@
       </c>
       <c r="E13" s="5" cm="1">
         <f t="array" ref="E13">_xll.\TMX.BOND.SIMPLE(B13, C13)</f>
-        <v>2394369040912</v>
+        <v>2319073705792</v>
       </c>
       <c r="F13" s="5" cm="1">
         <f t="array" ref="F13">_xll.\TMX.BOND.INSTRUMENT(E13, dated)</f>
-        <v>2392574247840</v>
+        <v>2319074064352</v>
       </c>
       <c r="H13">
         <v>0.6</v>
       </c>
-      <c r="I13">
-        <v>4.9688644922257018E-2</v>
+      <c r="I13" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
@@ -7432,17 +7589,18 @@
       </c>
       <c r="E14" s="5" cm="1">
         <f t="array" ref="E14">_xll.\TMX.BOND.SIMPLE(B14, C14)</f>
-        <v>2394369041968</v>
+        <v>2319073703392</v>
       </c>
       <c r="F14" s="5" cm="1">
         <f t="array" ref="F14">_xll.\TMX.BOND.INSTRUMENT(E14, dated)</f>
-        <v>2392574242800</v>
+        <v>2319074063632</v>
       </c>
       <c r="H14">
         <v>0.7</v>
       </c>
-      <c r="I14">
-        <v>4.9688644922257018E-2</v>
+      <c r="I14" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.3">
@@ -7457,17 +7615,18 @@
       </c>
       <c r="E15" s="5" cm="1">
         <f t="array" ref="E15">_xll.\TMX.BOND.SIMPLE(B15, C15)</f>
-        <v>2394369042256</v>
+        <v>2319073705504</v>
       </c>
       <c r="F15" s="5" cm="1">
         <f t="array" ref="F15">_xll.\TMX.BOND.INSTRUMENT(E15, dated)</f>
-        <v>2392574246976</v>
+        <v>2319074063344</v>
       </c>
       <c r="H15">
         <v>0.79999999999999993</v>
       </c>
-      <c r="I15">
-        <v>4.9688644922257018E-2</v>
+      <c r="I15" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
@@ -7482,749 +7641,841 @@
       </c>
       <c r="E16" s="5" cm="1">
         <f t="array" ref="E16">_xll.\TMX.BOND.SIMPLE(B16, C16)</f>
-        <v>2394369031504</v>
+        <v>2319073700608</v>
       </c>
       <c r="F16" s="5" cm="1">
         <f t="array" ref="F16">_xll.\TMX.BOND.INSTRUMENT(E16, dated)</f>
-        <v>2392574249424</v>
+        <v>2319074066800</v>
       </c>
       <c r="H16">
         <v>0.89999999999999991</v>
       </c>
-      <c r="I16">
-        <v>4.9688644922257018E-2</v>
+      <c r="I16" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="17" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H17">
         <v>0.99999999999999989</v>
       </c>
-      <c r="I17">
-        <v>4.9688644922257018E-2</v>
+      <c r="I17" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="18" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H18">
         <v>1.0999999999999999</v>
       </c>
-      <c r="I18">
-        <v>5.1859212468108845E-2</v>
+      <c r="I18" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="19" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H19">
         <v>1.2</v>
       </c>
-      <c r="I19">
-        <v>5.1859212468108845E-2</v>
+      <c r="I19" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="20" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H20">
         <v>1.3</v>
       </c>
-      <c r="I20">
-        <v>5.1859212468108845E-2</v>
+      <c r="I20" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="21" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H21">
         <v>1.4000000000000001</v>
       </c>
-      <c r="I21">
-        <v>5.1859212468108845E-2</v>
-      </c>
-      <c r="K21" cm="1">
-        <f t="array" ref="K21">_xll.TMX.PWFLAT.CURVE.VALUE(curve, H21)</f>
-        <v>5.1859212468108845E-2</v>
+      <c r="I21" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K21" t="e" cm="1">
+        <f t="array" aca="1" ref="K21" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve, H21)</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="22" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H22">
         <v>1.5000000000000002</v>
       </c>
-      <c r="I22">
-        <v>5.1859212468108845E-2</v>
+      <c r="I22" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="23" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H23">
         <v>1.6000000000000003</v>
       </c>
-      <c r="I23">
-        <v>5.1859212468108845E-2</v>
+      <c r="I23" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="24" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H24">
         <v>1.7000000000000004</v>
       </c>
-      <c r="I24">
-        <v>5.1859212468108845E-2</v>
+      <c r="I24" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="25" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H25">
         <v>1.8000000000000005</v>
       </c>
-      <c r="I25">
-        <v>5.1859212468108845E-2</v>
+      <c r="I25" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="26" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H26">
         <v>1.9000000000000006</v>
       </c>
-      <c r="I26">
-        <v>5.1859212468108845E-2</v>
+      <c r="I26" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="27" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H27">
         <v>2.0000000000000004</v>
       </c>
-      <c r="I27">
-        <v>5.1859212468108845E-2</v>
+      <c r="I27" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="28" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H28">
         <v>2.1000000000000005</v>
       </c>
-      <c r="I28">
-        <v>4.7683063278025691E-2</v>
+      <c r="I28" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="29" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H29">
         <v>2.2000000000000006</v>
       </c>
-      <c r="I29">
-        <v>4.7683063278025691E-2</v>
+      <c r="I29" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="30" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H30">
         <v>2.3000000000000007</v>
       </c>
-      <c r="I30">
-        <v>4.7683063278025691E-2</v>
+      <c r="I30" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="31" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H31">
         <v>2.4000000000000008</v>
       </c>
-      <c r="I31">
-        <v>4.7683063278025691E-2</v>
+      <c r="I31" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="32" spans="8:11" x14ac:dyDescent="0.3">
       <c r="H32">
         <v>2.5000000000000009</v>
       </c>
-      <c r="I32">
-        <v>4.7683063278025691E-2</v>
+      <c r="I32" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="33" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H33">
         <v>2.600000000000001</v>
       </c>
-      <c r="I33">
-        <v>4.7683063278025691E-2</v>
+      <c r="I33" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="34" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H34">
         <v>2.7000000000000011</v>
       </c>
-      <c r="I34">
-        <v>4.7683063278025691E-2</v>
+      <c r="I34" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="35" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H35">
         <v>2.8000000000000012</v>
       </c>
-      <c r="I35">
-        <v>4.7683063278025691E-2</v>
+      <c r="I35" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="36" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H36">
         <v>2.9000000000000012</v>
       </c>
-      <c r="I36">
-        <v>4.7683063278025691E-2</v>
+      <c r="I36" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="37" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H37">
         <v>3.0000000000000013</v>
       </c>
-      <c r="I37">
-        <v>4.7683063278025691E-2</v>
+      <c r="I37" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="38" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H38">
         <v>3.1000000000000014</v>
       </c>
-      <c r="I38">
-        <v>4.9823073127630173E-2</v>
+      <c r="I38" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="39" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H39">
         <v>3.2000000000000015</v>
       </c>
-      <c r="I39">
-        <v>4.9823073127630173E-2</v>
+      <c r="I39" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="40" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H40">
         <v>3.3000000000000016</v>
       </c>
-      <c r="I40">
-        <v>4.9823073127630173E-2</v>
+      <c r="I40" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="41" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H41">
         <v>3.4000000000000017</v>
       </c>
-      <c r="I41">
-        <v>4.9823073127630173E-2</v>
+      <c r="I41" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="42" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H42">
         <v>3.5000000000000018</v>
       </c>
-      <c r="I42">
-        <v>4.9823073127630173E-2</v>
+      <c r="I42" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="43" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H43">
         <v>3.6000000000000019</v>
       </c>
-      <c r="I43">
-        <v>4.9823073127630173E-2</v>
+      <c r="I43" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="44" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H44">
         <v>3.700000000000002</v>
       </c>
-      <c r="I44">
-        <v>4.9823073127630173E-2</v>
+      <c r="I44" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="45" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H45">
         <v>3.800000000000002</v>
       </c>
-      <c r="I45">
-        <v>4.9823073127630173E-2</v>
+      <c r="I45" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="46" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H46">
         <v>3.9000000000000021</v>
       </c>
-      <c r="I46">
-        <v>4.9823073127630173E-2</v>
+      <c r="I46" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="47" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H47">
         <v>4.0000000000000018</v>
       </c>
-      <c r="I47">
-        <v>4.9823073127630173E-2</v>
+      <c r="I47" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="48" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H48">
         <v>4.1000000000000014</v>
       </c>
-      <c r="I48">
-        <v>4.9688644922258357E-2</v>
+      <c r="I48" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="49" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H49">
         <v>4.2000000000000011</v>
       </c>
-      <c r="I49">
-        <v>4.9688644922258357E-2</v>
+      <c r="I49" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="50" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H50">
         <v>4.3000000000000007</v>
       </c>
-      <c r="I50">
-        <v>4.9688644922258357E-2</v>
+      <c r="I50" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="51" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H51">
         <v>4.4000000000000004</v>
       </c>
-      <c r="I51">
-        <v>4.9688644922258357E-2</v>
+      <c r="I51" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="52" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H52">
         <v>4.5</v>
       </c>
-      <c r="I52">
-        <v>4.9688644922258357E-2</v>
+      <c r="I52" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="53" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H53">
         <v>4.5999999999999996</v>
       </c>
-      <c r="I53">
-        <v>4.9688644922258357E-2</v>
+      <c r="I53" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="54" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H54">
         <v>4.6999999999999993</v>
       </c>
-      <c r="I54">
-        <v>4.9688644922258357E-2</v>
+      <c r="I54" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="55" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H55">
         <v>4.7999999999999989</v>
       </c>
-      <c r="I55">
-        <v>4.9688644922258357E-2</v>
+      <c r="I55" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="56" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H56">
         <v>4.8999999999999986</v>
       </c>
-      <c r="I56">
-        <v>4.9688644922258357E-2</v>
+      <c r="I56" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="57" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H57">
         <v>4.9999999999999982</v>
       </c>
-      <c r="I57">
-        <v>4.9688644922258357E-2</v>
+      <c r="I57" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="58" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H58">
         <v>5.0999999999999979</v>
       </c>
-      <c r="I58">
-        <v>4.9823073127630096E-2</v>
+      <c r="I58" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="59" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H59">
         <v>5.1999999999999975</v>
       </c>
-      <c r="I59">
-        <v>4.9823073127630096E-2</v>
+      <c r="I59" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="60" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H60">
         <v>5.2999999999999972</v>
       </c>
-      <c r="I60">
-        <v>4.9823073127630096E-2</v>
+      <c r="I60" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="61" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H61">
         <v>5.3999999999999968</v>
       </c>
-      <c r="I61">
-        <v>4.9823073127630096E-2</v>
+      <c r="I61" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="62" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H62">
         <v>5.4999999999999964</v>
       </c>
-      <c r="I62">
-        <v>4.9823073127630096E-2</v>
+      <c r="I62" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="63" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H63">
         <v>5.5999999999999961</v>
       </c>
-      <c r="I63">
-        <v>4.9823073127630096E-2</v>
+      <c r="I63" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="64" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H64">
         <v>5.6999999999999957</v>
       </c>
-      <c r="I64">
-        <v>4.9823073127630096E-2</v>
+      <c r="I64" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="65" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H65">
         <v>5.7999999999999954</v>
       </c>
-      <c r="I65">
-        <v>4.9823073127630096E-2</v>
+      <c r="I65" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="66" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H66">
         <v>5.899999999999995</v>
       </c>
-      <c r="I66">
-        <v>4.9823073127630096E-2</v>
+      <c r="I66" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="67" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H67">
         <v>5.9999999999999947</v>
       </c>
-      <c r="I67">
-        <v>4.9823073127630096E-2</v>
+      <c r="I67" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="68" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H68">
         <v>6.0999999999999943</v>
       </c>
-      <c r="I68">
-        <v>4.9823073127630096E-2</v>
+      <c r="I68" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="69" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H69">
         <v>6.199999999999994</v>
       </c>
-      <c r="I69">
-        <v>4.9823073127630096E-2</v>
+      <c r="I69" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="70" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H70">
         <v>6.2999999999999936</v>
       </c>
-      <c r="I70">
-        <v>4.9823073127630096E-2</v>
+      <c r="I70" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="71" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H71">
         <v>6.3999999999999932</v>
       </c>
-      <c r="I71">
-        <v>4.9823073127630096E-2</v>
+      <c r="I71" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="72" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H72">
         <v>6.4999999999999929</v>
       </c>
-      <c r="I72">
-        <v>4.9823073127630096E-2</v>
+      <c r="I72" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="73" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H73">
         <v>6.5999999999999925</v>
       </c>
-      <c r="I73">
-        <v>4.9823073127630096E-2</v>
+      <c r="I73" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="74" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H74">
         <v>6.6999999999999922</v>
       </c>
-      <c r="I74">
-        <v>4.9823073127630096E-2</v>
+      <c r="I74" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="75" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H75">
         <v>6.7999999999999918</v>
       </c>
-      <c r="I75">
-        <v>4.9823073127630096E-2</v>
+      <c r="I75" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="76" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H76">
         <v>6.8999999999999915</v>
       </c>
-      <c r="I76">
-        <v>4.9823073127630096E-2</v>
+      <c r="I76" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="77" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H77">
         <v>6.9999999999999911</v>
       </c>
-      <c r="I77">
-        <v>4.9823073127630096E-2</v>
+      <c r="I77" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="78" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H78">
         <v>7.0999999999999908</v>
       </c>
-      <c r="I78">
-        <v>4.9823073127630096E-2</v>
+      <c r="I78" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="79" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H79">
         <v>7.1999999999999904</v>
       </c>
-      <c r="I79">
-        <v>4.9823073127630096E-2</v>
+      <c r="I79" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="80" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H80">
         <v>7.2999999999999901</v>
       </c>
-      <c r="I80">
-        <v>4.9823073127630096E-2</v>
+      <c r="I80" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="81" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H81">
         <v>7.3999999999999897</v>
       </c>
-      <c r="I81">
-        <v>4.9823073127630096E-2</v>
+      <c r="I81" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="82" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H82">
         <v>7.4999999999999893</v>
       </c>
-      <c r="I82">
-        <v>4.9823073127630096E-2</v>
+      <c r="I82" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="83" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H83">
         <v>7.599999999999989</v>
       </c>
-      <c r="I83">
-        <v>4.9823073127630096E-2</v>
+      <c r="I83" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="84" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H84">
         <v>7.6999999999999886</v>
       </c>
-      <c r="I84">
-        <v>4.9823073127630096E-2</v>
+      <c r="I84" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="85" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H85">
         <v>7.7999999999999883</v>
       </c>
-      <c r="I85">
-        <v>4.9823073127630096E-2</v>
+      <c r="I85" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="86" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H86">
         <v>7.8999999999999879</v>
       </c>
-      <c r="I86">
-        <v>4.9823073127630096E-2</v>
+      <c r="I86" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="87" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H87">
         <v>7.9999999999999876</v>
       </c>
-      <c r="I87">
-        <v>4.9823073127630096E-2</v>
+      <c r="I87" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="88" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H88">
         <v>8.0999999999999872</v>
       </c>
-      <c r="I88">
-        <v>4.9688644922257615E-2</v>
+      <c r="I88" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="89" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H89">
         <v>8.1999999999999869</v>
       </c>
-      <c r="I89">
-        <v>4.9688644922257615E-2</v>
+      <c r="I89" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="90" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H90">
         <v>8.2999999999999865</v>
       </c>
-      <c r="I90">
-        <v>4.9688644922257615E-2</v>
+      <c r="I90" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="91" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H91">
         <v>8.3999999999999861</v>
       </c>
-      <c r="I91">
-        <v>4.9688644922257615E-2</v>
+      <c r="I91" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="92" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H92">
         <v>8.4999999999999858</v>
       </c>
-      <c r="I92">
-        <v>4.9688644922257615E-2</v>
+      <c r="I92" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="93" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H93">
         <v>8.5999999999999854</v>
       </c>
-      <c r="I93">
-        <v>4.9688644922257615E-2</v>
+      <c r="I93" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="94" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H94">
         <v>8.6999999999999851</v>
       </c>
-      <c r="I94">
-        <v>4.9688644922257615E-2</v>
+      <c r="I94" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="95" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H95">
         <v>8.7999999999999847</v>
       </c>
-      <c r="I95">
-        <v>4.9688644922257615E-2</v>
+      <c r="I95" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="96" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H96">
         <v>8.8999999999999844</v>
       </c>
-      <c r="I96">
-        <v>4.9688644922257615E-2</v>
+      <c r="I96" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="97" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H97">
         <v>8.999999999999984</v>
       </c>
-      <c r="I97">
-        <v>4.9688644922257615E-2</v>
+      <c r="I97" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="98" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H98">
         <v>9.0999999999999837</v>
       </c>
-      <c r="I98">
-        <v>4.9823073127629867E-2</v>
+      <c r="I98" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="99" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H99">
         <v>9.1999999999999833</v>
       </c>
-      <c r="I99">
-        <v>4.9823073127629867E-2</v>
+      <c r="I99" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="100" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H100">
         <v>9.2999999999999829</v>
       </c>
-      <c r="I100">
-        <v>4.9823073127629867E-2</v>
+      <c r="I100" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="101" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H101">
         <v>9.3999999999999826</v>
       </c>
-      <c r="I101">
-        <v>4.9823073127629867E-2</v>
+      <c r="I101" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="102" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H102">
         <v>9.4999999999999822</v>
       </c>
-      <c r="I102">
-        <v>4.9823073127629867E-2</v>
+      <c r="I102" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="103" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H103">
         <v>9.5999999999999819</v>
       </c>
-      <c r="I103">
-        <v>4.9823073127629867E-2</v>
+      <c r="I103" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="104" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H104">
         <v>9.6999999999999815</v>
       </c>
-      <c r="I104">
-        <v>4.9823073127629867E-2</v>
+      <c r="I104" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="105" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H105">
         <v>9.7999999999999812</v>
       </c>
-      <c r="I105">
-        <v>4.9823073127629867E-2</v>
+      <c r="I105" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="106" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H106">
         <v>9.8999999999999808</v>
       </c>
-      <c r="I106">
-        <v>4.9823073127629867E-2</v>
+      <c r="I106" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="107" spans="8:9" x14ac:dyDescent="0.3">
       <c r="H107">
         <v>9.9999999999999805</v>
       </c>
-      <c r="I107">
-        <v>4.9823073127629867E-2</v>
+      <c r="I107" t="e">
+        <f ca="1"/>
+        <v>#VALUE!</v>
       </c>
     </row>
   </sheetData>
@@ -8232,4 +8483,143 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CE10814-8BAC-41F3-9E28-9FC194E23C82}">
+  <dimension ref="B2:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.69921875" customWidth="1"/>
+    <col min="5" max="5" width="11.69921875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="9">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B6" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6">
+        <f>EXP(-r_*t)</f>
+        <v>0.36787944117144233</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7">
+        <f>EXP(-r_*u)</f>
+        <v>0.1353352832366127</v>
+      </c>
+      <c r="E7">
+        <f>Du/Dt</f>
+        <v>0.36787944117144233</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8">
+        <f ca="1">EXP(-r_*(u-t)-σ^2*(u-t)^3/6-σ*(u-t)*_xlfn.NORM.S.INV(RAND())*SQRT(t))</f>
+        <v>0.18096584160211318</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C9">
+        <f ca="1">LN(C8)</f>
+        <v>-1.7094469859565664</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B10" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" cm="1">
+        <f t="array" ref="C10">_xll.TMX.HO_LEE.ED(Dt, Du, t, u, σ)</f>
+        <v>0.34993774911115538</v>
+      </c>
+      <c r="D10" s="16" cm="1">
+        <f t="array" aca="1" ref="D10" ca="1">_xll.MONTE.MEAN(C8)</f>
+        <v>0.38067879287846046</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B11" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" cm="1">
+        <f t="array" ref="C11">_xll.TMX.HO_LEE.ELogD(Dt, Du, t, u, σ)</f>
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="D11" s="16">
+        <f t="array" aca="1" ref="D11:D12" ca="1">_xll.MONTE.STDEV(logD)</f>
+        <v>-1.016185039685831</v>
+      </c>
+      <c r="E11">
+        <f ca="1">(C11-D11)/D12</f>
+        <v>-0.26395273052976648</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B12" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" cm="1">
+        <f t="array" ref="C12">_xll.TMX.HO_LEE.VarLogD(t, u, σ)</f>
+        <v>0.1</v>
+      </c>
+      <c r="D12" s="16">
+        <f ca="1"/>
+        <v>0.31753776574293535</v>
+      </c>
+      <c r="E12" s="16">
+        <f>SQRT(C12)</f>
+        <v>0.31622776601683794</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bootstrap uses instruments xmod update xll uses new bondlib
</commit_message>
<xml_diff>
--- a/bondxll/bondlib.xlsx
+++ b/bondxll/bondlib.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keith\source\repos\tmcrossx\bondlib\bondxll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AB576B-25BB-4CCA-A315-303B0B7AB80F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0823582-6D0A-4E41-8280-228E726DE51F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{06412BBD-41CB-406E-9C18-9630F19E364B}"/>
+    <workbookView xWindow="1500" yWindow="1350" windowWidth="27030" windowHeight="14130" activeTab="5" xr2:uid="{06412BBD-41CB-406E-9C18-9630F19E364B}"/>
   </bookViews>
   <sheets>
     <sheet name="Enum" sheetId="4" r:id="rId1"/>
@@ -60,6 +60,7 @@
     <definedName name="σ">'Ho-Lee'!$C$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -102,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="60">
   <si>
     <t>maturity</t>
   </si>
@@ -168,15 +169,6 @@
   </si>
   <si>
     <t>discount</t>
-  </si>
-  <si>
-    <t>shift</t>
-  </si>
-  <si>
-    <t>translate</t>
-  </si>
-  <si>
-    <t>curve_</t>
   </si>
   <si>
     <t>frequency</t>
@@ -506,7 +498,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>value</c:v>
+                  <c:v>forward</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -662,37 +654,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>0.2</c:v>
@@ -752,37 +744,37 @@
                   <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -959,127 +951,127 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.25184833824705466</c:v>
+                  <c:v>0.95851248793963784</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.24713485295186788</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.24320694853921221</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.23988333711311896</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.23703452731932476</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.23456555883136976</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.23240521140440915</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.23049902249826745</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.22880463235947482</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.22728859907739721</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.22592416912352734</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.22945158964145462</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.23265833556684307</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.23558623402045858</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.2382701409362728</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.24073933529882191</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.24301859163348261</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.24512901416557584</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.24708869223109098</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.24891322008519129</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1259,124 +1251,124 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.97512965842601385</c:v>
+                  <c:v>0.90859916123799112</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.95087785074203446</c:v>
+                  <c:v>0.82555243580238102</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.92722919379894231</c:v>
+                  <c:v>0.75009625072802388</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.90416868703179076</c:v>
+                  <c:v>0.68153682425924444</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.88168170294480752</c:v>
+                  <c:v>0.61924378687475368</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.85975397783303642</c:v>
+                  <c:v>0.56264438535623851</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.83837160273473554</c:v>
+                  <c:v>0.51121821660994338</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.81752101460879245</c:v>
+                  <c:v>0.46449244282137631</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.79718898773156011</c:v>
+                  <c:v>0.42203744394888804</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.77736262530765599</c:v>
+                  <c:v>0.38346286758298537</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.76196981400482067</c:v>
+                  <c:v>0.37586979406724619</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.74688180078732025</c:v>
+                  <c:v>0.36842707348079806</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.73209255024869169</c:v>
+                  <c:v>0.36113172863616871</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.71759614649152659</c:v>
+                  <c:v>0.35398084129814772</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.70338679076103439</c:v>
+                  <c:v>0.34697155101645349</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.68945879912546226</c:v>
+                  <c:v>0.34010105398151486</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.67580660020244676</c:v>
+                  <c:v>0.33336660190291001</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.66242473293038706</c:v>
+                  <c:v>0.32676550091001366</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.64930784438394706</c:v>
+                  <c:v>0.32029511047441273</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.63645068763281409</c:v>
+                  <c:v>0.31395284235366</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.61764072713714113</c:v>
+                  <c:v>0.30467413360696821</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.59938668498789149</c:v>
+                  <c:v>0.29566965214664376</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.58167213131494588</c:v>
+                  <c:v>0.28693129333155148</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.5644811218242306</c:v>
+                  <c:v>0.27845119204890095</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.54779818344677589</c:v>
+                  <c:v>0.27022171563511382</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.53160830041190998</c:v>
+                  <c:v>0.26223545700591128</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.51589690073205152</c:v>
+                  <c:v>0.25448522798943846</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.5006498430869375</c:v>
+                  <c:v>0.24696405285642434</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.48585340409547995</c:v>
+                  <c:v>0.23966516204155472</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>0.2325819860504062</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0</c:v>
+                  <c:v>0.22346231593430321</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0</c:v>
+                  <c:v>0.21470023319819845</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0</c:v>
+                  <c:v>0.20628171664037007</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0</c:v>
+                  <c:v>0.1981932948382796</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0</c:v>
+                  <c:v>0.19042202459142168</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0</c:v>
+                  <c:v>0.18295547020944194</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0</c:v>
+                  <c:v>0.17578168361237931</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0</c:v>
+                  <c:v>0.16888918521118904</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0</c:v>
+                  <c:v>0.16226694553795112</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0</c:v>
+                  <c:v>0.15590436759636864</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2001,7 +1993,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>5.951694157529863E-312</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -4008,84 +4000,84 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C3" cm="1">
         <f t="array" ref="C3">_xll.TMX_FREQUENCY_ANNUALLY()</f>
         <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="E3" s="5" cm="1">
         <f t="array" ref="E3">_xll.TMX_DAY_COUNT_30_360()</f>
-        <v>140716368016338</v>
+        <v>140716946699303</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4" cm="1">
         <f t="array" ref="C4">_xll.TMX_FREQUENCY_SEMIANNUALLY()</f>
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E4" s="5" cm="1">
         <f t="array" ref="E4">_xll.TMX_DAY_COUNT_ACTUAL_360()</f>
-        <v>140716368009178</v>
+        <v>140716946692093</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C5" cm="1">
         <f t="array" ref="C5">_xll.TMX_FREQUENCY_QUARTERLY()</f>
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E5" s="5" cm="1">
         <f t="array" ref="E5">_xll.TMX_DAY_COUNT_ACTUAL_365()</f>
-        <v>140716368014703</v>
+        <v>140716946697698</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C6" cm="1">
         <f t="array" ref="C6">_xll.TMX_FREQUENCY_MONTHLY()</f>
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E6" s="5" cm="1">
         <f t="array" ref="E6">_xll.TMX_DAY_COUNT_ACTUAL_ACTUAL()</f>
-        <v>140716368019948</v>
+        <v>140716946702828</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E7" s="5" cm="1">
         <f t="array" ref="E7">_xll.TMX_DAY_COUNT_YEARS()</f>
-        <v>140716368051158</v>
+        <v>140716946733953</v>
       </c>
     </row>
   </sheetData>
@@ -4107,38 +4099,38 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C2" s="9">
         <f ca="1">50 + 100*RAND()</f>
-        <v>70.939913996476818</v>
+        <v>143.54256009219088</v>
       </c>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C3" s="9">
         <f ca="1">0.01 + 0.3*RAND()</f>
-        <v>0.20041430016721062</v>
+        <v>0.14724310424841439</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C4" s="9">
         <f ca="1">50 + 100*RAND()</f>
-        <v>83.06208725632095</v>
+        <v>103.83770923644002</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C5" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">_xll.TMX.BLACK.MONEYNESS(f, s, k)</f>
-        <v>0.88735223031421984</v>
+        <v>-2.1254789537184884</v>
       </c>
       <c r="D5">
         <v>1E-3</v>
@@ -4154,66 +4146,66 @@
       </c>
       <c r="C6" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">_xll.TMX.BLACK.PUT.VALUE(f, s, k)</f>
-        <v>14.008170277852862</v>
+        <v>8.7883691274255105E-2</v>
       </c>
       <c r="D6" cm="1">
         <f t="array" aca="1" ref="D6" ca="1">_xll.TMX.BLACK.PUT.VALUE(f + D5, s, k)</f>
-        <v>14.007416349856022</v>
+        <v>8.787217052021834E-2</v>
       </c>
       <c r="E6" cm="1">
         <f t="array" aca="1" ref="E6" ca="1">_xll.TMX.BLACK.PUT.VALUE(f + E5, s, k)</f>
-        <v>14.008924228012383</v>
+        <v>8.7895213454794785E-2</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="10" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C7" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">_xll.TMX.BLACK.PUT.DELTA(f, s, k)</f>
-        <v>-0.75393907829029194</v>
+        <v>-1.1521467267824437E-2</v>
       </c>
       <c r="D7">
         <f ca="1">(D6-E6)/(D5-E5)</f>
-        <v>-0.7539390781801103</v>
+        <v>-1.1521467288222453E-2</v>
       </c>
       <c r="E7">
         <f ca="1">(C7-D7)/C7</f>
-        <v>1.461413060563573E-10</v>
+        <v>-1.7704356689100097E-9</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C8" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_xll.TMX.BLACK.GAMMA(f, s, k)</f>
-        <v>2.2162689083151634E-2</v>
+        <v>1.4264982714608458E-3</v>
       </c>
       <c r="D8">
         <f ca="1">(D6-2*C6+E6)/(D5^2)</f>
-        <v>2.2162680579640437E-2</v>
+        <v>1.4265029157911613E-3</v>
       </c>
       <c r="E8">
         <f t="shared" ref="E8:E9" ca="1" si="0">(C8-D8)/C8</f>
-        <v>3.8368589503592664E-7</v>
+        <v>-3.2557560064581962E-6</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C9" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">_xll.TMX.BLACK.VEGA(f, s, k)</f>
-        <v>22.35282796350889</v>
+        <v>4.3278040590029576</v>
       </c>
       <c r="D9" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">(_xll.TMX.BLACK.PUT.VALUE(f, s + D5, k) - _xll.TMX.BLACK.PUT.VALUE(f, s + E5, k))/(D5 - E5)</f>
-        <v>22.352689086613253</v>
+        <v>4.3280975397321786</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>6.2129452194352632E-6</v>
+        <v>-6.7812850401685303E-5</v>
       </c>
     </row>
   </sheetData>
@@ -4246,7 +4238,7 @@
       </c>
       <c r="C2" s="8">
         <f ca="1">TODAY()</f>
-        <v>45094</v>
+        <v>45102</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.3">
@@ -4255,7 +4247,7 @@
       </c>
       <c r="C3" s="9">
         <f ca="1">10*RAND()</f>
-        <v>8.6147521318205058</v>
+        <v>5.2546234533343394</v>
       </c>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4264,18 +4256,18 @@
       </c>
       <c r="C4" s="2" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">_xll.TMX.DATE.ADD_YEARS(date,years)</f>
-        <v>48240.473599537036</v>
+        <v>47021.211805555555</v>
       </c>
       <c r="D4">
         <f ca="1">C4</f>
-        <v>48240.473599537036</v>
+        <v>47021.211805555555</v>
       </c>
     </row>
     <row r="5" spans="2:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="2" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">_xll.TMX.DATE.ADD_YEARS(C4,-years)</f>
-        <v>45094</v>
+        <v>45102</v>
       </c>
       <c r="D5" s="7">
         <f ca="1">C5-date</f>
@@ -4288,18 +4280,18 @@
       </c>
       <c r="C6" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">_xll.TMX.DATE.SUB_YEARS(C4,date)</f>
-        <v>8.6134554439858455</v>
+        <v>5.2540435464109461</v>
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="2" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">_xll.TMX.DATE.ADD_YEARS(date,C6)</f>
-        <v>48240</v>
+        <v>47021</v>
       </c>
       <c r="D7">
         <f ca="1">C7</f>
-        <v>48240</v>
+        <v>47021</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4344,7 +4336,7 @@
       </c>
       <c r="C11" s="2" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">_xll.TMX.DATE.ADD_YMD(date, years_,months, days)</f>
-        <v>45524</v>
+        <v>45532</v>
       </c>
     </row>
   </sheetData>
@@ -4360,8 +4352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B429FC-4136-41AD-B308-B590D229D902}">
   <dimension ref="B2:N43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -4386,13 +4378,13 @@
       </c>
       <c r="I2" s="5" cm="1">
         <f t="array" aca="1" ref="I2" ca="1">_xll.\TMX.PWFLAT.CURVE(time, rate, extrapolate)</f>
-        <v>2982856661520</v>
+        <v>1204148810288</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>20</v>
@@ -4407,37 +4399,32 @@
       </c>
       <c r="C3" s="15">
         <f ca="1">RAND()</f>
-        <v>0.25184833824705466</v>
+        <v>0.95851248793963784</v>
       </c>
       <c r="E3" cm="1">
-        <f t="array" aca="1" ref="E3:F6" ca="1">TRANSPOSE(_xll.TMX.PWFLAT.CURVE(curve_))</f>
+        <f t="array" aca="1" ref="E3:F6" ca="1">TRANSPOSE(_xll.TMX.PWFLAT.CURVE(curve))</f>
         <v>1</v>
       </c>
       <c r="F3" s="16">
         <f ca="1"/>
-        <v>0.25184833824705466</v>
+        <v>0.95851248793963784</v>
       </c>
       <c r="G3" s="16"/>
-      <c r="H3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
+      <c r="H3" s="3"/>
       <c r="K3" cm="1">
         <f t="array" ref="K3:K43">_xlfn.SEQUENCE(1+4/0.1,1,0,0.1)</f>
         <v>0</v>
       </c>
       <c r="L3" cm="1">
-        <f t="array" aca="1" ref="L3" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K3)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="L3" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K3)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="M3" cm="1">
-        <f t="array" aca="1" ref="M3" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K3)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="M3" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K3)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="N3" cm="1">
-        <f t="array" aca="1" ref="N3" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K3)</f>
+        <f t="array" aca="1" ref="N3" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K3)</f>
         <v>1</v>
       </c>
     </row>
@@ -4456,24 +4443,21 @@
         <f ca="1"/>
         <v>0.2</v>
       </c>
-      <c r="I4" s="5" cm="1">
-        <f t="array" aca="1" ref="I4" ca="1">_xll.\TMX.PWFLAT.CURVE.SHIFT(curve, shift)</f>
-        <v>2982856666272</v>
-      </c>
+      <c r="I4" s="5"/>
       <c r="K4">
         <v>0.1</v>
       </c>
       <c r="L4" cm="1">
-        <f t="array" aca="1" ref="L4" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K4)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="L4" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K4)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="M4" cm="1">
-        <f t="array" aca="1" ref="M4" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K4)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="M4" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K4)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="N4" cm="1">
-        <f t="array" aca="1" ref="N4" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K4)</f>
-        <v>0.97512965842601385</v>
+        <f t="array" aca="1" ref="N4" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K4)</f>
+        <v>0.90859916123799112</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.3">
@@ -4491,26 +4475,21 @@
         <f ca="1"/>
         <v>0.3</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
+      <c r="H5" s="3"/>
       <c r="K5">
         <v>0.2</v>
       </c>
       <c r="L5" cm="1">
-        <f t="array" aca="1" ref="L5" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K5)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="L5" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K5)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="M5" cm="1">
-        <f t="array" aca="1" ref="M5" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K5)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="M5" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K5)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="N5" cm="1">
-        <f t="array" aca="1" ref="N5" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K5)</f>
-        <v>0.95087785074203446</v>
+        <f t="array" aca="1" ref="N5" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K5)</f>
+        <v>0.82555243580238102</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
@@ -4524,31 +4503,26 @@
         <f ca="1"/>
         <v>3</v>
       </c>
-      <c r="F6" t="e">
-        <f ca="1"/>
-        <v>#NUM!</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I6" s="5" cm="1">
-        <f t="array" aca="1" ref="I6" ca="1">_xll.\TMX.PWFLAT.CURVE.TRANSLATE(I4, translate)</f>
-        <v>2982856670144</v>
-      </c>
+      <c r="F6">
+        <f ca="1"/>
+        <v>0.4</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="5"/>
       <c r="K6">
         <v>0.30000000000000004</v>
       </c>
       <c r="L6" cm="1">
-        <f t="array" aca="1" ref="L6" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K6)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="L6" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K6)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="M6" cm="1">
-        <f t="array" aca="1" ref="M6" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K6)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="M6" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K6)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="N6" cm="1">
-        <f t="array" aca="1" ref="N6" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K6)</f>
-        <v>0.92722919379894231</v>
+        <f t="array" aca="1" ref="N6" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K6)</f>
+        <v>0.75009625072802388</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -4556,16 +4530,16 @@
         <v>0.4</v>
       </c>
       <c r="L7" cm="1">
-        <f t="array" aca="1" ref="L7" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K7)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="L7" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K7)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="M7" cm="1">
-        <f t="array" aca="1" ref="M7" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K7)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="M7" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K7)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="N7" cm="1">
-        <f t="array" aca="1" ref="N7" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K7)</f>
-        <v>0.90416868703179076</v>
+        <f t="array" aca="1" ref="N7" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K7)</f>
+        <v>0.68153682425924444</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
@@ -4573,16 +4547,16 @@
         <v>0.5</v>
       </c>
       <c r="L8" cm="1">
-        <f t="array" aca="1" ref="L8" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K8)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="L8" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K8)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="M8" cm="1">
-        <f t="array" aca="1" ref="M8" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K8)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="M8" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K8)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="N8" cm="1">
-        <f t="array" aca="1" ref="N8" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K8)</f>
-        <v>0.88168170294480752</v>
+        <f t="array" aca="1" ref="N8" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K8)</f>
+        <v>0.61924378687475368</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
@@ -4590,16 +4564,16 @@
         <v>0.6</v>
       </c>
       <c r="L9" cm="1">
-        <f t="array" aca="1" ref="L9" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K9)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="L9" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K9)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="M9" cm="1">
-        <f t="array" aca="1" ref="M9" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K9)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="M9" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K9)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="N9" cm="1">
-        <f t="array" aca="1" ref="N9" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K9)</f>
-        <v>0.85975397783303642</v>
+        <f t="array" aca="1" ref="N9" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K9)</f>
+        <v>0.56264438535623851</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
@@ -4607,16 +4581,16 @@
         <v>0.7</v>
       </c>
       <c r="L10" cm="1">
-        <f t="array" aca="1" ref="L10" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K10)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="L10" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K10)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="M10" cm="1">
-        <f t="array" aca="1" ref="M10" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K10)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="M10" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K10)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="N10" cm="1">
-        <f t="array" aca="1" ref="N10" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K10)</f>
-        <v>0.83837160273473554</v>
+        <f t="array" aca="1" ref="N10" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K10)</f>
+        <v>0.51121821660994338</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -4624,16 +4598,16 @@
         <v>0.79999999999999993</v>
       </c>
       <c r="L11" cm="1">
-        <f t="array" aca="1" ref="L11" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K11)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="L11" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K11)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="M11" cm="1">
-        <f t="array" aca="1" ref="M11" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K11)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="M11" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K11)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="N11" cm="1">
-        <f t="array" aca="1" ref="N11" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K11)</f>
-        <v>0.81752101460879245</v>
+        <f t="array" aca="1" ref="N11" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K11)</f>
+        <v>0.46449244282137631</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -4641,16 +4615,16 @@
         <v>0.89999999999999991</v>
       </c>
       <c r="L12" cm="1">
-        <f t="array" aca="1" ref="L12" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K12)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="L12" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K12)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="M12" cm="1">
-        <f t="array" aca="1" ref="M12" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K12)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="M12" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K12)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="N12" cm="1">
-        <f t="array" aca="1" ref="N12" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K12)</f>
-        <v>0.79718898773156011</v>
+        <f t="array" aca="1" ref="N12" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K12)</f>
+        <v>0.42203744394888804</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -4658,16 +4632,16 @@
         <v>0.99999999999999989</v>
       </c>
       <c r="L13" cm="1">
-        <f t="array" aca="1" ref="L13" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K13)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="L13" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K13)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="M13" cm="1">
-        <f t="array" aca="1" ref="M13" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K13)</f>
-        <v>0.25184833824705466</v>
+        <f t="array" aca="1" ref="M13" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K13)</f>
+        <v>0.95851248793963784</v>
       </c>
       <c r="N13" cm="1">
-        <f t="array" aca="1" ref="N13" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K13)</f>
-        <v>0.77736262530765599</v>
+        <f t="array" aca="1" ref="N13" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K13)</f>
+        <v>0.38346286758298537</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.3">
@@ -4675,16 +4649,16 @@
         <v>1.0999999999999999</v>
       </c>
       <c r="L14" cm="1">
-        <f t="array" aca="1" ref="L14" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K14)</f>
+        <f t="array" aca="1" ref="L14" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K14)</f>
         <v>0.2</v>
       </c>
       <c r="M14" cm="1">
-        <f t="array" aca="1" ref="M14" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K14)</f>
-        <v>0.24713485295186788</v>
+        <f t="array" aca="1" ref="M14" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K14)</f>
+        <v>0.2</v>
       </c>
       <c r="N14" cm="1">
-        <f t="array" aca="1" ref="N14" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K14)</f>
-        <v>0.76196981400482067</v>
+        <f t="array" aca="1" ref="N14" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K14)</f>
+        <v>0.37586979406724619</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -4692,16 +4666,16 @@
         <v>1.2</v>
       </c>
       <c r="L15" cm="1">
-        <f t="array" aca="1" ref="L15" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K15)</f>
+        <f t="array" aca="1" ref="L15" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K15)</f>
         <v>0.2</v>
       </c>
       <c r="M15" cm="1">
-        <f t="array" aca="1" ref="M15" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K15)</f>
-        <v>0.24320694853921221</v>
+        <f t="array" aca="1" ref="M15" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K15)</f>
+        <v>0.2</v>
       </c>
       <c r="N15" cm="1">
-        <f t="array" aca="1" ref="N15" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K15)</f>
-        <v>0.74688180078732025</v>
+        <f t="array" aca="1" ref="N15" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K15)</f>
+        <v>0.36842707348079806</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.3">
@@ -4709,16 +4683,16 @@
         <v>1.3</v>
       </c>
       <c r="L16" cm="1">
-        <f t="array" aca="1" ref="L16" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K16)</f>
+        <f t="array" aca="1" ref="L16" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K16)</f>
         <v>0.2</v>
       </c>
       <c r="M16" cm="1">
-        <f t="array" aca="1" ref="M16" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K16)</f>
-        <v>0.23988333711311896</v>
+        <f t="array" aca="1" ref="M16" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K16)</f>
+        <v>0.2</v>
       </c>
       <c r="N16" cm="1">
-        <f t="array" aca="1" ref="N16" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K16)</f>
-        <v>0.73209255024869169</v>
+        <f t="array" aca="1" ref="N16" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K16)</f>
+        <v>0.36113172863616871</v>
       </c>
     </row>
     <row r="17" spans="11:14" x14ac:dyDescent="0.3">
@@ -4726,16 +4700,16 @@
         <v>1.4000000000000001</v>
       </c>
       <c r="L17" cm="1">
-        <f t="array" aca="1" ref="L17" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K17)</f>
+        <f t="array" aca="1" ref="L17" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K17)</f>
         <v>0.2</v>
       </c>
       <c r="M17" cm="1">
-        <f t="array" aca="1" ref="M17" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K17)</f>
-        <v>0.23703452731932476</v>
+        <f t="array" aca="1" ref="M17" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K17)</f>
+        <v>0.2</v>
       </c>
       <c r="N17" cm="1">
-        <f t="array" aca="1" ref="N17" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K17)</f>
-        <v>0.71759614649152659</v>
+        <f t="array" aca="1" ref="N17" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K17)</f>
+        <v>0.35398084129814772</v>
       </c>
     </row>
     <row r="18" spans="11:14" x14ac:dyDescent="0.3">
@@ -4743,16 +4717,16 @@
         <v>1.5000000000000002</v>
       </c>
       <c r="L18" cm="1">
-        <f t="array" aca="1" ref="L18" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K18)</f>
+        <f t="array" aca="1" ref="L18" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K18)</f>
         <v>0.2</v>
       </c>
       <c r="M18" cm="1">
-        <f t="array" aca="1" ref="M18" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K18)</f>
-        <v>0.23456555883136976</v>
+        <f t="array" aca="1" ref="M18" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K18)</f>
+        <v>0.2</v>
       </c>
       <c r="N18" cm="1">
-        <f t="array" aca="1" ref="N18" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K18)</f>
-        <v>0.70338679076103439</v>
+        <f t="array" aca="1" ref="N18" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K18)</f>
+        <v>0.34697155101645349</v>
       </c>
     </row>
     <row r="19" spans="11:14" x14ac:dyDescent="0.3">
@@ -4760,16 +4734,16 @@
         <v>1.6000000000000003</v>
       </c>
       <c r="L19" cm="1">
-        <f t="array" aca="1" ref="L19" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K19)</f>
+        <f t="array" aca="1" ref="L19" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K19)</f>
         <v>0.2</v>
       </c>
       <c r="M19" cm="1">
-        <f t="array" aca="1" ref="M19" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K19)</f>
-        <v>0.23240521140440915</v>
+        <f t="array" aca="1" ref="M19" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K19)</f>
+        <v>0.2</v>
       </c>
       <c r="N19" cm="1">
-        <f t="array" aca="1" ref="N19" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K19)</f>
-        <v>0.68945879912546226</v>
+        <f t="array" aca="1" ref="N19" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K19)</f>
+        <v>0.34010105398151486</v>
       </c>
     </row>
     <row r="20" spans="11:14" x14ac:dyDescent="0.3">
@@ -4777,16 +4751,16 @@
         <v>1.7000000000000004</v>
       </c>
       <c r="L20" cm="1">
-        <f t="array" aca="1" ref="L20" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K20)</f>
+        <f t="array" aca="1" ref="L20" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K20)</f>
         <v>0.2</v>
       </c>
       <c r="M20" cm="1">
-        <f t="array" aca="1" ref="M20" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K20)</f>
-        <v>0.23049902249826745</v>
+        <f t="array" aca="1" ref="M20" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K20)</f>
+        <v>0.2</v>
       </c>
       <c r="N20" cm="1">
-        <f t="array" aca="1" ref="N20" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K20)</f>
-        <v>0.67580660020244676</v>
+        <f t="array" aca="1" ref="N20" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K20)</f>
+        <v>0.33336660190291001</v>
       </c>
     </row>
     <row r="21" spans="11:14" x14ac:dyDescent="0.3">
@@ -4794,16 +4768,16 @@
         <v>1.8000000000000005</v>
       </c>
       <c r="L21" cm="1">
-        <f t="array" aca="1" ref="L21" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K21)</f>
+        <f t="array" aca="1" ref="L21" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K21)</f>
         <v>0.2</v>
       </c>
       <c r="M21" cm="1">
-        <f t="array" aca="1" ref="M21" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K21)</f>
-        <v>0.22880463235947482</v>
+        <f t="array" aca="1" ref="M21" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K21)</f>
+        <v>0.2</v>
       </c>
       <c r="N21" cm="1">
-        <f t="array" aca="1" ref="N21" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K21)</f>
-        <v>0.66242473293038706</v>
+        <f t="array" aca="1" ref="N21" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K21)</f>
+        <v>0.32676550091001366</v>
       </c>
     </row>
     <row r="22" spans="11:14" x14ac:dyDescent="0.3">
@@ -4811,16 +4785,16 @@
         <v>1.9000000000000006</v>
       </c>
       <c r="L22" cm="1">
-        <f t="array" aca="1" ref="L22" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K22)</f>
+        <f t="array" aca="1" ref="L22" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K22)</f>
         <v>0.2</v>
       </c>
       <c r="M22" cm="1">
-        <f t="array" aca="1" ref="M22" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K22)</f>
-        <v>0.22728859907739721</v>
+        <f t="array" aca="1" ref="M22" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K22)</f>
+        <v>0.2</v>
       </c>
       <c r="N22" cm="1">
-        <f t="array" aca="1" ref="N22" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K22)</f>
-        <v>0.64930784438394706</v>
+        <f t="array" aca="1" ref="N22" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K22)</f>
+        <v>0.32029511047441273</v>
       </c>
     </row>
     <row r="23" spans="11:14" x14ac:dyDescent="0.3">
@@ -4828,16 +4802,16 @@
         <v>2.0000000000000004</v>
       </c>
       <c r="L23" cm="1">
-        <f t="array" aca="1" ref="L23" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K23)</f>
+        <f t="array" aca="1" ref="L23" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K23)</f>
         <v>0.3</v>
       </c>
       <c r="M23" cm="1">
-        <f t="array" aca="1" ref="M23" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K23)</f>
-        <v>0.22592416912352734</v>
+        <f t="array" aca="1" ref="M23" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K23)</f>
+        <v>0.3</v>
       </c>
       <c r="N23" cm="1">
-        <f t="array" aca="1" ref="N23" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K23)</f>
-        <v>0.63645068763281409</v>
+        <f t="array" aca="1" ref="N23" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K23)</f>
+        <v>0.31395284235366</v>
       </c>
     </row>
     <row r="24" spans="11:14" x14ac:dyDescent="0.3">
@@ -4845,16 +4819,16 @@
         <v>2.1000000000000005</v>
       </c>
       <c r="L24" cm="1">
-        <f t="array" aca="1" ref="L24" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K24)</f>
+        <f t="array" aca="1" ref="L24" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K24)</f>
         <v>0.3</v>
       </c>
       <c r="M24" cm="1">
-        <f t="array" aca="1" ref="M24" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K24)</f>
-        <v>0.22945158964145462</v>
+        <f t="array" aca="1" ref="M24" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K24)</f>
+        <v>0.3</v>
       </c>
       <c r="N24" cm="1">
-        <f t="array" aca="1" ref="N24" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K24)</f>
-        <v>0.61764072713714113</v>
+        <f t="array" aca="1" ref="N24" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K24)</f>
+        <v>0.30467413360696821</v>
       </c>
     </row>
     <row r="25" spans="11:14" x14ac:dyDescent="0.3">
@@ -4862,16 +4836,16 @@
         <v>2.2000000000000006</v>
       </c>
       <c r="L25" cm="1">
-        <f t="array" aca="1" ref="L25" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K25)</f>
+        <f t="array" aca="1" ref="L25" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K25)</f>
         <v>0.3</v>
       </c>
       <c r="M25" cm="1">
-        <f t="array" aca="1" ref="M25" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K25)</f>
-        <v>0.23265833556684307</v>
+        <f t="array" aca="1" ref="M25" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K25)</f>
+        <v>0.3</v>
       </c>
       <c r="N25" cm="1">
-        <f t="array" aca="1" ref="N25" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K25)</f>
-        <v>0.59938668498789149</v>
+        <f t="array" aca="1" ref="N25" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K25)</f>
+        <v>0.29566965214664376</v>
       </c>
     </row>
     <row r="26" spans="11:14" x14ac:dyDescent="0.3">
@@ -4879,16 +4853,16 @@
         <v>2.3000000000000007</v>
       </c>
       <c r="L26" cm="1">
-        <f t="array" aca="1" ref="L26" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K26)</f>
+        <f t="array" aca="1" ref="L26" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K26)</f>
         <v>0.3</v>
       </c>
       <c r="M26" cm="1">
-        <f t="array" aca="1" ref="M26" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K26)</f>
-        <v>0.23558623402045858</v>
+        <f t="array" aca="1" ref="M26" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K26)</f>
+        <v>0.3</v>
       </c>
       <c r="N26" cm="1">
-        <f t="array" aca="1" ref="N26" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K26)</f>
-        <v>0.58167213131494588</v>
+        <f t="array" aca="1" ref="N26" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K26)</f>
+        <v>0.28693129333155148</v>
       </c>
     </row>
     <row r="27" spans="11:14" x14ac:dyDescent="0.3">
@@ -4896,16 +4870,16 @@
         <v>2.4000000000000008</v>
       </c>
       <c r="L27" cm="1">
-        <f t="array" aca="1" ref="L27" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K27)</f>
+        <f t="array" aca="1" ref="L27" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K27)</f>
         <v>0.3</v>
       </c>
       <c r="M27" cm="1">
-        <f t="array" aca="1" ref="M27" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K27)</f>
-        <v>0.2382701409362728</v>
+        <f t="array" aca="1" ref="M27" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K27)</f>
+        <v>0.3</v>
       </c>
       <c r="N27" cm="1">
-        <f t="array" aca="1" ref="N27" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K27)</f>
-        <v>0.5644811218242306</v>
+        <f t="array" aca="1" ref="N27" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K27)</f>
+        <v>0.27845119204890095</v>
       </c>
     </row>
     <row r="28" spans="11:14" x14ac:dyDescent="0.3">
@@ -4913,16 +4887,16 @@
         <v>2.5000000000000009</v>
       </c>
       <c r="L28" cm="1">
-        <f t="array" aca="1" ref="L28" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K28)</f>
+        <f t="array" aca="1" ref="L28" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K28)</f>
         <v>0.3</v>
       </c>
       <c r="M28" cm="1">
-        <f t="array" aca="1" ref="M28" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K28)</f>
-        <v>0.24073933529882191</v>
+        <f t="array" aca="1" ref="M28" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K28)</f>
+        <v>0.3</v>
       </c>
       <c r="N28" cm="1">
-        <f t="array" aca="1" ref="N28" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K28)</f>
-        <v>0.54779818344677589</v>
+        <f t="array" aca="1" ref="N28" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K28)</f>
+        <v>0.27022171563511382</v>
       </c>
     </row>
     <row r="29" spans="11:14" x14ac:dyDescent="0.3">
@@ -4930,16 +4904,16 @@
         <v>2.600000000000001</v>
       </c>
       <c r="L29" cm="1">
-        <f t="array" aca="1" ref="L29" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K29)</f>
+        <f t="array" aca="1" ref="L29" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K29)</f>
         <v>0.3</v>
       </c>
       <c r="M29" cm="1">
-        <f t="array" aca="1" ref="M29" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K29)</f>
-        <v>0.24301859163348261</v>
+        <f t="array" aca="1" ref="M29" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K29)</f>
+        <v>0.3</v>
       </c>
       <c r="N29" cm="1">
-        <f t="array" aca="1" ref="N29" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K29)</f>
-        <v>0.53160830041190998</v>
+        <f t="array" aca="1" ref="N29" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K29)</f>
+        <v>0.26223545700591128</v>
       </c>
     </row>
     <row r="30" spans="11:14" x14ac:dyDescent="0.3">
@@ -4947,16 +4921,16 @@
         <v>2.7000000000000011</v>
       </c>
       <c r="L30" cm="1">
-        <f t="array" aca="1" ref="L30" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K30)</f>
+        <f t="array" aca="1" ref="L30" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K30)</f>
         <v>0.3</v>
       </c>
       <c r="M30" cm="1">
-        <f t="array" aca="1" ref="M30" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K30)</f>
-        <v>0.24512901416557584</v>
+        <f t="array" aca="1" ref="M30" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K30)</f>
+        <v>0.3</v>
       </c>
       <c r="N30" cm="1">
-        <f t="array" aca="1" ref="N30" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K30)</f>
-        <v>0.51589690073205152</v>
+        <f t="array" aca="1" ref="N30" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K30)</f>
+        <v>0.25448522798943846</v>
       </c>
     </row>
     <row r="31" spans="11:14" x14ac:dyDescent="0.3">
@@ -4964,16 +4938,16 @@
         <v>2.8000000000000012</v>
       </c>
       <c r="L31" cm="1">
-        <f t="array" aca="1" ref="L31" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K31)</f>
+        <f t="array" aca="1" ref="L31" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K31)</f>
         <v>0.3</v>
       </c>
       <c r="M31" cm="1">
-        <f t="array" aca="1" ref="M31" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K31)</f>
-        <v>0.24708869223109098</v>
+        <f t="array" aca="1" ref="M31" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K31)</f>
+        <v>0.3</v>
       </c>
       <c r="N31" cm="1">
-        <f t="array" aca="1" ref="N31" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K31)</f>
-        <v>0.5006498430869375</v>
+        <f t="array" aca="1" ref="N31" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K31)</f>
+        <v>0.24696405285642434</v>
       </c>
     </row>
     <row r="32" spans="11:14" x14ac:dyDescent="0.3">
@@ -4981,203 +4955,203 @@
         <v>2.9000000000000012</v>
       </c>
       <c r="L32" cm="1">
-        <f t="array" aca="1" ref="L32" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K32)</f>
+        <f t="array" aca="1" ref="L32" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K32)</f>
         <v>0.3</v>
       </c>
       <c r="M32" cm="1">
-        <f t="array" aca="1" ref="M32" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K32)</f>
-        <v>0.24891322008519129</v>
+        <f t="array" aca="1" ref="M32" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K32)</f>
+        <v>0.3</v>
       </c>
       <c r="N32" cm="1">
-        <f t="array" aca="1" ref="N32" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K32)</f>
-        <v>0.48585340409547995</v>
+        <f t="array" aca="1" ref="N32" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K32)</f>
+        <v>0.23966516204155472</v>
       </c>
     </row>
     <row r="33" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K33">
         <v>3.0000000000000013</v>
       </c>
-      <c r="L33" t="e" cm="1">
-        <f t="array" aca="1" ref="L33" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K33)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M33" t="e" cm="1">
-        <f t="array" aca="1" ref="M33" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K33)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N33" t="e" cm="1">
-        <f t="array" aca="1" ref="N33" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K33)</f>
-        <v>#NUM!</v>
+      <c r="L33" cm="1">
+        <f t="array" aca="1" ref="L33" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K33)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M33" cm="1">
+        <f t="array" aca="1" ref="M33" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K33)</f>
+        <v>0.4</v>
+      </c>
+      <c r="N33" cm="1">
+        <f t="array" aca="1" ref="N33" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K33)</f>
+        <v>0.2325819860504062</v>
       </c>
     </row>
     <row r="34" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K34">
         <v>3.1000000000000014</v>
       </c>
-      <c r="L34" t="e" cm="1">
-        <f t="array" aca="1" ref="L34" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K34)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M34" t="e" cm="1">
-        <f t="array" aca="1" ref="M34" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K34)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N34" t="e" cm="1">
-        <f t="array" aca="1" ref="N34" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K34)</f>
-        <v>#NUM!</v>
+      <c r="L34" cm="1">
+        <f t="array" aca="1" ref="L34" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K34)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M34" cm="1">
+        <f t="array" aca="1" ref="M34" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K34)</f>
+        <v>0.4</v>
+      </c>
+      <c r="N34" cm="1">
+        <f t="array" aca="1" ref="N34" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K34)</f>
+        <v>0.22346231593430321</v>
       </c>
     </row>
     <row r="35" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K35">
         <v>3.2000000000000015</v>
       </c>
-      <c r="L35" t="e" cm="1">
-        <f t="array" aca="1" ref="L35" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K35)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M35" t="e" cm="1">
-        <f t="array" aca="1" ref="M35" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K35)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N35" t="e" cm="1">
-        <f t="array" aca="1" ref="N35" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K35)</f>
-        <v>#NUM!</v>
+      <c r="L35" cm="1">
+        <f t="array" aca="1" ref="L35" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K35)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M35" cm="1">
+        <f t="array" aca="1" ref="M35" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K35)</f>
+        <v>0.4</v>
+      </c>
+      <c r="N35" cm="1">
+        <f t="array" aca="1" ref="N35" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K35)</f>
+        <v>0.21470023319819845</v>
       </c>
     </row>
     <row r="36" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K36">
         <v>3.3000000000000016</v>
       </c>
-      <c r="L36" t="e" cm="1">
-        <f t="array" aca="1" ref="L36" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K36)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M36" t="e" cm="1">
-        <f t="array" aca="1" ref="M36" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K36)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N36" t="e" cm="1">
-        <f t="array" aca="1" ref="N36" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K36)</f>
-        <v>#NUM!</v>
+      <c r="L36" cm="1">
+        <f t="array" aca="1" ref="L36" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K36)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M36" cm="1">
+        <f t="array" aca="1" ref="M36" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K36)</f>
+        <v>0.4</v>
+      </c>
+      <c r="N36" cm="1">
+        <f t="array" aca="1" ref="N36" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K36)</f>
+        <v>0.20628171664037007</v>
       </c>
     </row>
     <row r="37" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K37">
         <v>3.4000000000000017</v>
       </c>
-      <c r="L37" t="e" cm="1">
-        <f t="array" aca="1" ref="L37" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K37)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M37" t="e" cm="1">
-        <f t="array" aca="1" ref="M37" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K37)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N37" t="e" cm="1">
-        <f t="array" aca="1" ref="N37" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K37)</f>
-        <v>#NUM!</v>
+      <c r="L37" cm="1">
+        <f t="array" aca="1" ref="L37" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K37)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M37" cm="1">
+        <f t="array" aca="1" ref="M37" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K37)</f>
+        <v>0.4</v>
+      </c>
+      <c r="N37" cm="1">
+        <f t="array" aca="1" ref="N37" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K37)</f>
+        <v>0.1981932948382796</v>
       </c>
     </row>
     <row r="38" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K38">
         <v>3.5000000000000018</v>
       </c>
-      <c r="L38" t="e" cm="1">
-        <f t="array" aca="1" ref="L38" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K38)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M38" t="e" cm="1">
-        <f t="array" aca="1" ref="M38" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K38)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N38" t="e" cm="1">
-        <f t="array" aca="1" ref="N38" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K38)</f>
-        <v>#NUM!</v>
+      <c r="L38" cm="1">
+        <f t="array" aca="1" ref="L38" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K38)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M38" cm="1">
+        <f t="array" aca="1" ref="M38" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K38)</f>
+        <v>0.4</v>
+      </c>
+      <c r="N38" cm="1">
+        <f t="array" aca="1" ref="N38" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K38)</f>
+        <v>0.19042202459142168</v>
       </c>
     </row>
     <row r="39" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K39">
         <v>3.6000000000000019</v>
       </c>
-      <c r="L39" t="e" cm="1">
-        <f t="array" aca="1" ref="L39" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K39)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M39" t="e" cm="1">
-        <f t="array" aca="1" ref="M39" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K39)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N39" t="e" cm="1">
-        <f t="array" aca="1" ref="N39" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K39)</f>
-        <v>#NUM!</v>
+      <c r="L39" cm="1">
+        <f t="array" aca="1" ref="L39" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K39)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M39" cm="1">
+        <f t="array" aca="1" ref="M39" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K39)</f>
+        <v>0.4</v>
+      </c>
+      <c r="N39" cm="1">
+        <f t="array" aca="1" ref="N39" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K39)</f>
+        <v>0.18295547020944194</v>
       </c>
     </row>
     <row r="40" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K40">
         <v>3.700000000000002</v>
       </c>
-      <c r="L40" t="e" cm="1">
-        <f t="array" aca="1" ref="L40" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K40)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M40" t="e" cm="1">
-        <f t="array" aca="1" ref="M40" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K40)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N40" t="e" cm="1">
-        <f t="array" aca="1" ref="N40" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K40)</f>
-        <v>#NUM!</v>
+      <c r="L40" cm="1">
+        <f t="array" aca="1" ref="L40" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K40)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M40" cm="1">
+        <f t="array" aca="1" ref="M40" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K40)</f>
+        <v>0.4</v>
+      </c>
+      <c r="N40" cm="1">
+        <f t="array" aca="1" ref="N40" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K40)</f>
+        <v>0.17578168361237931</v>
       </c>
     </row>
     <row r="41" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K41">
         <v>3.800000000000002</v>
       </c>
-      <c r="L41" t="e" cm="1">
-        <f t="array" aca="1" ref="L41" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K41)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M41" t="e" cm="1">
-        <f t="array" aca="1" ref="M41" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K41)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N41" t="e" cm="1">
-        <f t="array" aca="1" ref="N41" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K41)</f>
-        <v>#NUM!</v>
+      <c r="L41" cm="1">
+        <f t="array" aca="1" ref="L41" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K41)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M41" cm="1">
+        <f t="array" aca="1" ref="M41" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K41)</f>
+        <v>0.4</v>
+      </c>
+      <c r="N41" cm="1">
+        <f t="array" aca="1" ref="N41" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K41)</f>
+        <v>0.16888918521118904</v>
       </c>
     </row>
     <row r="42" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K42">
         <v>3.9000000000000021</v>
       </c>
-      <c r="L42" t="e" cm="1">
-        <f t="array" aca="1" ref="L42" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K42)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M42" t="e" cm="1">
-        <f t="array" aca="1" ref="M42" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K42)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N42" t="e" cm="1">
-        <f t="array" aca="1" ref="N42" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K42)</f>
-        <v>#NUM!</v>
+      <c r="L42" cm="1">
+        <f t="array" aca="1" ref="L42" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K42)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M42" cm="1">
+        <f t="array" aca="1" ref="M42" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K42)</f>
+        <v>0.4</v>
+      </c>
+      <c r="N42" cm="1">
+        <f t="array" aca="1" ref="N42" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K42)</f>
+        <v>0.16226694553795112</v>
       </c>
     </row>
     <row r="43" spans="11:14" x14ac:dyDescent="0.3">
       <c r="K43">
         <v>4.0000000000000018</v>
       </c>
-      <c r="L43" t="e" cm="1">
-        <f t="array" aca="1" ref="L43" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve_,K43)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="M43" t="e" cm="1">
-        <f t="array" aca="1" ref="M43" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve_,K43)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="N43" t="e" cm="1">
-        <f t="array" aca="1" ref="N43" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve_,K43)</f>
-        <v>#NUM!</v>
+      <c r="L43" cm="1">
+        <f t="array" aca="1" ref="L43" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K43)</f>
+        <v>0.4</v>
+      </c>
+      <c r="M43" cm="1">
+        <f t="array" aca="1" ref="M43" ca="1">_xll.TMX.PWFLAT.CURVE.SPOT(curve,K43)</f>
+        <v>0.4</v>
+      </c>
+      <c r="N43" cm="1">
+        <f t="array" aca="1" ref="N43" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K43)</f>
+        <v>0.15590436759636864</v>
       </c>
     </row>
   </sheetData>
@@ -5190,7 +5164,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8A3DD8-75E7-4A72-9366-AF366CC35FAC}">
   <dimension ref="B1:G552"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5216,7 +5192,7 @@
       </c>
       <c r="E2" s="5" cm="1">
         <f t="array" ref="E2">_xll.\TMX.BOND.SIMPLE(D2,D3,D4,D5)</f>
-        <v>2982917215248</v>
+        <v>1204222248384</v>
       </c>
       <c r="F2" cm="1">
         <f t="array" ref="F2:F5">_xll.TMX.BOND.SIMPLE(E2)</f>
@@ -5247,10 +5223,10 @@
     </row>
     <row r="4" spans="2:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D4">
         <v>12</v>
@@ -5265,16 +5241,16 @@
     </row>
     <row r="5" spans="2:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5">
-        <v>140716368016338</v>
+        <v>140716946699303</v>
       </c>
       <c r="F5" s="5">
-        <v>140716368016338</v>
+        <v>140716946699303</v>
       </c>
       <c r="G5" s="17" t="b">
         <f t="shared" si="0"/>
@@ -5283,11 +5259,11 @@
     </row>
     <row r="6" spans="2:7" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C6" s="5" cm="1">
         <f t="array" ref="C6">_xll.\TMX.BOND.SIMPLE(maturity, coupon, _xll.ENUM(frequency), _xll.ENUM(day_count))</f>
-        <v>2984500273248</v>
+        <v>1204222233696</v>
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
@@ -5296,46 +5272,46 @@
       </c>
       <c r="C7" s="2">
         <f ca="1">TODAY()</f>
-        <v>45094</v>
+        <v>45102</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B8" s="10" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C8" s="5" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_xll.\TMX.BOND.INSTRUMENT(bond.simple, dated)</f>
-        <v>2983253086896</v>
+        <v>1204148803248</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="10" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9" s="20" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">_xll.TMX.VALUE.YIELD(instrument, 1)</f>
-        <v>4.8786680314628891E-2</v>
+        <v>4.8786679882032745E-2</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C10" s="20"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C11" s="20"/>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C12" s="20" cm="1">
         <f t="array" aca="1" ref="C12" ca="1">_xll.TMX.VALUE.COMPOUND_YIELD(C9,12/_xll.ENUM(frequency))</f>
-        <v>4.9996341958828738E-2</v>
+        <v>4.9996341504604302E-2</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
@@ -5343,7 +5319,7 @@
         <v>16</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>8</v>
@@ -5361,7 +5337,7 @@
       </c>
       <c r="E14" s="2" cm="1">
         <f t="array" aca="1" ref="E14:E17" ca="1">_xlfn.MAP(INDEX(_xlfn.ANCHORARRAY(C14),,1),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.DATE.ADD_YEARS(dated,_xlpm.t)))</f>
-        <v>45460</v>
+        <v>45468</v>
       </c>
       <c r="G14" s="2"/>
     </row>
@@ -5376,7 +5352,7 @@
       </c>
       <c r="E15" s="2">
         <f ca="1"/>
-        <v>45824.999988425923</v>
+        <v>45832.999988425923</v>
       </c>
       <c r="G15" s="2"/>
     </row>
@@ -5391,7 +5367,7 @@
       </c>
       <c r="E16" s="2">
         <f ca="1"/>
-        <v>46190</v>
+        <v>46198</v>
       </c>
       <c r="G16" s="2"/>
     </row>
@@ -5406,7 +5382,7 @@
       </c>
       <c r="E17" s="2">
         <f ca="1"/>
-        <v>46555</v>
+        <v>46563</v>
       </c>
       <c r="G17" s="2"/>
     </row>
@@ -7380,9 +7356,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D92863B8-4C87-4474-B5B0-52EEB5BB3C33}">
-  <dimension ref="B2:K107"/>
+  <dimension ref="B2:P107"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -7395,12 +7373,102 @@
     <col min="10" max="10" width="9.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:16" ht="21" x14ac:dyDescent="0.3">
       <c r="B2" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="F2" cm="1">
+        <f t="array" aca="1" ref="F2:P3" ca="1">_xll.TMX.PWFLAT.CURVE(curve)</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f ca="1"/>
+        <v>-1.4566508585916602E+144</v>
+      </c>
+      <c r="H2">
+        <f ca="1"/>
+        <v>-1.4568153451023237E+144</v>
+      </c>
+      <c r="I2">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <f ca="1"/>
+        <v>-1.4568159901474629E+144</v>
+      </c>
+      <c r="K2">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <f ca="1"/>
+        <v>0</v>
+      </c>
+      <c r="P3" t="e">
+        <f ca="1"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -7411,15 +7479,15 @@
       <c r="F4" s="3"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:16" x14ac:dyDescent="0.3">
       <c r="G5" s="19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="H5">
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -7437,16 +7505,16 @@
       </c>
       <c r="G6" s="5" cm="1">
         <f t="array" aca="1" ref="G6" ca="1">_xll.\TMX.BOOTSTRAP(instrument, price)</f>
-        <v>2982856662048</v>
+        <v>1204148805008</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>1</v>
       </c>
@@ -7458,40 +7526,40 @@
       </c>
       <c r="E7" s="5" cm="1">
         <f t="array" ref="E7">_xll.\TMX.BOND.SIMPLE(B7, C7)</f>
-        <v>2982927163792</v>
+        <v>1204222233024</v>
       </c>
       <c r="F7" s="5" cm="1">
         <f t="array" ref="F7">_xll.\TMX.BOND.INSTRUMENT(E7, dated)</f>
-        <v>2983254600688</v>
+        <v>1204151950928</v>
       </c>
       <c r="H7" cm="1">
         <f t="array" ref="H7:H107">_xlfn.SEQUENCE(1+10/H5,1,0,H5)</f>
         <v>0</v>
       </c>
-      <c r="I7" s="21" t="e" cm="1">
-        <f t="array" aca="1" ref="I7:I107" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(H7),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.PWFLAT.CURVE.VALUE(curve,_xlpm.t)))</f>
-        <v>#NUM!</v>
+      <c r="I7" s="21" cm="1">
+        <f t="array" aca="1" ref="I7:I107" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(H7),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.PWFLAT.CURVE.FORWARD(curve,_xlpm.t)))</f>
+        <v>0</v>
       </c>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" s="18">
         <f ca="1">0.05 + 0.01*RAND()</f>
-        <v>5.3318075122254296E-2</v>
+        <v>5.2378599755430709E-2</v>
       </c>
       <c r="D8" s="6">
         <v>1</v>
       </c>
       <c r="E8" s="5" cm="1">
         <f t="array" aca="1" ref="E8" ca="1">_xll.\TMX.BOND.SIMPLE(B8, C8)</f>
-        <v>2984490708224</v>
+        <v>1204697061760</v>
       </c>
       <c r="F8" s="5" cm="1">
         <f t="array" aca="1" ref="F8" ca="1">_xll.\TMX.BOND.INSTRUMENT(E8, dated)</f>
-        <v>2983253091856</v>
+        <v>1204148804304</v>
       </c>
       <c r="H8">
         <v>0.1</v>
@@ -7501,7 +7569,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>3</v>
       </c>
@@ -7513,11 +7581,11 @@
       </c>
       <c r="E9" s="5" cm="1">
         <f t="array" ref="E9">_xll.\TMX.BOND.SIMPLE(B9, C9)</f>
-        <v>2982917218896</v>
+        <v>1204222248096</v>
       </c>
       <c r="F9" s="5" cm="1">
         <f t="array" ref="F9">_xll.\TMX.BOND.INSTRUMENT(E9, dated)</f>
-        <v>2983254605808</v>
+        <v>1204151955680</v>
       </c>
       <c r="H9">
         <v>0.2</v>
@@ -7527,7 +7595,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>4</v>
       </c>
@@ -7539,11 +7607,11 @@
       </c>
       <c r="E10" s="5" cm="1">
         <f t="array" ref="E10">_xll.\TMX.BOND.SIMPLE(B10, C10)</f>
-        <v>2982927155824</v>
+        <v>1204222247904</v>
       </c>
       <c r="F10" s="5" cm="1">
         <f t="array" ref="F10">_xll.\TMX.BOND.INSTRUMENT(E10, dated)</f>
-        <v>2983254604208</v>
+        <v>1204151952512</v>
       </c>
       <c r="H10">
         <v>0.30000000000000004</v>
@@ -7553,7 +7621,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>5</v>
       </c>
@@ -7565,11 +7633,11 @@
       </c>
       <c r="E11" s="5" cm="1">
         <f t="array" ref="E11">_xll.\TMX.BOND.SIMPLE(B11, C11)</f>
-        <v>2982927155728</v>
+        <v>1204222246368</v>
       </c>
       <c r="F11" s="5" cm="1">
         <f t="array" ref="F11">_xll.\TMX.BOND.INSTRUMENT(E11, dated)</f>
-        <v>2983254598928</v>
+        <v>1204151955856</v>
       </c>
       <c r="H11">
         <v>0.4</v>
@@ -7579,7 +7647,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>6</v>
       </c>
@@ -7591,11 +7659,11 @@
       </c>
       <c r="E12" s="5" cm="1">
         <f t="array" ref="E12">_xll.\TMX.BOND.SIMPLE(B12, C12)</f>
-        <v>2982927162160</v>
+        <v>1204222246272</v>
       </c>
       <c r="F12" s="5" cm="1">
         <f t="array" ref="F12">_xll.\TMX.BOND.INSTRUMENT(E12, dated)</f>
-        <v>2983254606128</v>
+        <v>1204151956736</v>
       </c>
       <c r="H12">
         <v>0.5</v>
@@ -7605,7 +7673,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>7</v>
       </c>
@@ -7617,11 +7685,11 @@
       </c>
       <c r="E13" s="5" cm="1">
         <f t="array" ref="E13">_xll.\TMX.BOND.SIMPLE(B13, C13)</f>
-        <v>2982927481312</v>
+        <v>1204222244832</v>
       </c>
       <c r="F13" s="5" cm="1">
         <f t="array" ref="F13">_xll.\TMX.BOND.INSTRUMENT(E13, dated)</f>
-        <v>2983254602608</v>
+        <v>1204151950576</v>
       </c>
       <c r="H13">
         <v>0.6</v>
@@ -7631,7 +7699,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>8</v>
       </c>
@@ -7643,11 +7711,11 @@
       </c>
       <c r="E14" s="5" cm="1">
         <f t="array" ref="E14">_xll.\TMX.BOND.SIMPLE(B14, C14)</f>
-        <v>2982917218320</v>
+        <v>1204222251936</v>
       </c>
       <c r="F14" s="5" cm="1">
         <f t="array" ref="F14">_xll.\TMX.BOND.INSTRUMENT(E14, dated)</f>
-        <v>2983254605488</v>
+        <v>1204151955504</v>
       </c>
       <c r="H14">
         <v>0.7</v>
@@ -7657,7 +7725,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>9</v>
       </c>
@@ -7669,11 +7737,11 @@
       </c>
       <c r="E15" s="5" cm="1">
         <f t="array" ref="E15">_xll.\TMX.BOND.SIMPLE(B15, C15)</f>
-        <v>2982917228784</v>
+        <v>1204222250880</v>
       </c>
       <c r="F15" s="5" cm="1">
         <f t="array" ref="F15">_xll.\TMX.BOND.INSTRUMENT(E15, dated)</f>
-        <v>2983254603088</v>
+        <v>1204151951808</v>
       </c>
       <c r="H15">
         <v>0.79999999999999993</v>
@@ -7683,7 +7751,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>10</v>
       </c>
@@ -7695,11 +7763,11 @@
       </c>
       <c r="E16" s="5" cm="1">
         <f t="array" ref="E16">_xll.\TMX.BOND.SIMPLE(B16, C16)</f>
-        <v>2982917218224</v>
+        <v>1204222248288</v>
       </c>
       <c r="F16" s="5" cm="1">
         <f t="array" ref="F16">_xll.\TMX.BOND.INSTRUMENT(E16, dated)</f>
-        <v>2983254601808</v>
+        <v>1204151956384</v>
       </c>
       <c r="H16">
         <v>0.89999999999999991</v>
@@ -7709,7 +7777,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="17" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H17">
         <v>0.99999999999999989</v>
       </c>
@@ -7718,7 +7786,8 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="18" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:11" x14ac:dyDescent="0.3">
+      <c r="E18" s="5"/>
       <c r="H18">
         <v>1.0999999999999999</v>
       </c>
@@ -7727,7 +7796,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="19" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H19">
         <v>1.2</v>
       </c>
@@ -7736,7 +7805,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="20" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H20">
         <v>1.3</v>
       </c>
@@ -7745,7 +7814,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="21" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H21">
         <v>1.4000000000000001</v>
       </c>
@@ -7755,10 +7824,10 @@
       </c>
       <c r="K21" t="e" cm="1">
         <f t="array" aca="1" ref="K21" ca="1">_xll.TMX.PWFLAT.CURVE.VALUE(curve, H21)</f>
-        <v>#NUM!</v>
-      </c>
-    </row>
-    <row r="22" spans="8:11" x14ac:dyDescent="0.3">
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="22" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H22">
         <v>1.5000000000000002</v>
       </c>
@@ -7767,7 +7836,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="23" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H23">
         <v>1.6000000000000003</v>
       </c>
@@ -7776,7 +7845,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="24" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H24">
         <v>1.7000000000000004</v>
       </c>
@@ -7785,7 +7854,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="25" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H25">
         <v>1.8000000000000005</v>
       </c>
@@ -7794,7 +7863,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="26" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H26">
         <v>1.9000000000000006</v>
       </c>
@@ -7803,7 +7872,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="27" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H27">
         <v>2.0000000000000004</v>
       </c>
@@ -7812,7 +7881,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="28" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H28">
         <v>2.1000000000000005</v>
       </c>
@@ -7821,7 +7890,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="29" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H29">
         <v>2.2000000000000006</v>
       </c>
@@ -7830,7 +7899,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="30" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H30">
         <v>2.3000000000000007</v>
       </c>
@@ -7839,7 +7908,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="31" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H31">
         <v>2.4000000000000008</v>
       </c>
@@ -7848,7 +7917,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="32" spans="8:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="5:11" x14ac:dyDescent="0.3">
       <c r="H32">
         <v>2.5000000000000009</v>
       </c>
@@ -8555,7 +8624,7 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C2" s="9">
         <v>0.1</v>
@@ -8563,7 +8632,7 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C3" s="9">
         <v>0.01</v>
@@ -8571,7 +8640,7 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B4" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C4" s="9">
         <v>10</v>
@@ -8579,7 +8648,7 @@
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C5" s="9">
         <v>20</v>
@@ -8587,7 +8656,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C6">
         <f>EXP(-r_*t)</f>
@@ -8596,7 +8665,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B7" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C7">
         <f>EXP(-r_*u)</f>
@@ -8609,25 +8678,25 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B8" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C8">
         <f ca="1">EXP(-r_*(u-t)-σ^2*(u-t)^3/6-σ*(u-t)*_xlfn.NORM.S.INV(RAND())*SQRT(t))</f>
-        <v>0.43184198897970238</v>
+        <v>0.3102389784365393</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B9" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C9">
         <f ca="1">LN(C8)</f>
-        <v>-0.83969552389750657</v>
+        <v>-1.1704123803099415</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B10" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C10" cm="1">
         <f t="array" ref="C10">_xll.TMX.HO_LEE.ED(Dt, Du, t, u, σ)</f>
@@ -8640,7 +8709,7 @@
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B11" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C11" cm="1">
         <f t="array" ref="C11">_xll.TMX.HO_LEE.ELogD(Dt, Du, t, u, σ)</f>
@@ -8657,7 +8726,7 @@
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B12" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C12" cm="1">
         <f t="array" ref="C12">_xll.TMX.HO_LEE.VarLogD(t, u, σ)</f>

</xml_diff>

<commit_message>
implied vol use Newton in bootstrap covariance for Ho-Lee bullet instrument
</commit_message>
<xml_diff>
--- a/bondxll/bondlib.xlsx
+++ b/bondxll/bondlib.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keith\source\repos\tmcrossx\bondlib\bondxll\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE2964D1-706C-4768-8864-2F36017D3B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED51BCB9-147F-4B01-B634-C7EED12F36EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{06412BBD-41CB-406E-9C18-9630F19E364B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{06412BBD-41CB-406E-9C18-9630F19E364B}"/>
   </bookViews>
   <sheets>
     <sheet name="Enum" sheetId="4" r:id="rId1"/>
@@ -327,7 +327,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -390,6 +390,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -512,7 +519,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Check Cell" xfId="3" builtinId="23"/>
@@ -715,91 +722,91 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.2</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.2</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.2</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.2</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.2</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.2</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.2</c:v>
+                  <c:v>0.3</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.2</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.2</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.2</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.3</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.3</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.3</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.3</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.3</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.3</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.3</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.3</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.3</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0.5</c:v>
@@ -1006,124 +1013,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.21249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.22222222222222224</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.58491436821452436</c:v>
+                  <c:v>0.22999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.54992215292229485</c:v>
+                  <c:v>0.23636363636363641</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.52076197351210363</c:v>
+                  <c:v>0.24166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.49608797554963407</c:v>
+                  <c:v>0.2461538461538462</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.47493883443894597</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.45660957880968289</c:v>
+                  <c:v>0.25333333333333335</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.44057148013407771</c:v>
+                  <c:v>0.25624999999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.42642021659677898</c:v>
+                  <c:v>0.25882352941176467</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.4138413156747357</c:v>
+                  <c:v>0.27222222222222225</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.40258650958659176</c:v>
+                  <c:v>0.28421052631578947</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.39245718410726216</c:v>
+                  <c:v>0.29499999999999998</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.38805446105453539</c:v>
+                  <c:v>0.30476190476190473</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.3840519855520565</c:v>
+                  <c:v>0.3136363636363636</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.38039755139761927</c:v>
+                  <c:v>0.32173913043478258</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.37704765342271845</c:v>
+                  <c:v>0.32916666666666661</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.37396574728580972</c:v>
+                  <c:v>0.33600000000000002</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.37112091085174015</c:v>
+                  <c:v>0.34230769230769231</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.36848680304241643</c:v>
+                  <c:v>0.3481481481481481</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.36604084579090151</c:v>
+                  <c:v>0.35357142857142854</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.36376357524638764</c:v>
+                  <c:v>0.35862068965517241</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.36163812273817481</c:v>
+                  <c:v>0.36333333333333334</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.3661014091014595</c:v>
+                  <c:v>0.36774193548387096</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.37028574006703885</c:v>
+                  <c:v>0.37187499999999996</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.37421647521652257</c:v>
+                  <c:v>0.37575757575757573</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.37791599065133069</c:v>
+                  <c:v>0.37941176470588234</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.38140410520414986</c:v>
+                  <c:v>0.38285714285714284</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.38469843561514566</c:v>
+                  <c:v>0.38611111111111107</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.38781469411203362</c:v>
+                  <c:v>0.38918918918918916</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.3907669390038222</c:v>
+                  <c:v>0.39210526315789473</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.39356778672167292</c:v>
+                  <c:v>0.39487179487179486</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.39622859205363109</c:v>
+                  <c:v>0.39749999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1297,124 +1304,124 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.94318631703792211</c:v>
+                  <c:v>0.98019867330675525</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.88960042864755973</c:v>
+                  <c:v>0.96078943915232318</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.83905895193144875</c:v>
+                  <c:v>0.94176453358424872</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.79138892264992211</c:v>
+                  <c:v>0.92311634638663576</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.74642720329878909</c:v>
+                  <c:v>0.90483741803595952</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.70401992481630127</c:v>
+                  <c:v>0.88692043671715748</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.66402196000880198</c:v>
+                  <c:v>0.86935823539880586</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.62629642689300435</c:v>
+                  <c:v>0.8436648165963837</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.59071422025522302</c:v>
+                  <c:v>0.81873075307798182</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.55715356982445186</c:v>
+                  <c:v>0.79453360250333405</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.54612118997005032</c:v>
+                  <c:v>0.77105158580356614</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.53530726587334976</c:v>
+                  <c:v>0.74826356757856527</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.52470747182052402</c:v>
+                  <c:v>0.72614903707369083</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.51431756775261928</c:v>
+                  <c:v>0.70468808971871344</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.50413339756947462</c:v>
+                  <c:v>0.68386140921235583</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.49415088746722613</c:v>
+                  <c:v>0.6636502501363194</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.48436604430873076</c:v>
+                  <c:v>0.64403642108314141</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.47477495402625897</c:v>
+                  <c:v>0.61262639418441589</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.46537378005581476</c:v>
+                  <c:v>0.58274825237398964</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.4561587618024594</c:v>
+                  <c:v>0.5543272847345071</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.44267723298021455</c:v>
+                  <c:v>0.52729242404304855</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.42959414354926156</c:v>
+                  <c:v>0.50157606906605556</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.41689771784597751</c:v>
+                  <c:v>0.47711391552103427</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.40457652823019508</c:v>
+                  <c:v>0.45384479528235583</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.39261948479955472</c:v>
+                  <c:v>0.43171052342907956</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.38101582540784434</c:v>
+                  <c:v>0.41065575275234545</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.36975510597834071</c:v>
+                  <c:v>0.39062783535852114</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.35882719110343608</c:v>
+                  <c:v>0.3715766910220456</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.34822224492208653</c:v>
+                  <c:v>0.35345468195878016</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.33793072226687343</c:v>
+                  <c:v>0.33621649370673323</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.3214496464630287</c:v>
+                  <c:v>0.31981902181630384</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.30577236221098475</c:v>
+                  <c:v>0.30422126406670408</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.29085966813417891</c:v>
+                  <c:v>0.28938421793905056</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.27667427472974365</c:v>
+                  <c:v>0.27527078308975234</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.26318071112532648</c:v>
+                  <c:v>0.26184566858032593</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.25034523638343303</c:v>
+                  <c:v>0.24907530463166816</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.23813575513150817</c:v>
+                  <c:v>0.23692775868212176</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.22652173730678746</c:v>
+                  <c:v>0.22537265553943867</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.21547414181523736</c:v>
+                  <c:v>0.21438110142697794</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.2049653439136935</c:v>
+                  <c:v>0.20392561173421347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1588,91 +1595,91 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="41"/>
                 <c:pt idx="0">
-                  <c:v>0.68491436821452434</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.68491436821452434</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.68491436821452434</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.68491436821452434</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.68491436821452434</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.68491436821452434</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.68491436821452434</c:v>
+                  <c:v>0.30000000000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.68491436821452434</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.68491436821452434</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.68491436821452434</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.30000000000000004</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.4</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.4</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.4</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.4</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.4</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.4</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.4</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.4</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.4</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>0.6</c:v>
@@ -2330,307 +2337,307 @@
                 <c:formatCode>0.000%</c:formatCode>
                 <c:ptCount val="101"/>
                 <c:pt idx="0">
-                  <c:v>4.9283011639120938E-2</c:v>
+                  <c:v>4.9283013956455027E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9283011639120938E-2</c:v>
+                  <c:v>4.9283013956455027E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9283011639120938E-2</c:v>
+                  <c:v>4.9283013956455027E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9283011639120938E-2</c:v>
+                  <c:v>4.9283013956455027E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.9283011639120938E-2</c:v>
+                  <c:v>4.9283013956455027E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.9283011639120938E-2</c:v>
+                  <c:v>4.9283013956455027E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.9283011639120938E-2</c:v>
+                  <c:v>4.9283013956455027E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.9283011639120938E-2</c:v>
+                  <c:v>4.9283013956455027E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.9283011639120938E-2</c:v>
+                  <c:v>4.9283013956455027E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.9283011639120938E-2</c:v>
+                  <c:v>4.9283013956455027E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4.9283011639120938E-2</c:v>
+                  <c:v>4.9283013956455027E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.1585054314548233E-2</c:v>
+                  <c:v>4.04216230000293E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.1585054314548233E-2</c:v>
+                  <c:v>4.04216230000293E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.1585054314548233E-2</c:v>
+                  <c:v>4.04216230000293E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.1585054314548233E-2</c:v>
+                  <c:v>4.04216230000293E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.1585054314548233E-2</c:v>
+                  <c:v>4.04216230000293E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.1585054314548233E-2</c:v>
+                  <c:v>4.04216230000293E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.1585054314548233E-2</c:v>
+                  <c:v>4.04216230000293E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.1585054314548233E-2</c:v>
+                  <c:v>4.04216230000293E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.1585054314548233E-2</c:v>
+                  <c:v>4.04216230000293E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.1585054314548233E-2</c:v>
+                  <c:v>4.04216230000293E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4.7137984858476464E-2</c:v>
+                  <c:v>5.8868051747390009E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.7137984858476464E-2</c:v>
+                  <c:v>5.8868051747390009E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.7137984858476464E-2</c:v>
+                  <c:v>5.8868051747390009E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4.7137984858476464E-2</c:v>
+                  <c:v>5.8868051747390009E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.7137984858476464E-2</c:v>
+                  <c:v>5.8868051747390009E-2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4.7137984858476464E-2</c:v>
+                  <c:v>5.8868051747390009E-2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.7137984858476464E-2</c:v>
+                  <c:v>5.8868051747390009E-2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4.7137984858476464E-2</c:v>
+                  <c:v>5.8868051747390009E-2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4.7137984858476464E-2</c:v>
+                  <c:v>5.8868051747390009E-2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.7137984858476464E-2</c:v>
+                  <c:v>5.8868051747390009E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.9416364517221215E-2</c:v>
+                  <c:v>4.9416393249193918E-2</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.9416364517221215E-2</c:v>
+                  <c:v>4.9416393249193918E-2</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.9416364517221215E-2</c:v>
+                  <c:v>4.9416393249193918E-2</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.9416364517221215E-2</c:v>
+                  <c:v>4.9416393249193918E-2</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.9416364517221215E-2</c:v>
+                  <c:v>4.9416393249193918E-2</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.9416364517221215E-2</c:v>
+                  <c:v>4.9416393249193918E-2</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.9416364517221215E-2</c:v>
+                  <c:v>4.9416393249193918E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.9416364517221215E-2</c:v>
+                  <c:v>4.9416393249193918E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.9416364517221215E-2</c:v>
+                  <c:v>4.9416393249193918E-2</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.9416364517221215E-2</c:v>
+                  <c:v>4.9416393249193918E-2</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.9283017362953575E-2</c:v>
+                  <c:v>4.928301622797935E-2</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.9283017362953575E-2</c:v>
+                  <c:v>4.928301622797935E-2</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.9283017362953575E-2</c:v>
+                  <c:v>4.928301622797935E-2</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4.9283017362953575E-2</c:v>
+                  <c:v>4.928301622797935E-2</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4.9283017362953575E-2</c:v>
+                  <c:v>4.928301622797935E-2</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4.9283017362953575E-2</c:v>
+                  <c:v>4.928301622797935E-2</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4.9283017362953575E-2</c:v>
+                  <c:v>4.928301622797935E-2</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4.9283017362953575E-2</c:v>
+                  <c:v>4.928301622797935E-2</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4.9283017362953575E-2</c:v>
+                  <c:v>4.928301622797935E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4.9283017362953575E-2</c:v>
+                  <c:v>4.928301622797935E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.941632836041359E-2</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.941632836041359E-2</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.941632836041359E-2</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.941632836041359E-2</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.941632836041359E-2</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.941632836041359E-2</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.941632836041359E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.941632836041359E-2</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.941632836041359E-2</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.941632836041359E-2</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>4.9416357720749815E-2</c:v>
+                  <c:v>4.9416364453131766E-2</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>4.9283035687621969E-2</c:v>
+                  <c:v>4.928305695371818E-2</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>4.9283035687621969E-2</c:v>
+                  <c:v>4.928305695371818E-2</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>4.9283035687621969E-2</c:v>
+                  <c:v>4.928305695371818E-2</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>4.9283035687621969E-2</c:v>
+                  <c:v>4.928305695371818E-2</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>4.9283035687621969E-2</c:v>
+                  <c:v>4.928305695371818E-2</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>4.9283035687621969E-2</c:v>
+                  <c:v>4.928305695371818E-2</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>4.9283035687621969E-2</c:v>
+                  <c:v>4.928305695371818E-2</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>4.9283035687621969E-2</c:v>
+                  <c:v>4.928305695371818E-2</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>4.9283035687621969E-2</c:v>
+                  <c:v>4.928305695371818E-2</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>4.9283035687621969E-2</c:v>
+                  <c:v>4.928305695371818E-2</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>4.9416357721872958E-2</c:v>
+                  <c:v>4.941630721492847E-2</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>4.9416357721872958E-2</c:v>
+                  <c:v>4.941630721492847E-2</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>4.9416357721872958E-2</c:v>
+                  <c:v>4.941630721492847E-2</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>4.9416357721872958E-2</c:v>
+                  <c:v>4.941630721492847E-2</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>4.9416357721872958E-2</c:v>
+                  <c:v>4.941630721492847E-2</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>4.9416357721872958E-2</c:v>
+                  <c:v>4.941630721492847E-2</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>4.9416357721872958E-2</c:v>
+                  <c:v>4.941630721492847E-2</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>4.9416357721872958E-2</c:v>
+                  <c:v>4.941630721492847E-2</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>4.9416357721872958E-2</c:v>
+                  <c:v>4.941630721492847E-2</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>4.9416357721872958E-2</c:v>
+                  <c:v>4.941630721492847E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4323,7 +4330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E28EA81D-C5B8-44E1-B499-71D23FEEDB1B}">
   <dimension ref="B2:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4357,7 +4364,7 @@
       </c>
       <c r="E3" s="4" cm="1">
         <f t="array" ref="E3">_xll.ENUM(D3)</f>
-        <v>140716601127980</v>
+        <v>140716816282658</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.3">
@@ -4373,7 +4380,7 @@
       </c>
       <c r="E4" s="4" cm="1">
         <f t="array" ref="E4">_xll.ENUM(D4)</f>
-        <v>140716601120750</v>
+        <v>140716816275433</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
@@ -4389,7 +4396,7 @@
       </c>
       <c r="E5" s="4" cm="1">
         <f t="array" ref="E5">_xll.ENUM(D5)</f>
-        <v>140716601126340</v>
+        <v>140716816281013</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.3">
@@ -4405,7 +4412,7 @@
       </c>
       <c r="E6" s="4" cm="1">
         <f t="array" ref="E6">_xll.ENUM(D6)</f>
-        <v>140716601131645</v>
+        <v>140716816286318</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
@@ -4414,7 +4421,7 @@
       </c>
       <c r="E7" s="4" cm="1">
         <f t="array" ref="E7">_xll.ENUM(D7)</f>
-        <v>140716601163150</v>
+        <v>140716816317818</v>
       </c>
     </row>
   </sheetData>
@@ -4441,7 +4448,7 @@
       </c>
       <c r="C2" s="8">
         <f ca="1">50 + 100*RAND()</f>
-        <v>124.59833498475891</v>
+        <v>103.88369677903663</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
@@ -4450,7 +4457,7 @@
       </c>
       <c r="C3" s="8">
         <f ca="1">0.01 + 0.3*RAND()</f>
-        <v>0.29802669645075003</v>
+        <v>3.8538256359418266E-2</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
@@ -4459,7 +4466,7 @@
       </c>
       <c r="C4" s="8">
         <f ca="1">50 + 100*RAND()</f>
-        <v>103.88413278061428</v>
+        <v>130.27888599583795</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -4468,7 +4475,7 @@
       </c>
       <c r="C5" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">_xll.TMX.BLACK.MONEYNESS(f, s, k)</f>
-        <v>-0.46106311594071869</v>
+        <v>5.8940926863297287</v>
       </c>
       <c r="D5">
         <v>1E-3</v>
@@ -4487,19 +4494,19 @@
       </c>
       <c r="C6" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">_xll.TMX.BLACK.PUT.VALUE(f, s, k)</f>
-        <v>5.5923254240287044</v>
+        <v>26.395189218333897</v>
       </c>
       <c r="D6" cm="1">
         <f t="array" aca="1" ref="D6" ca="1">_xll.TMX.BLACK.PUT.VALUE(f + D5, s, k)</f>
-        <v>5.5921015286392688</v>
+        <v>26.394189218336265</v>
       </c>
       <c r="E6" cm="1">
         <f t="array" aca="1" ref="E6" ca="1">_xll.TMX.BLACK.PUT.VALUE(f + E5, s, k)</f>
-        <v>5.5925493274722733</v>
+        <v>26.396189218331529</v>
       </c>
       <c r="G6" cm="1">
         <f t="array" aca="1" ref="G6" ca="1">_xll.TMX.BLACK.CALL.VALUE(f, s, k)</f>
-        <v>26.306527628173331</v>
+        <v>1.5325696267609601E-9</v>
       </c>
       <c r="H6" s="16">
         <f ca="1">G6-C6-f+k</f>
@@ -4512,19 +4519,19 @@
       </c>
       <c r="C7" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">_xll.TMX.BLACK.PUT.DELTA(f, s, k)</f>
-        <v>-0.22389941646934114</v>
+        <v>-0.9999999976228936</v>
       </c>
       <c r="D7">
         <f ca="1">(D6-E6)/(D5-E5)</f>
-        <v>-0.22389941650224898</v>
+        <v>-0.99999999763156211</v>
       </c>
       <c r="E7" s="16">
         <f ca="1">(C7-D7)/C7</f>
-        <v>-1.4697601108605043E-10</v>
+        <v>-8.6685103745767319E-12</v>
       </c>
       <c r="G7" cm="1">
         <f t="array" aca="1" ref="G7" ca="1">_xll.TMX.BLACK.CALL.DELTA(f, s, k)</f>
-        <v>0.22389941646934114</v>
+        <v>0.9999999976228936</v>
       </c>
       <c r="H7" s="16">
         <f ca="1">G7+C7</f>
@@ -4537,15 +4544,15 @@
       </c>
       <c r="C8" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_xll.TMX.BLACK.GAMMA(f, s, k)</f>
-        <v>8.0541303100472323E-3</v>
+        <v>3.5729813123032195E-9</v>
       </c>
       <c r="D8">
         <f ca="1">(D6-2*C6+E6)/(D5^2)</f>
-        <v>8.0541333602468512E-3</v>
+        <v>0</v>
       </c>
       <c r="E8" s="16">
         <f t="shared" ref="E8:E9" ca="1" si="0">(C8-D8)/C8</f>
-        <v>-3.7871247440807396E-7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -4554,15 +4561,15 @@
       </c>
       <c r="C9" cm="1">
         <f t="array" aca="1" ref="C9" ca="1">_xll.TMX.BLACK.VEGA(f, s, k)</f>
-        <v>37.264757413253818</v>
+        <v>1.4859958547599377E-6</v>
       </c>
       <c r="D9" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">(_xll.TMX.BLACK.PUT.VALUE(f, s + D5, k) - _xll.TMX.BLACK.PUT.VALUE(f, s + E5, k))/(D5 - E5)</f>
-        <v>37.264686347766585</v>
+        <v>1.6717009998501453E-6</v>
       </c>
       <c r="E9" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>1.9070427977156908E-6</v>
+        <v>-0.12497016360803258</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.3"/>
@@ -4577,9 +4584,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6DAD46C-D019-4BB0-8142-A427C42D3B36}">
-  <dimension ref="B2:D11"/>
+  <dimension ref="B2:H11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4588,69 +4597,79 @@
     <col min="4" max="4" width="10.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="7">
         <f ca="1">TODAY()</f>
-        <v>45114</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
+        <v>45115</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45115</v>
+      </c>
+      <c r="G2" s="15">
+        <v>2.0014100221085989</v>
+      </c>
+      <c r="H2" s="31" cm="1">
+        <f t="array" ref="H2">_xll.TMX.DATE.ADD_YEARS(F2,G2)</f>
+        <v>45845.999988425923</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="8">
         <f ca="1">10*RAND()</f>
-        <v>2.3365534051456374</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+        <v>4.9696885705002947</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2" cm="1">
         <f t="array" aca="1" ref="C4" ca="1">_xll.TMX.DATE.ADD_YEARS(date,years)</f>
-        <v>45967.408599537041</v>
+        <v>46930.141469907408</v>
       </c>
       <c r="D4">
         <f ca="1">C4</f>
-        <v>45967.408599537041</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>46930.141469907408</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="2" cm="1">
         <f t="array" aca="1" ref="C5" ca="1">_xll.TMX.DATE.ADD_YEARS(C4,-years)</f>
-        <v>45114.000000000007</v>
+        <v>45115</v>
       </c>
       <c r="D5" s="6">
         <f ca="1">C5-date</f>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C6" cm="1">
         <f t="array" aca="1" ref="C6" ca="1">_xll.TMX.DATE.SUB_YEARS(C4,date)</f>
-        <v>2.3354346769611971</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+        <v>4.9693012176841416</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
       <c r="C7" s="2" cm="1">
         <f t="array" aca="1" ref="C7" ca="1">_xll.TMX.DATE.ADD_YEARS(date,C6)</f>
-        <v>45967</v>
+        <v>46930</v>
       </c>
       <c r="D7">
         <f ca="1">C7</f>
-        <v>45967</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>46930</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="3" t="s">
         <v>14</v>
       </c>
@@ -4662,7 +4681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
@@ -4674,7 +4693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
         <v>12</v>
       </c>
@@ -4686,18 +4705,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="2" cm="1">
         <f t="array" aca="1" ref="C11" ca="1">_xll.TMX.DATE.ADD_YMD(date, years_,months, days)</f>
-        <v>45545</v>
+        <v>45546</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError xmlns:x16r3="http://schemas.microsoft.com/office/spreadsheetml/2018/08/main" sqref="D4 D7" x16r3:misleadingFormat="1"/>
   </ignoredErrors>
@@ -4708,9 +4727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B429FC-4136-41AD-B308-B590D229D902}">
   <dimension ref="B2:O42"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -4734,7 +4751,7 @@
         <v>63</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>15</v>
@@ -4758,7 +4775,7 @@
       </c>
       <c r="C3" s="14">
         <f ca="1">RAND()</f>
-        <v>0.58491436821452436</v>
+        <v>0.14206838973162428</v>
       </c>
       <c r="E3" s="25" cm="1">
         <f t="array" aca="1" ref="E3:F6" ca="1">TRANSPOSE(_xll.TMX.PWFLAT.CURVE(curve))</f>
@@ -4766,7 +4783,7 @@
       </c>
       <c r="F3" s="26">
         <f ca="1"/>
-        <v>0.58491436821452436</v>
+        <v>0.14206838973162428</v>
       </c>
       <c r="G3" s="15"/>
       <c r="H3" s="3" t="s">
@@ -4774,7 +4791,7 @@
       </c>
       <c r="I3" s="4" cm="1">
         <f t="array" aca="1" ref="I3" ca="1">_xll.\TMX.PWFLAT.CURVE(time, rate, extrapolate)</f>
-        <v>2046831270480</v>
+        <v>1522057182656</v>
       </c>
       <c r="K3" cm="1">
         <f t="array" ref="K3:K42">_xll.ARRAY.SEQUENCE(0.1,4,0.1)</f>
@@ -4782,19 +4799,19 @@
       </c>
       <c r="L3" cm="1">
         <f t="array" aca="1" ref="L3" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K3,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.2</v>
       </c>
       <c r="M3" cm="1">
         <f t="array" aca="1" ref="M3" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K3,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.2</v>
       </c>
       <c r="N3" cm="1">
         <f t="array" aca="1" ref="N3" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K3,translate)</f>
-        <v>0.94318631703792211</v>
+        <v>0.98019867330675525</v>
       </c>
       <c r="O3" cm="1">
         <f t="array" aca="1" ref="O3" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K3,translate)</f>
-        <v>0.68491436821452434</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.3">
@@ -4823,19 +4840,19 @@
       </c>
       <c r="L4" cm="1">
         <f t="array" aca="1" ref="L4" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K4,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.2</v>
       </c>
       <c r="M4" cm="1">
         <f t="array" aca="1" ref="M4" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K4,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.2</v>
       </c>
       <c r="N4" cm="1">
         <f t="array" aca="1" ref="N4" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K4,translate)</f>
-        <v>0.88960042864755973</v>
+        <v>0.96078943915232318</v>
       </c>
       <c r="O4" cm="1">
         <f t="array" aca="1" ref="O4" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K4,translate)</f>
-        <v>0.68491436821452434</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
@@ -4858,26 +4875,26 @@
       </c>
       <c r="I5" s="4" cm="1">
         <f t="array" aca="1" ref="I5" ca="1">_xll.\TMX.PWFLAT.CURVE.SHIFT(curve,spread)</f>
-        <v>2046831278928</v>
+        <v>1522057175264</v>
       </c>
       <c r="K5">
         <v>0.30000000000000004</v>
       </c>
       <c r="L5" cm="1">
         <f t="array" aca="1" ref="L5" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K5,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.2</v>
       </c>
       <c r="M5" cm="1">
         <f t="array" aca="1" ref="M5" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K5,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.2</v>
       </c>
       <c r="N5" cm="1">
         <f t="array" aca="1" ref="N5" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K5,translate)</f>
-        <v>0.83905895193144875</v>
+        <v>0.94176453358424872</v>
       </c>
       <c r="O5" cm="1">
         <f t="array" aca="1" ref="O5" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K5,translate)</f>
-        <v>0.68491436821452434</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.3">
@@ -4902,19 +4919,19 @@
       </c>
       <c r="L6" cm="1">
         <f t="array" aca="1" ref="L6" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K6,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.2</v>
       </c>
       <c r="M6" cm="1">
         <f t="array" aca="1" ref="M6" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K6,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.2</v>
       </c>
       <c r="N6" cm="1">
         <f t="array" aca="1" ref="N6" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K6,translate)</f>
-        <v>0.79138892264992211</v>
+        <v>0.92311634638663576</v>
       </c>
       <c r="O6" cm="1">
         <f t="array" aca="1" ref="O6" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K6,translate)</f>
-        <v>0.68491436821452434</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.3">
@@ -4923,19 +4940,19 @@
       </c>
       <c r="L7" cm="1">
         <f t="array" aca="1" ref="L7" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K7,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.2</v>
       </c>
       <c r="M7" cm="1">
         <f t="array" aca="1" ref="M7" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K7,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.2</v>
       </c>
       <c r="N7" cm="1">
         <f t="array" aca="1" ref="N7" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K7,translate)</f>
-        <v>0.74642720329878909</v>
+        <v>0.90483741803595952</v>
       </c>
       <c r="O7" cm="1">
         <f t="array" aca="1" ref="O7" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K7,translate)</f>
-        <v>0.68491436821452434</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.3">
@@ -4944,19 +4961,19 @@
       </c>
       <c r="L8" cm="1">
         <f t="array" aca="1" ref="L8" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K8,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.2</v>
       </c>
       <c r="M8" cm="1">
         <f t="array" aca="1" ref="M8" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K8,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.2</v>
       </c>
       <c r="N8" cm="1">
         <f t="array" aca="1" ref="N8" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K8,translate)</f>
-        <v>0.70401992481630127</v>
+        <v>0.88692043671715748</v>
       </c>
       <c r="O8" cm="1">
         <f t="array" aca="1" ref="O8" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K8,translate)</f>
-        <v>0.68491436821452434</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.3">
@@ -4965,19 +4982,19 @@
       </c>
       <c r="L9" cm="1">
         <f t="array" aca="1" ref="L9" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K9,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.2</v>
       </c>
       <c r="M9" cm="1">
         <f t="array" aca="1" ref="M9" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K9,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.2</v>
       </c>
       <c r="N9" cm="1">
         <f t="array" aca="1" ref="N9" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K9,translate)</f>
-        <v>0.66402196000880198</v>
+        <v>0.86935823539880586</v>
       </c>
       <c r="O9" cm="1">
         <f t="array" aca="1" ref="O9" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K9,translate)</f>
-        <v>0.68491436821452434</v>
+        <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.3">
@@ -4986,19 +5003,19 @@
       </c>
       <c r="L10" cm="1">
         <f t="array" aca="1" ref="L10" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K10,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.3</v>
       </c>
       <c r="M10" cm="1">
         <f t="array" aca="1" ref="M10" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K10,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.21249999999999999</v>
       </c>
       <c r="N10" cm="1">
         <f t="array" aca="1" ref="N10" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K10,translate)</f>
-        <v>0.62629642689300435</v>
+        <v>0.8436648165963837</v>
       </c>
       <c r="O10" cm="1">
         <f t="array" aca="1" ref="O10" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K10,translate)</f>
-        <v>0.68491436821452434</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.3">
@@ -5007,19 +5024,19 @@
       </c>
       <c r="L11" cm="1">
         <f t="array" aca="1" ref="L11" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K11,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.3</v>
       </c>
       <c r="M11" cm="1">
         <f t="array" aca="1" ref="M11" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K11,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.22222222222222224</v>
       </c>
       <c r="N11" cm="1">
         <f t="array" aca="1" ref="N11" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K11,translate)</f>
-        <v>0.59071422025522302</v>
+        <v>0.81873075307798182</v>
       </c>
       <c r="O11" cm="1">
         <f t="array" aca="1" ref="O11" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K11,translate)</f>
-        <v>0.68491436821452434</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.3">
@@ -5028,19 +5045,19 @@
       </c>
       <c r="L12" cm="1">
         <f t="array" aca="1" ref="L12" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K12,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.3</v>
       </c>
       <c r="M12" cm="1">
         <f t="array" aca="1" ref="M12" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K12,translate)</f>
-        <v>0.58491436821452436</v>
+        <v>0.22999999999999998</v>
       </c>
       <c r="N12" cm="1">
         <f t="array" aca="1" ref="N12" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K12,translate)</f>
-        <v>0.55715356982445186</v>
+        <v>0.79453360250333405</v>
       </c>
       <c r="O12" cm="1">
         <f t="array" aca="1" ref="O12" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K12,translate)</f>
-        <v>0.68491436821452434</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.3">
@@ -5049,19 +5066,19 @@
       </c>
       <c r="L13" cm="1">
         <f t="array" aca="1" ref="L13" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K13,translate)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="M13" cm="1">
         <f t="array" aca="1" ref="M13" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K13,translate)</f>
-        <v>0.54992215292229485</v>
+        <v>0.23636363636363641</v>
       </c>
       <c r="N13" cm="1">
         <f t="array" aca="1" ref="N13" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K13,translate)</f>
-        <v>0.54612118997005032</v>
+        <v>0.77105158580356614</v>
       </c>
       <c r="O13" cm="1">
         <f t="array" aca="1" ref="O13" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K13,translate)</f>
-        <v>0.30000000000000004</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.3">
@@ -5070,19 +5087,19 @@
       </c>
       <c r="L14" cm="1">
         <f t="array" aca="1" ref="L14" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K14,translate)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="M14" cm="1">
         <f t="array" aca="1" ref="M14" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K14,translate)</f>
-        <v>0.52076197351210363</v>
+        <v>0.24166666666666667</v>
       </c>
       <c r="N14" cm="1">
         <f t="array" aca="1" ref="N14" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K14,translate)</f>
-        <v>0.53530726587334976</v>
+        <v>0.74826356757856527</v>
       </c>
       <c r="O14" cm="1">
         <f t="array" aca="1" ref="O14" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K14,translate)</f>
-        <v>0.30000000000000004</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.3">
@@ -5091,19 +5108,19 @@
       </c>
       <c r="L15" cm="1">
         <f t="array" aca="1" ref="L15" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K15,translate)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="M15" cm="1">
         <f t="array" aca="1" ref="M15" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K15,translate)</f>
-        <v>0.49608797554963407</v>
+        <v>0.2461538461538462</v>
       </c>
       <c r="N15" cm="1">
         <f t="array" aca="1" ref="N15" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K15,translate)</f>
-        <v>0.52470747182052402</v>
+        <v>0.72614903707369083</v>
       </c>
       <c r="O15" cm="1">
         <f t="array" aca="1" ref="O15" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K15,translate)</f>
-        <v>0.30000000000000004</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
@@ -5112,19 +5129,19 @@
       </c>
       <c r="L16" cm="1">
         <f t="array" aca="1" ref="L16" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K16,translate)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="M16" cm="1">
         <f t="array" aca="1" ref="M16" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K16,translate)</f>
-        <v>0.47493883443894597</v>
+        <v>0.25</v>
       </c>
       <c r="N16" cm="1">
         <f t="array" aca="1" ref="N16" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K16,translate)</f>
-        <v>0.51431756775261928</v>
+        <v>0.70468808971871344</v>
       </c>
       <c r="O16" cm="1">
         <f t="array" aca="1" ref="O16" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K16,translate)</f>
-        <v>0.30000000000000004</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="17" spans="11:15" x14ac:dyDescent="0.3">
@@ -5133,19 +5150,19 @@
       </c>
       <c r="L17" cm="1">
         <f t="array" aca="1" ref="L17" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K17,translate)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="M17" cm="1">
         <f t="array" aca="1" ref="M17" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K17,translate)</f>
-        <v>0.45660957880968289</v>
+        <v>0.25333333333333335</v>
       </c>
       <c r="N17" cm="1">
         <f t="array" aca="1" ref="N17" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K17,translate)</f>
-        <v>0.50413339756947462</v>
+        <v>0.68386140921235583</v>
       </c>
       <c r="O17" cm="1">
         <f t="array" aca="1" ref="O17" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K17,translate)</f>
-        <v>0.30000000000000004</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="18" spans="11:15" x14ac:dyDescent="0.3">
@@ -5154,19 +5171,19 @@
       </c>
       <c r="L18" cm="1">
         <f t="array" aca="1" ref="L18" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K18,translate)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="M18" cm="1">
         <f t="array" aca="1" ref="M18" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K18,translate)</f>
-        <v>0.44057148013407771</v>
+        <v>0.25624999999999998</v>
       </c>
       <c r="N18" cm="1">
         <f t="array" aca="1" ref="N18" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K18,translate)</f>
-        <v>0.49415088746722613</v>
+        <v>0.6636502501363194</v>
       </c>
       <c r="O18" cm="1">
         <f t="array" aca="1" ref="O18" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K18,translate)</f>
-        <v>0.30000000000000004</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="19" spans="11:15" x14ac:dyDescent="0.3">
@@ -5175,19 +5192,19 @@
       </c>
       <c r="L19" cm="1">
         <f t="array" aca="1" ref="L19" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K19,translate)</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="M19" cm="1">
         <f t="array" aca="1" ref="M19" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K19,translate)</f>
-        <v>0.42642021659677898</v>
+        <v>0.25882352941176467</v>
       </c>
       <c r="N19" cm="1">
         <f t="array" aca="1" ref="N19" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K19,translate)</f>
-        <v>0.48436604430873076</v>
+        <v>0.64403642108314141</v>
       </c>
       <c r="O19" cm="1">
         <f t="array" aca="1" ref="O19" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K19,translate)</f>
-        <v>0.30000000000000004</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="20" spans="11:15" x14ac:dyDescent="0.3">
@@ -5196,19 +5213,19 @@
       </c>
       <c r="L20" cm="1">
         <f t="array" aca="1" ref="L20" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K20,translate)</f>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="M20" cm="1">
         <f t="array" aca="1" ref="M20" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K20,translate)</f>
-        <v>0.4138413156747357</v>
+        <v>0.27222222222222225</v>
       </c>
       <c r="N20" cm="1">
         <f t="array" aca="1" ref="N20" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K20,translate)</f>
-        <v>0.47477495402625897</v>
+        <v>0.61262639418441589</v>
       </c>
       <c r="O20" cm="1">
         <f t="array" aca="1" ref="O20" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K20,translate)</f>
-        <v>0.30000000000000004</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="21" spans="11:15" x14ac:dyDescent="0.3">
@@ -5217,19 +5234,19 @@
       </c>
       <c r="L21" cm="1">
         <f t="array" aca="1" ref="L21" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K21,translate)</f>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="M21" cm="1">
         <f t="array" aca="1" ref="M21" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K21,translate)</f>
-        <v>0.40258650958659176</v>
+        <v>0.28421052631578947</v>
       </c>
       <c r="N21" cm="1">
         <f t="array" aca="1" ref="N21" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K21,translate)</f>
-        <v>0.46537378005581476</v>
+        <v>0.58274825237398964</v>
       </c>
       <c r="O21" cm="1">
         <f t="array" aca="1" ref="O21" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K21,translate)</f>
-        <v>0.30000000000000004</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="22" spans="11:15" x14ac:dyDescent="0.3">
@@ -5238,19 +5255,19 @@
       </c>
       <c r="L22" cm="1">
         <f t="array" aca="1" ref="L22" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K22,translate)</f>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="M22" cm="1">
         <f t="array" aca="1" ref="M22" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K22,translate)</f>
-        <v>0.39245718410726216</v>
+        <v>0.29499999999999998</v>
       </c>
       <c r="N22" cm="1">
         <f t="array" aca="1" ref="N22" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K22,translate)</f>
-        <v>0.4561587618024594</v>
+        <v>0.5543272847345071</v>
       </c>
       <c r="O22" cm="1">
         <f t="array" aca="1" ref="O22" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K22,translate)</f>
-        <v>0.30000000000000004</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="23" spans="11:15" x14ac:dyDescent="0.3">
@@ -5259,19 +5276,19 @@
       </c>
       <c r="L23" cm="1">
         <f t="array" aca="1" ref="L23" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K23,translate)</f>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="M23" cm="1">
         <f t="array" aca="1" ref="M23" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K23,translate)</f>
-        <v>0.38805446105453539</v>
+        <v>0.30476190476190473</v>
       </c>
       <c r="N23" cm="1">
         <f t="array" aca="1" ref="N23" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K23,translate)</f>
-        <v>0.44267723298021455</v>
+        <v>0.52729242404304855</v>
       </c>
       <c r="O23" cm="1">
         <f t="array" aca="1" ref="O23" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K23,translate)</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="24" spans="11:15" x14ac:dyDescent="0.3">
@@ -5280,19 +5297,19 @@
       </c>
       <c r="L24" cm="1">
         <f t="array" aca="1" ref="L24" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K24,translate)</f>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="M24" cm="1">
         <f t="array" aca="1" ref="M24" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K24,translate)</f>
-        <v>0.3840519855520565</v>
+        <v>0.3136363636363636</v>
       </c>
       <c r="N24" cm="1">
         <f t="array" aca="1" ref="N24" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K24,translate)</f>
-        <v>0.42959414354926156</v>
+        <v>0.50157606906605556</v>
       </c>
       <c r="O24" cm="1">
         <f t="array" aca="1" ref="O24" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K24,translate)</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="25" spans="11:15" x14ac:dyDescent="0.3">
@@ -5301,19 +5318,19 @@
       </c>
       <c r="L25" cm="1">
         <f t="array" aca="1" ref="L25" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K25,translate)</f>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="M25" cm="1">
         <f t="array" aca="1" ref="M25" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K25,translate)</f>
-        <v>0.38039755139761927</v>
+        <v>0.32173913043478258</v>
       </c>
       <c r="N25" cm="1">
         <f t="array" aca="1" ref="N25" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K25,translate)</f>
-        <v>0.41689771784597751</v>
+        <v>0.47711391552103427</v>
       </c>
       <c r="O25" cm="1">
         <f t="array" aca="1" ref="O25" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K25,translate)</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="26" spans="11:15" x14ac:dyDescent="0.3">
@@ -5322,19 +5339,19 @@
       </c>
       <c r="L26" cm="1">
         <f t="array" aca="1" ref="L26" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K26,translate)</f>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="M26" cm="1">
         <f t="array" aca="1" ref="M26" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K26,translate)</f>
-        <v>0.37704765342271845</v>
+        <v>0.32916666666666661</v>
       </c>
       <c r="N26" cm="1">
         <f t="array" aca="1" ref="N26" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K26,translate)</f>
-        <v>0.40457652823019508</v>
+        <v>0.45384479528235583</v>
       </c>
       <c r="O26" cm="1">
         <f t="array" aca="1" ref="O26" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K26,translate)</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="27" spans="11:15" x14ac:dyDescent="0.3">
@@ -5343,19 +5360,19 @@
       </c>
       <c r="L27" cm="1">
         <f t="array" aca="1" ref="L27" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K27,translate)</f>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="M27" cm="1">
         <f t="array" aca="1" ref="M27" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K27,translate)</f>
-        <v>0.37396574728580972</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="N27" cm="1">
         <f t="array" aca="1" ref="N27" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K27,translate)</f>
-        <v>0.39261948479955472</v>
+        <v>0.43171052342907956</v>
       </c>
       <c r="O27" cm="1">
         <f t="array" aca="1" ref="O27" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K27,translate)</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="28" spans="11:15" x14ac:dyDescent="0.3">
@@ -5364,19 +5381,19 @@
       </c>
       <c r="L28" cm="1">
         <f t="array" aca="1" ref="L28" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K28,translate)</f>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="M28" cm="1">
         <f t="array" aca="1" ref="M28" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K28,translate)</f>
-        <v>0.37112091085174015</v>
+        <v>0.34230769230769231</v>
       </c>
       <c r="N28" cm="1">
         <f t="array" aca="1" ref="N28" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K28,translate)</f>
-        <v>0.38101582540784434</v>
+        <v>0.41065575275234545</v>
       </c>
       <c r="O28" cm="1">
         <f t="array" aca="1" ref="O28" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K28,translate)</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="29" spans="11:15" x14ac:dyDescent="0.3">
@@ -5385,19 +5402,19 @@
       </c>
       <c r="L29" cm="1">
         <f t="array" aca="1" ref="L29" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K29,translate)</f>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="M29" cm="1">
         <f t="array" aca="1" ref="M29" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K29,translate)</f>
-        <v>0.36848680304241643</v>
+        <v>0.3481481481481481</v>
       </c>
       <c r="N29" cm="1">
         <f t="array" aca="1" ref="N29" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K29,translate)</f>
-        <v>0.36975510597834071</v>
+        <v>0.39062783535852114</v>
       </c>
       <c r="O29" cm="1">
         <f t="array" aca="1" ref="O29" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K29,translate)</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="30" spans="11:15" x14ac:dyDescent="0.3">
@@ -5406,19 +5423,19 @@
       </c>
       <c r="L30" cm="1">
         <f t="array" aca="1" ref="L30" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K30,translate)</f>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="M30" cm="1">
         <f t="array" aca="1" ref="M30" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K30,translate)</f>
-        <v>0.36604084579090151</v>
+        <v>0.35357142857142854</v>
       </c>
       <c r="N30" cm="1">
         <f t="array" aca="1" ref="N30" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K30,translate)</f>
-        <v>0.35882719110343608</v>
+        <v>0.3715766910220456</v>
       </c>
       <c r="O30" cm="1">
         <f t="array" aca="1" ref="O30" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K30,translate)</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="31" spans="11:15" x14ac:dyDescent="0.3">
@@ -5427,19 +5444,19 @@
       </c>
       <c r="L31" cm="1">
         <f t="array" aca="1" ref="L31" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(curve,K31,translate)</f>
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="M31" cm="1">
         <f t="array" aca="1" ref="M31" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K31,translate)</f>
-        <v>0.36376357524638764</v>
+        <v>0.35862068965517241</v>
       </c>
       <c r="N31" cm="1">
         <f t="array" aca="1" ref="N31" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K31,translate)</f>
-        <v>0.34822224492208653</v>
+        <v>0.35345468195878016</v>
       </c>
       <c r="O31" cm="1">
         <f t="array" aca="1" ref="O31" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K31,translate)</f>
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="32" spans="11:15" x14ac:dyDescent="0.3">
@@ -5452,11 +5469,11 @@
       </c>
       <c r="M32" cm="1">
         <f t="array" aca="1" ref="M32" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K32,translate)</f>
-        <v>0.36163812273817481</v>
+        <v>0.36333333333333334</v>
       </c>
       <c r="N32" cm="1">
         <f t="array" aca="1" ref="N32" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K32,translate)</f>
-        <v>0.33793072226687343</v>
+        <v>0.33621649370673323</v>
       </c>
       <c r="O32" cm="1">
         <f t="array" aca="1" ref="O32" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K32,translate)</f>
@@ -5473,11 +5490,11 @@
       </c>
       <c r="M33" cm="1">
         <f t="array" aca="1" ref="M33" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K33,translate)</f>
-        <v>0.3661014091014595</v>
+        <v>0.36774193548387096</v>
       </c>
       <c r="N33" cm="1">
         <f t="array" aca="1" ref="N33" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K33,translate)</f>
-        <v>0.3214496464630287</v>
+        <v>0.31981902181630384</v>
       </c>
       <c r="O33" cm="1">
         <f t="array" aca="1" ref="O33" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K33,translate)</f>
@@ -5494,11 +5511,11 @@
       </c>
       <c r="M34" cm="1">
         <f t="array" aca="1" ref="M34" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K34,translate)</f>
-        <v>0.37028574006703885</v>
+        <v>0.37187499999999996</v>
       </c>
       <c r="N34" cm="1">
         <f t="array" aca="1" ref="N34" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K34,translate)</f>
-        <v>0.30577236221098475</v>
+        <v>0.30422126406670408</v>
       </c>
       <c r="O34" cm="1">
         <f t="array" aca="1" ref="O34" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K34,translate)</f>
@@ -5515,11 +5532,11 @@
       </c>
       <c r="M35" cm="1">
         <f t="array" aca="1" ref="M35" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K35,translate)</f>
-        <v>0.37421647521652257</v>
+        <v>0.37575757575757573</v>
       </c>
       <c r="N35" cm="1">
         <f t="array" aca="1" ref="N35" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K35,translate)</f>
-        <v>0.29085966813417891</v>
+        <v>0.28938421793905056</v>
       </c>
       <c r="O35" cm="1">
         <f t="array" aca="1" ref="O35" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K35,translate)</f>
@@ -5536,11 +5553,11 @@
       </c>
       <c r="M36" cm="1">
         <f t="array" aca="1" ref="M36" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K36,translate)</f>
-        <v>0.37791599065133069</v>
+        <v>0.37941176470588234</v>
       </c>
       <c r="N36" cm="1">
         <f t="array" aca="1" ref="N36" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K36,translate)</f>
-        <v>0.27667427472974365</v>
+        <v>0.27527078308975234</v>
       </c>
       <c r="O36" cm="1">
         <f t="array" aca="1" ref="O36" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K36,translate)</f>
@@ -5557,11 +5574,11 @@
       </c>
       <c r="M37" cm="1">
         <f t="array" aca="1" ref="M37" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K37,translate)</f>
-        <v>0.38140410520414986</v>
+        <v>0.38285714285714284</v>
       </c>
       <c r="N37" cm="1">
         <f t="array" aca="1" ref="N37" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K37,translate)</f>
-        <v>0.26318071112532648</v>
+        <v>0.26184566858032593</v>
       </c>
       <c r="O37" cm="1">
         <f t="array" aca="1" ref="O37" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K37,translate)</f>
@@ -5578,11 +5595,11 @@
       </c>
       <c r="M38" cm="1">
         <f t="array" aca="1" ref="M38" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K38,translate)</f>
-        <v>0.38469843561514566</v>
+        <v>0.38611111111111107</v>
       </c>
       <c r="N38" cm="1">
         <f t="array" aca="1" ref="N38" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K38,translate)</f>
-        <v>0.25034523638343303</v>
+        <v>0.24907530463166816</v>
       </c>
       <c r="O38" cm="1">
         <f t="array" aca="1" ref="O38" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K38,translate)</f>
@@ -5599,11 +5616,11 @@
       </c>
       <c r="M39" cm="1">
         <f t="array" aca="1" ref="M39" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K39,translate)</f>
-        <v>0.38781469411203362</v>
+        <v>0.38918918918918916</v>
       </c>
       <c r="N39" cm="1">
         <f t="array" aca="1" ref="N39" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K39,translate)</f>
-        <v>0.23813575513150817</v>
+        <v>0.23692775868212176</v>
       </c>
       <c r="O39" cm="1">
         <f t="array" aca="1" ref="O39" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K39,translate)</f>
@@ -5620,11 +5637,11 @@
       </c>
       <c r="M40" cm="1">
         <f t="array" aca="1" ref="M40" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K40,translate)</f>
-        <v>0.3907669390038222</v>
+        <v>0.39210526315789473</v>
       </c>
       <c r="N40" cm="1">
         <f t="array" aca="1" ref="N40" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K40,translate)</f>
-        <v>0.22652173730678746</v>
+        <v>0.22537265553943867</v>
       </c>
       <c r="O40" cm="1">
         <f t="array" aca="1" ref="O40" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K40,translate)</f>
@@ -5641,11 +5658,11 @@
       </c>
       <c r="M41" cm="1">
         <f t="array" aca="1" ref="M41" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K41,translate)</f>
-        <v>0.39356778672167292</v>
+        <v>0.39487179487179486</v>
       </c>
       <c r="N41" cm="1">
         <f t="array" aca="1" ref="N41" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K41,translate)</f>
-        <v>0.21547414181523736</v>
+        <v>0.21438110142697794</v>
       </c>
       <c r="O41" cm="1">
         <f t="array" aca="1" ref="O41" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K41,translate)</f>
@@ -5662,11 +5679,11 @@
       </c>
       <c r="M42" cm="1">
         <f t="array" aca="1" ref="M42" ca="1">_xll.TMX.PWFLAT.CURVE.YIELD(curve,K42,translate)</f>
-        <v>0.39622859205363109</v>
+        <v>0.39749999999999996</v>
       </c>
       <c r="N42" cm="1">
         <f t="array" aca="1" ref="N42" ca="1">_xll.TMX.PWFLAT.CURVE.DISCOUNT(curve,K42,translate)</f>
-        <v>0.2049653439136935</v>
+        <v>0.20392561173421347</v>
       </c>
       <c r="O42" cm="1">
         <f t="array" aca="1" ref="O42" ca="1">_xll.TMX.PWFLAT.CURVE.FORWARD(shift,K42,translate)</f>
@@ -5683,7 +5700,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A8A3DD8-75E7-4A72-9366-AF366CC35FAC}">
   <dimension ref="B1:I553"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5711,7 +5730,7 @@
       </c>
       <c r="E2" s="4" cm="1">
         <f t="array" ref="E2">_xll.\TMX.BOND.SIMPLE(D2,D3,D4,D5)</f>
-        <v>2047199131520</v>
+        <v>1522377567984</v>
       </c>
       <c r="F2" s="25" cm="1">
         <f t="array" ref="F2:F5">_xll.TMX.BOND.SIMPLE(E2)</f>
@@ -5766,10 +5785,10 @@
         <v>26</v>
       </c>
       <c r="D5" s="28">
-        <v>140716601127980</v>
+        <v>140716816282658</v>
       </c>
       <c r="F5" s="28">
-        <v>140716601127980</v>
+        <v>140716816282658</v>
       </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
@@ -5782,7 +5801,7 @@
       </c>
       <c r="C6" s="4" cm="1">
         <f t="array" ref="C6">_xll.\TMX.BOND.SIMPLE(maturity, coupon, _xll.ENUM(frequency), _xll.ENUM(day_count))</f>
-        <v>2047199127008</v>
+        <v>1522377564336</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
@@ -5791,9 +5810,8 @@
       </c>
       <c r="C7" s="2">
         <f ca="1">TODAY()</f>
-        <v>45114</v>
-      </c>
-      <c r="D7" s="31"/>
+        <v>45115</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="9" t="s">
@@ -5801,7 +5819,7 @@
       </c>
       <c r="C8" s="4" cm="1">
         <f t="array" aca="1" ref="C8" ca="1">_xll.\TMX.BOND.INSTRUMENT(bond.simple, dated)</f>
-        <v>2046831277168</v>
+        <v>1522057180544</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
@@ -5814,7 +5832,7 @@
       </c>
       <c r="D9" s="4" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">_xll.\TMX.PWFLAT.CURVE(0,0,yield)</f>
-        <v>2046831271712</v>
+        <v>1522057176672</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
@@ -5917,7 +5935,7 @@
       </c>
       <c r="E16" s="2" cm="1">
         <f t="array" aca="1" ref="E16:E25" ca="1">_xlfn.MAP(time,_xlfn.LAMBDA(_xlpm.t,_xll.TMX.DATE.ADD_YEARS(dated,_xlpm.t)))</f>
-        <v>45298</v>
+        <v>45299</v>
       </c>
       <c r="F16" s="15" cm="1">
         <f t="array" aca="1" ref="F16:F25" ca="1">_xlfn.MAP(time,_xlfn.LAMBDA(_xlpm.t, _xll.TMX.PWFLAT.CURVE.DISCOUNT($D$9, _xlpm.t)))</f>
@@ -5947,7 +5965,7 @@
       </c>
       <c r="E17" s="2">
         <f ca="1"/>
-        <v>45480</v>
+        <v>45481</v>
       </c>
       <c r="F17" s="15">
         <f ca="1"/>
@@ -5977,7 +5995,7 @@
       </c>
       <c r="E18" s="2">
         <f ca="1"/>
-        <v>45664</v>
+        <v>45665</v>
       </c>
       <c r="F18" s="15">
         <f ca="1"/>
@@ -6007,7 +6025,7 @@
       </c>
       <c r="E19" s="2">
         <f ca="1"/>
-        <v>45844.999988425923</v>
+        <v>45845.999988425923</v>
       </c>
       <c r="F19" s="15">
         <f ca="1"/>
@@ -6037,7 +6055,7 @@
       </c>
       <c r="E20" s="2">
         <f ca="1"/>
-        <v>46029</v>
+        <v>46030</v>
       </c>
       <c r="F20" s="15">
         <f ca="1"/>
@@ -6067,7 +6085,7 @@
       </c>
       <c r="E21" s="2">
         <f ca="1"/>
-        <v>46210</v>
+        <v>46211</v>
       </c>
       <c r="F21" s="15">
         <f ca="1"/>
@@ -6097,7 +6115,7 @@
       </c>
       <c r="E22" s="2">
         <f ca="1"/>
-        <v>46394</v>
+        <v>46395</v>
       </c>
       <c r="F22" s="15">
         <f ca="1"/>
@@ -6127,7 +6145,7 @@
       </c>
       <c r="E23" s="2">
         <f ca="1"/>
-        <v>46575</v>
+        <v>46576</v>
       </c>
       <c r="F23" s="15">
         <f ca="1"/>
@@ -6157,7 +6175,7 @@
       </c>
       <c r="E24" s="2">
         <f ca="1"/>
-        <v>46759</v>
+        <v>46760</v>
       </c>
       <c r="F24" s="15">
         <f ca="1"/>
@@ -6187,7 +6205,7 @@
       </c>
       <c r="E25" s="2">
         <f ca="1"/>
-        <v>46941</v>
+        <v>46942</v>
       </c>
       <c r="F25" s="15">
         <f ca="1"/>
@@ -8885,15 +8903,15 @@
       </c>
       <c r="E5" s="4" cm="1">
         <f t="array" ref="E5">_xll.\TMX.BOND.SIMPLE(B5, C5)</f>
-        <v>2046729851696</v>
+        <v>1522377567120</v>
       </c>
       <c r="F5" s="4" cm="1">
         <f t="array" ref="F5">_xll.\TMX.BOND.INSTRUMENT(E5, dated)</f>
-        <v>2046721694800</v>
+        <v>1522383929520</v>
       </c>
       <c r="G5" s="4" cm="1">
         <f t="array" aca="1" ref="G5" ca="1">_xll.\TMX.BOOTSTRAP.CURVE(instrument, price)</f>
-        <v>2046831283328</v>
+        <v>1522057176848</v>
       </c>
       <c r="H5" cm="1">
         <f t="array" ref="H5:H105">_xll.ARRAY.SEQUENCE(0,10,H3)</f>
@@ -8901,7 +8919,7 @@
       </c>
       <c r="I5" s="20" cm="1">
         <f t="array" aca="1" ref="I5:I105" ca="1">_xlfn.MAP(_xlfn.ANCHORARRAY(H5),_xlfn.LAMBDA(_xlpm.t,_xll.TMX.PWFLAT.CURVE.FORWARD(curve,_xlpm.t)))</f>
-        <v>4.9283011639120938E-2</v>
+        <v>4.9283013956455027E-2</v>
       </c>
       <c r="J5" s="2"/>
       <c r="R5" s="21"/>
@@ -8913,25 +8931,25 @@
       </c>
       <c r="C6" s="17">
         <f ca="1">0.05 + 0.01*RAND() - 0.005</f>
-        <v>5.1083037526668477E-2</v>
+        <v>4.550141789351856E-2</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
       </c>
       <c r="E6" s="4" cm="1">
         <f t="array" aca="1" ref="E6" ca="1">_xll.\TMX.BOND.SIMPLE(B6, C6)</f>
-        <v>2047191942656</v>
+        <v>1522054607520</v>
       </c>
       <c r="F6" s="4" cm="1">
         <f t="array" aca="1" ref="F6" ca="1">_xll.\TMX.BOND.INSTRUMENT(E6, dated)</f>
-        <v>2046831271536</v>
+        <v>1522057183888</v>
       </c>
       <c r="H6">
         <v>0.1</v>
       </c>
       <c r="I6" s="19">
         <f ca="1"/>
-        <v>4.9283011639120938E-2</v>
+        <v>4.9283013956455027E-2</v>
       </c>
       <c r="R6" s="21"/>
       <c r="S6" s="21"/>
@@ -8948,18 +8966,18 @@
       </c>
       <c r="E7" s="4" cm="1">
         <f t="array" ref="E7">_xll.\TMX.BOND.SIMPLE(B7, C7)</f>
-        <v>2046729853328</v>
+        <v>1522377504528</v>
       </c>
       <c r="F7" s="4" cm="1">
         <f t="array" ref="F7">_xll.\TMX.BOND.INSTRUMENT(E7, dated)</f>
-        <v>2046721691808</v>
+        <v>1522383934976</v>
       </c>
       <c r="H7">
         <v>0.2</v>
       </c>
       <c r="I7" s="19">
         <f ca="1"/>
-        <v>4.9283011639120938E-2</v>
+        <v>4.9283013956455027E-2</v>
       </c>
       <c r="R7" s="21"/>
       <c r="S7" s="21"/>
@@ -8976,18 +8994,18 @@
       </c>
       <c r="E8" s="4" cm="1">
         <f t="array" ref="E8">_xll.\TMX.BOND.SIMPLE(B8, C8)</f>
-        <v>2046729853520</v>
+        <v>1522377567312</v>
       </c>
       <c r="F8" s="4" cm="1">
         <f t="array" ref="F8">_xll.\TMX.BOND.INSTRUMENT(E8, dated)</f>
-        <v>2046721691632</v>
+        <v>1522383939728</v>
       </c>
       <c r="H8">
         <v>0.30000000000000004</v>
       </c>
       <c r="I8" s="19">
         <f ca="1"/>
-        <v>4.9283011639120938E-2</v>
+        <v>4.9283013956455027E-2</v>
       </c>
       <c r="R8" s="21"/>
       <c r="S8" s="21"/>
@@ -9004,18 +9022,18 @@
       </c>
       <c r="E9" s="4" cm="1">
         <f t="array" ref="E9">_xll.\TMX.BOND.SIMPLE(B9, C9)</f>
-        <v>2046729854672</v>
+        <v>1522377568176</v>
       </c>
       <c r="F9" s="4" cm="1">
         <f t="array" ref="F9">_xll.\TMX.BOND.INSTRUMENT(E9, dated)</f>
-        <v>2046721692336</v>
+        <v>1522383938848</v>
       </c>
       <c r="H9">
         <v>0.4</v>
       </c>
       <c r="I9" s="19">
         <f ca="1"/>
-        <v>4.9283011639120938E-2</v>
+        <v>4.9283013956455027E-2</v>
       </c>
       <c r="R9" s="21"/>
       <c r="S9" s="21"/>
@@ -9032,18 +9050,18 @@
       </c>
       <c r="E10" s="4" cm="1">
         <f t="array" ref="E10">_xll.\TMX.BOND.SIMPLE(B10, C10)</f>
-        <v>2046729854768</v>
+        <v>1522377504912</v>
       </c>
       <c r="F10" s="4" cm="1">
         <f t="array" ref="F10">_xll.\TMX.BOND.INSTRUMENT(E10, dated)</f>
-        <v>2046721695152</v>
+        <v>1522383936560</v>
       </c>
       <c r="H10">
         <v>0.5</v>
       </c>
       <c r="I10" s="19">
         <f ca="1"/>
-        <v>4.9283011639120938E-2</v>
+        <v>4.9283013956455027E-2</v>
       </c>
       <c r="R10" s="21"/>
       <c r="S10" s="21"/>
@@ -9060,18 +9078,18 @@
       </c>
       <c r="E11" s="4" cm="1">
         <f t="array" ref="E11">_xll.\TMX.BOND.SIMPLE(B11, C11)</f>
-        <v>2046729853712</v>
+        <v>1522377566640</v>
       </c>
       <c r="F11" s="4" cm="1">
         <f t="array" ref="F11">_xll.\TMX.BOND.INSTRUMENT(E11, dated)</f>
-        <v>2046721693920</v>
+        <v>1522383930048</v>
       </c>
       <c r="H11">
         <v>0.60000000000000009</v>
       </c>
       <c r="I11" s="19">
         <f ca="1"/>
-        <v>4.9283011639120938E-2</v>
+        <v>4.9283013956455027E-2</v>
       </c>
       <c r="R11" s="21"/>
       <c r="S11" s="21"/>
@@ -9088,18 +9106,18 @@
       </c>
       <c r="E12" s="4" cm="1">
         <f t="array" ref="E12">_xll.\TMX.BOND.SIMPLE(B12, C12)</f>
-        <v>2046729853616</v>
+        <v>1522377508464</v>
       </c>
       <c r="F12" s="4" cm="1">
         <f t="array" ref="F12">_xll.\TMX.BOND.INSTRUMENT(E12, dated)</f>
-        <v>2046721696208</v>
+        <v>1522383939024</v>
       </c>
       <c r="H12">
         <v>0.70000000000000007</v>
       </c>
       <c r="I12" s="19">
         <f ca="1"/>
-        <v>4.9283011639120938E-2</v>
+        <v>4.9283013956455027E-2</v>
       </c>
       <c r="R12" s="21"/>
       <c r="S12" s="21"/>
@@ -9116,18 +9134,18 @@
       </c>
       <c r="E13" s="4" cm="1">
         <f t="array" ref="E13">_xll.\TMX.BOND.SIMPLE(B13, C13)</f>
-        <v>2046729854480</v>
+        <v>1522377504432</v>
       </c>
       <c r="F13" s="4" cm="1">
         <f t="array" ref="F13">_xll.\TMX.BOND.INSTRUMENT(E13, dated)</f>
-        <v>2046721696032</v>
+        <v>1522383930400</v>
       </c>
       <c r="H13">
         <v>0.8</v>
       </c>
       <c r="I13" s="19">
         <f ca="1"/>
-        <v>4.9283011639120938E-2</v>
+        <v>4.9283013956455027E-2</v>
       </c>
       <c r="R13" s="21"/>
       <c r="S13" s="21"/>
@@ -9144,18 +9162,18 @@
       </c>
       <c r="E14" s="4" cm="1">
         <f t="array" ref="E14">_xll.\TMX.BOND.SIMPLE(B14, C14)</f>
-        <v>2046729853424</v>
+        <v>1522377505392</v>
       </c>
       <c r="F14" s="4" cm="1">
         <f t="array" ref="F14">_xll.\TMX.BOND.INSTRUMENT(E14, dated)</f>
-        <v>2046721691456</v>
+        <v>1522383930928</v>
       </c>
       <c r="H14">
         <v>0.9</v>
       </c>
       <c r="I14" s="19">
         <f ca="1"/>
-        <v>4.9283011639120938E-2</v>
+        <v>4.9283013956455027E-2</v>
       </c>
       <c r="R14" s="21"/>
       <c r="S14" s="21"/>
@@ -9166,7 +9184,7 @@
       </c>
       <c r="I15" s="19">
         <f ca="1"/>
-        <v>4.9283011639120938E-2</v>
+        <v>4.9283013956455027E-2</v>
       </c>
       <c r="R15" s="21"/>
       <c r="S15" s="21"/>
@@ -9178,7 +9196,7 @@
       </c>
       <c r="I16" s="19">
         <f ca="1"/>
-        <v>5.1585054314548233E-2</v>
+        <v>4.04216230000293E-2</v>
       </c>
     </row>
     <row r="17" spans="8:9" x14ac:dyDescent="0.3">
@@ -9187,7 +9205,7 @@
       </c>
       <c r="I17" s="19">
         <f ca="1"/>
-        <v>5.1585054314548233E-2</v>
+        <v>4.04216230000293E-2</v>
       </c>
     </row>
     <row r="18" spans="8:9" x14ac:dyDescent="0.3">
@@ -9196,7 +9214,7 @@
       </c>
       <c r="I18" s="19">
         <f ca="1"/>
-        <v>5.1585054314548233E-2</v>
+        <v>4.04216230000293E-2</v>
       </c>
     </row>
     <row r="19" spans="8:9" x14ac:dyDescent="0.3">
@@ -9205,7 +9223,7 @@
       </c>
       <c r="I19" s="19">
         <f ca="1"/>
-        <v>5.1585054314548233E-2</v>
+        <v>4.04216230000293E-2</v>
       </c>
     </row>
     <row r="20" spans="8:9" x14ac:dyDescent="0.3">
@@ -9214,7 +9232,7 @@
       </c>
       <c r="I20" s="19">
         <f ca="1"/>
-        <v>5.1585054314548233E-2</v>
+        <v>4.04216230000293E-2</v>
       </c>
     </row>
     <row r="21" spans="8:9" x14ac:dyDescent="0.3">
@@ -9223,7 +9241,7 @@
       </c>
       <c r="I21" s="19">
         <f ca="1"/>
-        <v>5.1585054314548233E-2</v>
+        <v>4.04216230000293E-2</v>
       </c>
     </row>
     <row r="22" spans="8:9" x14ac:dyDescent="0.3">
@@ -9232,7 +9250,7 @@
       </c>
       <c r="I22" s="19">
         <f ca="1"/>
-        <v>5.1585054314548233E-2</v>
+        <v>4.04216230000293E-2</v>
       </c>
     </row>
     <row r="23" spans="8:9" x14ac:dyDescent="0.3">
@@ -9241,7 +9259,7 @@
       </c>
       <c r="I23" s="19">
         <f ca="1"/>
-        <v>5.1585054314548233E-2</v>
+        <v>4.04216230000293E-2</v>
       </c>
     </row>
     <row r="24" spans="8:9" x14ac:dyDescent="0.3">
@@ -9250,7 +9268,7 @@
       </c>
       <c r="I24" s="19">
         <f ca="1"/>
-        <v>5.1585054314548233E-2</v>
+        <v>4.04216230000293E-2</v>
       </c>
     </row>
     <row r="25" spans="8:9" x14ac:dyDescent="0.3">
@@ -9259,7 +9277,7 @@
       </c>
       <c r="I25" s="19">
         <f ca="1"/>
-        <v>5.1585054314548233E-2</v>
+        <v>4.04216230000293E-2</v>
       </c>
     </row>
     <row r="26" spans="8:9" x14ac:dyDescent="0.3">
@@ -9268,7 +9286,7 @@
       </c>
       <c r="I26" s="19">
         <f ca="1"/>
-        <v>4.7137984858476464E-2</v>
+        <v>5.8868051747390009E-2</v>
       </c>
     </row>
     <row r="27" spans="8:9" x14ac:dyDescent="0.3">
@@ -9277,7 +9295,7 @@
       </c>
       <c r="I27" s="19">
         <f ca="1"/>
-        <v>4.7137984858476464E-2</v>
+        <v>5.8868051747390009E-2</v>
       </c>
     </row>
     <row r="28" spans="8:9" x14ac:dyDescent="0.3">
@@ -9286,7 +9304,7 @@
       </c>
       <c r="I28" s="19">
         <f ca="1"/>
-        <v>4.7137984858476464E-2</v>
+        <v>5.8868051747390009E-2</v>
       </c>
     </row>
     <row r="29" spans="8:9" x14ac:dyDescent="0.3">
@@ -9295,7 +9313,7 @@
       </c>
       <c r="I29" s="19">
         <f ca="1"/>
-        <v>4.7137984858476464E-2</v>
+        <v>5.8868051747390009E-2</v>
       </c>
     </row>
     <row r="30" spans="8:9" x14ac:dyDescent="0.3">
@@ -9304,7 +9322,7 @@
       </c>
       <c r="I30" s="19">
         <f ca="1"/>
-        <v>4.7137984858476464E-2</v>
+        <v>5.8868051747390009E-2</v>
       </c>
     </row>
     <row r="31" spans="8:9" x14ac:dyDescent="0.3">
@@ -9313,7 +9331,7 @@
       </c>
       <c r="I31" s="19">
         <f ca="1"/>
-        <v>4.7137984858476464E-2</v>
+        <v>5.8868051747390009E-2</v>
       </c>
     </row>
     <row r="32" spans="8:9" x14ac:dyDescent="0.3">
@@ -9322,7 +9340,7 @@
       </c>
       <c r="I32" s="19">
         <f ca="1"/>
-        <v>4.7137984858476464E-2</v>
+        <v>5.8868051747390009E-2</v>
       </c>
     </row>
     <row r="33" spans="8:9" x14ac:dyDescent="0.3">
@@ -9331,7 +9349,7 @@
       </c>
       <c r="I33" s="19">
         <f ca="1"/>
-        <v>4.7137984858476464E-2</v>
+        <v>5.8868051747390009E-2</v>
       </c>
     </row>
     <row r="34" spans="8:9" x14ac:dyDescent="0.3">
@@ -9340,7 +9358,7 @@
       </c>
       <c r="I34" s="19">
         <f ca="1"/>
-        <v>4.7137984858476464E-2</v>
+        <v>5.8868051747390009E-2</v>
       </c>
     </row>
     <row r="35" spans="8:9" x14ac:dyDescent="0.3">
@@ -9349,7 +9367,7 @@
       </c>
       <c r="I35" s="19">
         <f ca="1"/>
-        <v>4.7137984858476464E-2</v>
+        <v>5.8868051747390009E-2</v>
       </c>
     </row>
     <row r="36" spans="8:9" x14ac:dyDescent="0.3">
@@ -9358,7 +9376,7 @@
       </c>
       <c r="I36" s="19">
         <f ca="1"/>
-        <v>4.9416364517221215E-2</v>
+        <v>4.9416393249193918E-2</v>
       </c>
     </row>
     <row r="37" spans="8:9" x14ac:dyDescent="0.3">
@@ -9367,7 +9385,7 @@
       </c>
       <c r="I37" s="19">
         <f ca="1"/>
-        <v>4.9416364517221215E-2</v>
+        <v>4.9416393249193918E-2</v>
       </c>
     </row>
     <row r="38" spans="8:9" x14ac:dyDescent="0.3">
@@ -9376,7 +9394,7 @@
       </c>
       <c r="I38" s="19">
         <f ca="1"/>
-        <v>4.9416364517221215E-2</v>
+        <v>4.9416393249193918E-2</v>
       </c>
     </row>
     <row r="39" spans="8:9" x14ac:dyDescent="0.3">
@@ -9385,7 +9403,7 @@
       </c>
       <c r="I39" s="19">
         <f ca="1"/>
-        <v>4.9416364517221215E-2</v>
+        <v>4.9416393249193918E-2</v>
       </c>
     </row>
     <row r="40" spans="8:9" x14ac:dyDescent="0.3">
@@ -9394,7 +9412,7 @@
       </c>
       <c r="I40" s="19">
         <f ca="1"/>
-        <v>4.9416364517221215E-2</v>
+        <v>4.9416393249193918E-2</v>
       </c>
     </row>
     <row r="41" spans="8:9" x14ac:dyDescent="0.3">
@@ -9403,7 +9421,7 @@
       </c>
       <c r="I41" s="19">
         <f ca="1"/>
-        <v>4.9416364517221215E-2</v>
+        <v>4.9416393249193918E-2</v>
       </c>
     </row>
     <row r="42" spans="8:9" x14ac:dyDescent="0.3">
@@ -9412,7 +9430,7 @@
       </c>
       <c r="I42" s="19">
         <f ca="1"/>
-        <v>4.9416364517221215E-2</v>
+        <v>4.9416393249193918E-2</v>
       </c>
     </row>
     <row r="43" spans="8:9" x14ac:dyDescent="0.3">
@@ -9421,7 +9439,7 @@
       </c>
       <c r="I43" s="19">
         <f ca="1"/>
-        <v>4.9416364517221215E-2</v>
+        <v>4.9416393249193918E-2</v>
       </c>
     </row>
     <row r="44" spans="8:9" x14ac:dyDescent="0.3">
@@ -9430,7 +9448,7 @@
       </c>
       <c r="I44" s="19">
         <f ca="1"/>
-        <v>4.9416364517221215E-2</v>
+        <v>4.9416393249193918E-2</v>
       </c>
     </row>
     <row r="45" spans="8:9" x14ac:dyDescent="0.3">
@@ -9439,7 +9457,7 @@
       </c>
       <c r="I45" s="19">
         <f ca="1"/>
-        <v>4.9416364517221215E-2</v>
+        <v>4.9416393249193918E-2</v>
       </c>
     </row>
     <row r="46" spans="8:9" x14ac:dyDescent="0.3">
@@ -9448,7 +9466,7 @@
       </c>
       <c r="I46" s="19">
         <f ca="1"/>
-        <v>4.9283017362953575E-2</v>
+        <v>4.928301622797935E-2</v>
       </c>
     </row>
     <row r="47" spans="8:9" x14ac:dyDescent="0.3">
@@ -9457,7 +9475,7 @@
       </c>
       <c r="I47" s="19">
         <f ca="1"/>
-        <v>4.9283017362953575E-2</v>
+        <v>4.928301622797935E-2</v>
       </c>
     </row>
     <row r="48" spans="8:9" x14ac:dyDescent="0.3">
@@ -9466,7 +9484,7 @@
       </c>
       <c r="I48" s="19">
         <f ca="1"/>
-        <v>4.9283017362953575E-2</v>
+        <v>4.928301622797935E-2</v>
       </c>
     </row>
     <row r="49" spans="8:9" x14ac:dyDescent="0.3">
@@ -9475,7 +9493,7 @@
       </c>
       <c r="I49" s="19">
         <f ca="1"/>
-        <v>4.9283017362953575E-2</v>
+        <v>4.928301622797935E-2</v>
       </c>
     </row>
     <row r="50" spans="8:9" x14ac:dyDescent="0.3">
@@ -9484,7 +9502,7 @@
       </c>
       <c r="I50" s="19">
         <f ca="1"/>
-        <v>4.9283017362953575E-2</v>
+        <v>4.928301622797935E-2</v>
       </c>
     </row>
     <row r="51" spans="8:9" x14ac:dyDescent="0.3">
@@ -9493,7 +9511,7 @@
       </c>
       <c r="I51" s="19">
         <f ca="1"/>
-        <v>4.9283017362953575E-2</v>
+        <v>4.928301622797935E-2</v>
       </c>
     </row>
     <row r="52" spans="8:9" x14ac:dyDescent="0.3">
@@ -9502,7 +9520,7 @@
       </c>
       <c r="I52" s="19">
         <f ca="1"/>
-        <v>4.9283017362953575E-2</v>
+        <v>4.928301622797935E-2</v>
       </c>
     </row>
     <row r="53" spans="8:9" x14ac:dyDescent="0.3">
@@ -9511,7 +9529,7 @@
       </c>
       <c r="I53" s="19">
         <f ca="1"/>
-        <v>4.9283017362953575E-2</v>
+        <v>4.928301622797935E-2</v>
       </c>
     </row>
     <row r="54" spans="8:9" x14ac:dyDescent="0.3">
@@ -9520,7 +9538,7 @@
       </c>
       <c r="I54" s="19">
         <f ca="1"/>
-        <v>4.9283017362953575E-2</v>
+        <v>4.928301622797935E-2</v>
       </c>
     </row>
     <row r="55" spans="8:9" x14ac:dyDescent="0.3">
@@ -9529,7 +9547,7 @@
       </c>
       <c r="I55" s="19">
         <f ca="1"/>
-        <v>4.9283017362953575E-2</v>
+        <v>4.928301622797935E-2</v>
       </c>
     </row>
     <row r="56" spans="8:9" x14ac:dyDescent="0.3">
@@ -9538,7 +9556,7 @@
       </c>
       <c r="I56" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.941632836041359E-2</v>
       </c>
     </row>
     <row r="57" spans="8:9" x14ac:dyDescent="0.3">
@@ -9547,7 +9565,7 @@
       </c>
       <c r="I57" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.941632836041359E-2</v>
       </c>
     </row>
     <row r="58" spans="8:9" x14ac:dyDescent="0.3">
@@ -9556,7 +9574,7 @@
       </c>
       <c r="I58" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.941632836041359E-2</v>
       </c>
     </row>
     <row r="59" spans="8:9" x14ac:dyDescent="0.3">
@@ -9565,7 +9583,7 @@
       </c>
       <c r="I59" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.941632836041359E-2</v>
       </c>
     </row>
     <row r="60" spans="8:9" x14ac:dyDescent="0.3">
@@ -9574,7 +9592,7 @@
       </c>
       <c r="I60" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.941632836041359E-2</v>
       </c>
     </row>
     <row r="61" spans="8:9" x14ac:dyDescent="0.3">
@@ -9583,7 +9601,7 @@
       </c>
       <c r="I61" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.941632836041359E-2</v>
       </c>
     </row>
     <row r="62" spans="8:9" x14ac:dyDescent="0.3">
@@ -9592,7 +9610,7 @@
       </c>
       <c r="I62" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.941632836041359E-2</v>
       </c>
     </row>
     <row r="63" spans="8:9" x14ac:dyDescent="0.3">
@@ -9601,7 +9619,7 @@
       </c>
       <c r="I63" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.941632836041359E-2</v>
       </c>
     </row>
     <row r="64" spans="8:9" x14ac:dyDescent="0.3">
@@ -9610,7 +9628,7 @@
       </c>
       <c r="I64" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.941632836041359E-2</v>
       </c>
     </row>
     <row r="65" spans="8:9" x14ac:dyDescent="0.3">
@@ -9619,7 +9637,7 @@
       </c>
       <c r="I65" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.941632836041359E-2</v>
       </c>
     </row>
     <row r="66" spans="8:9" x14ac:dyDescent="0.3">
@@ -9628,7 +9646,7 @@
       </c>
       <c r="I66" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="67" spans="8:9" x14ac:dyDescent="0.3">
@@ -9637,7 +9655,7 @@
       </c>
       <c r="I67" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="68" spans="8:9" x14ac:dyDescent="0.3">
@@ -9646,7 +9664,7 @@
       </c>
       <c r="I68" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="69" spans="8:9" x14ac:dyDescent="0.3">
@@ -9655,7 +9673,7 @@
       </c>
       <c r="I69" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="70" spans="8:9" x14ac:dyDescent="0.3">
@@ -9664,7 +9682,7 @@
       </c>
       <c r="I70" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="71" spans="8:9" x14ac:dyDescent="0.3">
@@ -9673,7 +9691,7 @@
       </c>
       <c r="I71" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="72" spans="8:9" x14ac:dyDescent="0.3">
@@ -9682,7 +9700,7 @@
       </c>
       <c r="I72" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="73" spans="8:9" x14ac:dyDescent="0.3">
@@ -9691,7 +9709,7 @@
       </c>
       <c r="I73" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="74" spans="8:9" x14ac:dyDescent="0.3">
@@ -9700,7 +9718,7 @@
       </c>
       <c r="I74" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="75" spans="8:9" x14ac:dyDescent="0.3">
@@ -9709,7 +9727,7 @@
       </c>
       <c r="I75" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="76" spans="8:9" x14ac:dyDescent="0.3">
@@ -9718,7 +9736,7 @@
       </c>
       <c r="I76" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="77" spans="8:9" x14ac:dyDescent="0.3">
@@ -9727,7 +9745,7 @@
       </c>
       <c r="I77" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="78" spans="8:9" x14ac:dyDescent="0.3">
@@ -9736,7 +9754,7 @@
       </c>
       <c r="I78" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="79" spans="8:9" x14ac:dyDescent="0.3">
@@ -9745,7 +9763,7 @@
       </c>
       <c r="I79" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="80" spans="8:9" x14ac:dyDescent="0.3">
@@ -9754,7 +9772,7 @@
       </c>
       <c r="I80" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="81" spans="8:9" x14ac:dyDescent="0.3">
@@ -9763,7 +9781,7 @@
       </c>
       <c r="I81" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="82" spans="8:9" x14ac:dyDescent="0.3">
@@ -9772,7 +9790,7 @@
       </c>
       <c r="I82" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="83" spans="8:9" x14ac:dyDescent="0.3">
@@ -9781,7 +9799,7 @@
       </c>
       <c r="I83" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="84" spans="8:9" x14ac:dyDescent="0.3">
@@ -9790,7 +9808,7 @@
       </c>
       <c r="I84" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="85" spans="8:9" x14ac:dyDescent="0.3">
@@ -9799,7 +9817,7 @@
       </c>
       <c r="I85" s="19">
         <f ca="1"/>
-        <v>4.9416357720749815E-2</v>
+        <v>4.9416364453131766E-2</v>
       </c>
     </row>
     <row r="86" spans="8:9" x14ac:dyDescent="0.3">
@@ -9808,7 +9826,7 @@
       </c>
       <c r="I86" s="19">
         <f ca="1"/>
-        <v>4.9283035687621969E-2</v>
+        <v>4.928305695371818E-2</v>
       </c>
     </row>
     <row r="87" spans="8:9" x14ac:dyDescent="0.3">
@@ -9817,7 +9835,7 @@
       </c>
       <c r="I87" s="19">
         <f ca="1"/>
-        <v>4.9283035687621969E-2</v>
+        <v>4.928305695371818E-2</v>
       </c>
     </row>
     <row r="88" spans="8:9" x14ac:dyDescent="0.3">
@@ -9826,7 +9844,7 @@
       </c>
       <c r="I88" s="19">
         <f ca="1"/>
-        <v>4.9283035687621969E-2</v>
+        <v>4.928305695371818E-2</v>
       </c>
     </row>
     <row r="89" spans="8:9" x14ac:dyDescent="0.3">
@@ -9835,7 +9853,7 @@
       </c>
       <c r="I89" s="19">
         <f ca="1"/>
-        <v>4.9283035687621969E-2</v>
+        <v>4.928305695371818E-2</v>
       </c>
     </row>
     <row r="90" spans="8:9" x14ac:dyDescent="0.3">
@@ -9844,7 +9862,7 @@
       </c>
       <c r="I90" s="19">
         <f ca="1"/>
-        <v>4.9283035687621969E-2</v>
+        <v>4.928305695371818E-2</v>
       </c>
     </row>
     <row r="91" spans="8:9" x14ac:dyDescent="0.3">
@@ -9853,7 +9871,7 @@
       </c>
       <c r="I91" s="19">
         <f ca="1"/>
-        <v>4.9283035687621969E-2</v>
+        <v>4.928305695371818E-2</v>
       </c>
     </row>
     <row r="92" spans="8:9" x14ac:dyDescent="0.3">
@@ -9862,7 +9880,7 @@
       </c>
       <c r="I92" s="19">
         <f ca="1"/>
-        <v>4.9283035687621969E-2</v>
+        <v>4.928305695371818E-2</v>
       </c>
     </row>
     <row r="93" spans="8:9" x14ac:dyDescent="0.3">
@@ -9871,7 +9889,7 @@
       </c>
       <c r="I93" s="19">
         <f ca="1"/>
-        <v>4.9283035687621969E-2</v>
+        <v>4.928305695371818E-2</v>
       </c>
     </row>
     <row r="94" spans="8:9" x14ac:dyDescent="0.3">
@@ -9880,7 +9898,7 @@
       </c>
       <c r="I94" s="19">
         <f ca="1"/>
-        <v>4.9283035687621969E-2</v>
+        <v>4.928305695371818E-2</v>
       </c>
     </row>
     <row r="95" spans="8:9" x14ac:dyDescent="0.3">
@@ -9889,7 +9907,7 @@
       </c>
       <c r="I95" s="19">
         <f ca="1"/>
-        <v>4.9283035687621969E-2</v>
+        <v>4.928305695371818E-2</v>
       </c>
     </row>
     <row r="96" spans="8:9" x14ac:dyDescent="0.3">
@@ -9898,7 +9916,7 @@
       </c>
       <c r="I96" s="19">
         <f ca="1"/>
-        <v>4.9416357721872958E-2</v>
+        <v>4.941630721492847E-2</v>
       </c>
     </row>
     <row r="97" spans="8:9" x14ac:dyDescent="0.3">
@@ -9907,7 +9925,7 @@
       </c>
       <c r="I97" s="19">
         <f ca="1"/>
-        <v>4.9416357721872958E-2</v>
+        <v>4.941630721492847E-2</v>
       </c>
     </row>
     <row r="98" spans="8:9" x14ac:dyDescent="0.3">
@@ -9916,7 +9934,7 @@
       </c>
       <c r="I98" s="19">
         <f ca="1"/>
-        <v>4.9416357721872958E-2</v>
+        <v>4.941630721492847E-2</v>
       </c>
     </row>
     <row r="99" spans="8:9" x14ac:dyDescent="0.3">
@@ -9925,7 +9943,7 @@
       </c>
       <c r="I99" s="19">
         <f ca="1"/>
-        <v>4.9416357721872958E-2</v>
+        <v>4.941630721492847E-2</v>
       </c>
     </row>
     <row r="100" spans="8:9" x14ac:dyDescent="0.3">
@@ -9934,7 +9952,7 @@
       </c>
       <c r="I100" s="19">
         <f ca="1"/>
-        <v>4.9416357721872958E-2</v>
+        <v>4.941630721492847E-2</v>
       </c>
     </row>
     <row r="101" spans="8:9" x14ac:dyDescent="0.3">
@@ -9943,7 +9961,7 @@
       </c>
       <c r="I101" s="19">
         <f ca="1"/>
-        <v>4.9416357721872958E-2</v>
+        <v>4.941630721492847E-2</v>
       </c>
     </row>
     <row r="102" spans="8:9" x14ac:dyDescent="0.3">
@@ -9952,7 +9970,7 @@
       </c>
       <c r="I102" s="19">
         <f ca="1"/>
-        <v>4.9416357721872958E-2</v>
+        <v>4.941630721492847E-2</v>
       </c>
     </row>
     <row r="103" spans="8:9" x14ac:dyDescent="0.3">
@@ -9961,7 +9979,7 @@
       </c>
       <c r="I103" s="19">
         <f ca="1"/>
-        <v>4.9416357721872958E-2</v>
+        <v>4.941630721492847E-2</v>
       </c>
     </row>
     <row r="104" spans="8:9" x14ac:dyDescent="0.3">
@@ -9970,7 +9988,7 @@
       </c>
       <c r="I104" s="19">
         <f ca="1"/>
-        <v>4.9416357721872958E-2</v>
+        <v>4.941630721492847E-2</v>
       </c>
     </row>
     <row r="105" spans="8:9" x14ac:dyDescent="0.3">
@@ -9979,7 +9997,7 @@
       </c>
       <c r="I105" s="19">
         <f ca="1"/>
-        <v>4.9416357721872958E-2</v>
+        <v>4.941630721492847E-2</v>
       </c>
     </row>
   </sheetData>
@@ -10040,7 +10058,7 @@
       </c>
       <c r="C6">
         <f ca="1">_xlfn.NORM.S.INV(RAND())</f>
-        <v>-0.81136812950484949</v>
+        <v>-1.9798174888206843</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.3">
@@ -10067,7 +10085,7 @@
       </c>
       <c r="C9">
         <f ca="1">EXP(-φ*t+Z*SQRT(t)*(σ^2)*(t^3)/6)</f>
-        <v>0.90361465124500207</v>
+        <v>0.90185665031261952</v>
       </c>
       <c r="D9" s="23" cm="1">
         <f t="array" aca="1" ref="D9" ca="1">_xll.MONTE.MEAN(C9)</f>
@@ -10084,7 +10102,7 @@
       </c>
       <c r="C10">
         <f ca="1">EXP(-φ*(u-t) + (σ^2)*((u-t)^3)/6 - σ*(u-t)*Z*SQRT(t))</f>
-        <v>0.98295049584499938</v>
+        <v>1.1047824254628449</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.3">
@@ -10093,7 +10111,7 @@
       </c>
       <c r="C11">
         <f ca="1">LN(C10)</f>
-        <v>-1.719652038284844E-2</v>
+        <v>9.964841554873502E-2</v>
       </c>
     </row>
     <row r="12" spans="2:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>